<commit_message>
Chỉnh sửa nội dung của AS0053_Cap nhat nhan vien.xlsx và WF0008 Danh muc phieu nhap xuat vcnb.xlsx
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/WF0008 Danh muc phieu nhap xuat vcnb.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/WF0008 Danh muc phieu nhap xuat vcnb.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DANGTHITIEUMAI\Products\ASOFT_ERP81\10_DOCUMENT\13_DETAIL_DESIGN\2.PROJECTS\2015\0.ERP PROJECTS\02.Quan ly mat hang theo quy cach\ASOFT-WM\2015-06-19 Phieu nhap kho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SOFT\201512\10_DOCUMENT\13_DETAIL_DESIGN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Update History" sheetId="1" r:id="rId1"/>
@@ -1928,7 +1928,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="258">
   <si>
     <t>Detail Design</t>
   </si>
@@ -2866,6 +2866,78 @@
   </si>
   <si>
     <t>- Sửa câu @SQL001 trong sheet Data Input</t>
+  </si>
+  <si>
+    <t>Thị Phượng</t>
+  </si>
+  <si>
+    <t>@SQL004</t>
+  </si>
+  <si>
+    <t>Kiểm tra điều kiện khi thực hiện Sửa phiếu cập nhật</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT TOP 1 1 FROM AT2006
+WHERE DivisionID = @DivisionID
+AND VoucherID = @VoucherID </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>AND IsWeb=1</t>
+    </r>
+  </si>
+  <si>
+    <t>@DivisionID @VoucherID
+@IsWeb</t>
+  </si>
+  <si>
+    <t>@@DivisionID
+@@VoucherID
+1</t>
+  </si>
+  <si>
+    <t>Thực hiện câu @SQL004 để kiểm tra điệu kiện để load màn hình Cập nhật khi thực hiện Click LinkEdit</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>LinkEdit</t>
+  </si>
+  <si>
+    <t>Sửa</t>
+  </si>
+  <si>
+    <t>Require</t>
+  </si>
+  <si>
+    <t>Click LinkEdit</t>
+  </si>
+  <si>
+    <t>Click</t>
+  </si>
+  <si>
+    <t>WFML000186</t>
+  </si>
+  <si>
+    <t>WFML000185</t>
+  </si>
+  <si>
+    <t>Click LickEdit Thực thi @SQL0004 để kiểm tra điều kiện IsWeb,
+- Nếu =1 cảnh báo message WFML000185 nếu là Phiếu VCNB, và WFML000186 nếu là Phiếu nhập or Phiếu xuất
+- Nếu =0 thực thi @SQL002 load form Detail</t>
+  </si>
+  <si>
+    <t>- Thêm câu @SQL004 trong sheet Data Input
+- Thêm WFML000185 và WFML000186 trong sheet Input Check
+- Thêm sự kiện Sửa trong sheet Form Func Spec</t>
   </si>
 </sst>
 </file>
@@ -3321,7 +3393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="268">
+  <cellXfs count="289">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3813,6 +3885,90 @@
     <xf numFmtId="0" fontId="7" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3843,68 +3999,38 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3924,30 +4050,6 @@
     <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3996,6 +4098,24 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4005,15 +4125,6 @@
     <xf numFmtId="0" fontId="7" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4029,44 +4140,68 @@
     <xf numFmtId="0" fontId="7" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4405,8 +4540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="C1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:J8"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4425,10 +4560,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="214" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="186"/>
+      <c r="B1" s="214"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -4450,11 +4585,13 @@
       <c r="I1" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="126"/>
+      <c r="J1" s="126" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="186"/>
-      <c r="B2" s="186"/>
+      <c r="A2" s="214"/>
+      <c r="B2" s="214"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -4476,7 +4613,9 @@
       <c r="I2" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="15"/>
+      <c r="J2" s="15">
+        <v>42381</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
@@ -4503,14 +4642,14 @@
       <c r="D4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="187" t="s">
+      <c r="E4" s="215" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="187"/>
-      <c r="G4" s="187"/>
-      <c r="H4" s="187"/>
-      <c r="I4" s="187"/>
-      <c r="J4" s="187"/>
+      <c r="F4" s="215"/>
+      <c r="G4" s="215"/>
+      <c r="H4" s="215"/>
+      <c r="I4" s="215"/>
+      <c r="J4" s="215"/>
     </row>
     <row r="5" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
@@ -4527,14 +4666,14 @@
         <f>H1</f>
         <v>Thanh Sơn</v>
       </c>
-      <c r="E5" s="188" t="s">
+      <c r="E5" s="216" t="s">
         <v>176</v>
       </c>
-      <c r="F5" s="189"/>
-      <c r="G5" s="189"/>
-      <c r="H5" s="189"/>
-      <c r="I5" s="189"/>
-      <c r="J5" s="189"/>
+      <c r="F5" s="217"/>
+      <c r="G5" s="217"/>
+      <c r="H5" s="217"/>
+      <c r="I5" s="217"/>
+      <c r="J5" s="217"/>
     </row>
     <row r="6" spans="1:10" s="111" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
@@ -4549,14 +4688,14 @@
       <c r="D6" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="190" t="s">
+      <c r="E6" s="218" t="s">
         <v>179</v>
       </c>
-      <c r="F6" s="191"/>
-      <c r="G6" s="191"/>
-      <c r="H6" s="191"/>
-      <c r="I6" s="191"/>
-      <c r="J6" s="192"/>
+      <c r="F6" s="219"/>
+      <c r="G6" s="219"/>
+      <c r="H6" s="219"/>
+      <c r="I6" s="219"/>
+      <c r="J6" s="220"/>
     </row>
     <row r="7" spans="1:10" s="111" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="112">
@@ -4571,30 +4710,36 @@
       <c r="D7" s="115" t="s">
         <v>239</v>
       </c>
-      <c r="E7" s="267" t="s">
+      <c r="E7" s="221" t="s">
         <v>240</v>
       </c>
-      <c r="F7" s="193"/>
-      <c r="G7" s="193"/>
-      <c r="H7" s="193"/>
-      <c r="I7" s="193"/>
-      <c r="J7" s="194"/>
-    </row>
-    <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="222"/>
+      <c r="G7" s="222"/>
+      <c r="H7" s="222"/>
+      <c r="I7" s="222"/>
+      <c r="J7" s="223"/>
+    </row>
+    <row r="8" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
       <c r="B8" s="21">
         <v>4</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="183"/>
-      <c r="F8" s="184"/>
-      <c r="G8" s="184"/>
-      <c r="H8" s="184"/>
-      <c r="I8" s="184"/>
-      <c r="J8" s="185"/>
+      <c r="C8" s="22">
+        <v>42381</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="E8" s="211" t="s">
+        <v>257</v>
+      </c>
+      <c r="F8" s="212"/>
+      <c r="G8" s="212"/>
+      <c r="H8" s="212"/>
+      <c r="I8" s="212"/>
+      <c r="J8" s="213"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -4605,12 +4750,12 @@
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="26"/>
-      <c r="E9" s="196"/>
-      <c r="F9" s="197"/>
-      <c r="G9" s="197"/>
-      <c r="H9" s="197"/>
-      <c r="I9" s="197"/>
-      <c r="J9" s="198"/>
+      <c r="E9" s="193"/>
+      <c r="F9" s="194"/>
+      <c r="G9" s="194"/>
+      <c r="H9" s="194"/>
+      <c r="I9" s="194"/>
+      <c r="J9" s="195"/>
     </row>
     <row r="10" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -4621,12 +4766,12 @@
       </c>
       <c r="C10" s="117"/>
       <c r="D10" s="118"/>
-      <c r="E10" s="199"/>
-      <c r="F10" s="200"/>
-      <c r="G10" s="200"/>
-      <c r="H10" s="200"/>
-      <c r="I10" s="200"/>
-      <c r="J10" s="201"/>
+      <c r="E10" s="196"/>
+      <c r="F10" s="197"/>
+      <c r="G10" s="197"/>
+      <c r="H10" s="197"/>
+      <c r="I10" s="197"/>
+      <c r="J10" s="198"/>
     </row>
     <row r="11" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -4637,12 +4782,12 @@
       </c>
       <c r="C11" s="120"/>
       <c r="D11" s="121"/>
-      <c r="E11" s="202"/>
-      <c r="F11" s="203"/>
-      <c r="G11" s="203"/>
-      <c r="H11" s="203"/>
-      <c r="I11" s="203"/>
-      <c r="J11" s="204"/>
+      <c r="E11" s="199"/>
+      <c r="F11" s="200"/>
+      <c r="G11" s="200"/>
+      <c r="H11" s="200"/>
+      <c r="I11" s="200"/>
+      <c r="J11" s="201"/>
     </row>
     <row r="12" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -4653,12 +4798,12 @@
       </c>
       <c r="C12" s="123"/>
       <c r="D12" s="124"/>
-      <c r="E12" s="205"/>
-      <c r="F12" s="206"/>
-      <c r="G12" s="206"/>
-      <c r="H12" s="206"/>
-      <c r="I12" s="206"/>
-      <c r="J12" s="207"/>
+      <c r="E12" s="202"/>
+      <c r="F12" s="203"/>
+      <c r="G12" s="203"/>
+      <c r="H12" s="203"/>
+      <c r="I12" s="203"/>
+      <c r="J12" s="204"/>
     </row>
     <row r="13" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -4669,12 +4814,12 @@
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="29"/>
-      <c r="E13" s="208"/>
-      <c r="F13" s="209"/>
-      <c r="G13" s="209"/>
-      <c r="H13" s="209"/>
-      <c r="I13" s="209"/>
-      <c r="J13" s="210"/>
+      <c r="E13" s="205"/>
+      <c r="F13" s="206"/>
+      <c r="G13" s="206"/>
+      <c r="H13" s="206"/>
+      <c r="I13" s="206"/>
+      <c r="J13" s="207"/>
     </row>
     <row r="14" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
@@ -4685,361 +4830,369 @@
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="33"/>
-      <c r="E14" s="211"/>
-      <c r="F14" s="212"/>
-      <c r="G14" s="212"/>
-      <c r="H14" s="212"/>
-      <c r="I14" s="212"/>
-      <c r="J14" s="213"/>
+      <c r="E14" s="208"/>
+      <c r="F14" s="209"/>
+      <c r="G14" s="209"/>
+      <c r="H14" s="209"/>
+      <c r="I14" s="209"/>
+      <c r="J14" s="210"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="195"/>
-      <c r="F15" s="195"/>
-      <c r="G15" s="195"/>
-      <c r="H15" s="195"/>
-      <c r="I15" s="195"/>
-      <c r="J15" s="195"/>
+      <c r="E15" s="192"/>
+      <c r="F15" s="192"/>
+      <c r="G15" s="192"/>
+      <c r="H15" s="192"/>
+      <c r="I15" s="192"/>
+      <c r="J15" s="192"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="195"/>
-      <c r="F16" s="195"/>
-      <c r="G16" s="195"/>
-      <c r="H16" s="195"/>
-      <c r="I16" s="195"/>
-      <c r="J16" s="195"/>
+      <c r="E16" s="192"/>
+      <c r="F16" s="192"/>
+      <c r="G16" s="192"/>
+      <c r="H16" s="192"/>
+      <c r="I16" s="192"/>
+      <c r="J16" s="192"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="195"/>
-      <c r="F17" s="195"/>
-      <c r="G17" s="195"/>
-      <c r="H17" s="195"/>
-      <c r="I17" s="195"/>
-      <c r="J17" s="195"/>
+      <c r="E17" s="192"/>
+      <c r="F17" s="192"/>
+      <c r="G17" s="192"/>
+      <c r="H17" s="192"/>
+      <c r="I17" s="192"/>
+      <c r="J17" s="192"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="195"/>
-      <c r="F18" s="195"/>
-      <c r="G18" s="195"/>
-      <c r="H18" s="195"/>
-      <c r="I18" s="195"/>
-      <c r="J18" s="195"/>
+      <c r="E18" s="192"/>
+      <c r="F18" s="192"/>
+      <c r="G18" s="192"/>
+      <c r="H18" s="192"/>
+      <c r="I18" s="192"/>
+      <c r="J18" s="192"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="195"/>
-      <c r="F19" s="195"/>
-      <c r="G19" s="195"/>
-      <c r="H19" s="195"/>
-      <c r="I19" s="195"/>
-      <c r="J19" s="195"/>
+      <c r="E19" s="192"/>
+      <c r="F19" s="192"/>
+      <c r="G19" s="192"/>
+      <c r="H19" s="192"/>
+      <c r="I19" s="192"/>
+      <c r="J19" s="192"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="195"/>
-      <c r="F20" s="195"/>
-      <c r="G20" s="195"/>
-      <c r="H20" s="195"/>
-      <c r="I20" s="195"/>
-      <c r="J20" s="195"/>
+      <c r="E20" s="192"/>
+      <c r="F20" s="192"/>
+      <c r="G20" s="192"/>
+      <c r="H20" s="192"/>
+      <c r="I20" s="192"/>
+      <c r="J20" s="192"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="195"/>
-      <c r="F21" s="195"/>
-      <c r="G21" s="195"/>
-      <c r="H21" s="195"/>
-      <c r="I21" s="195"/>
-      <c r="J21" s="195"/>
+      <c r="E21" s="192"/>
+      <c r="F21" s="192"/>
+      <c r="G21" s="192"/>
+      <c r="H21" s="192"/>
+      <c r="I21" s="192"/>
+      <c r="J21" s="192"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="195"/>
-      <c r="F22" s="195"/>
-      <c r="G22" s="195"/>
-      <c r="H22" s="195"/>
-      <c r="I22" s="195"/>
-      <c r="J22" s="195"/>
+      <c r="E22" s="192"/>
+      <c r="F22" s="192"/>
+      <c r="G22" s="192"/>
+      <c r="H22" s="192"/>
+      <c r="I22" s="192"/>
+      <c r="J22" s="192"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="195"/>
-      <c r="F23" s="195"/>
-      <c r="G23" s="195"/>
-      <c r="H23" s="195"/>
-      <c r="I23" s="195"/>
-      <c r="J23" s="195"/>
+      <c r="E23" s="192"/>
+      <c r="F23" s="192"/>
+      <c r="G23" s="192"/>
+      <c r="H23" s="192"/>
+      <c r="I23" s="192"/>
+      <c r="J23" s="192"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="195"/>
-      <c r="F24" s="195"/>
-      <c r="G24" s="195"/>
-      <c r="H24" s="195"/>
-      <c r="I24" s="195"/>
-      <c r="J24" s="195"/>
+      <c r="E24" s="192"/>
+      <c r="F24" s="192"/>
+      <c r="G24" s="192"/>
+      <c r="H24" s="192"/>
+      <c r="I24" s="192"/>
+      <c r="J24" s="192"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="195"/>
-      <c r="F25" s="195"/>
-      <c r="G25" s="195"/>
-      <c r="H25" s="195"/>
-      <c r="I25" s="195"/>
-      <c r="J25" s="195"/>
+      <c r="E25" s="192"/>
+      <c r="F25" s="192"/>
+      <c r="G25" s="192"/>
+      <c r="H25" s="192"/>
+      <c r="I25" s="192"/>
+      <c r="J25" s="192"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="195"/>
-      <c r="F26" s="195"/>
-      <c r="G26" s="195"/>
-      <c r="H26" s="195"/>
-      <c r="I26" s="195"/>
-      <c r="J26" s="195"/>
+      <c r="E26" s="192"/>
+      <c r="F26" s="192"/>
+      <c r="G26" s="192"/>
+      <c r="H26" s="192"/>
+      <c r="I26" s="192"/>
+      <c r="J26" s="192"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="195"/>
-      <c r="F27" s="195"/>
-      <c r="G27" s="195"/>
-      <c r="H27" s="195"/>
-      <c r="I27" s="195"/>
-      <c r="J27" s="195"/>
+      <c r="E27" s="192"/>
+      <c r="F27" s="192"/>
+      <c r="G27" s="192"/>
+      <c r="H27" s="192"/>
+      <c r="I27" s="192"/>
+      <c r="J27" s="192"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="195"/>
-      <c r="F28" s="195"/>
-      <c r="G28" s="195"/>
-      <c r="H28" s="195"/>
-      <c r="I28" s="195"/>
-      <c r="J28" s="195"/>
+      <c r="E28" s="192"/>
+      <c r="F28" s="192"/>
+      <c r="G28" s="192"/>
+      <c r="H28" s="192"/>
+      <c r="I28" s="192"/>
+      <c r="J28" s="192"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="195"/>
-      <c r="F29" s="195"/>
-      <c r="G29" s="195"/>
-      <c r="H29" s="195"/>
-      <c r="I29" s="195"/>
-      <c r="J29" s="195"/>
+      <c r="E29" s="192"/>
+      <c r="F29" s="192"/>
+      <c r="G29" s="192"/>
+      <c r="H29" s="192"/>
+      <c r="I29" s="192"/>
+      <c r="J29" s="192"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="195"/>
-      <c r="F30" s="195"/>
-      <c r="G30" s="195"/>
-      <c r="H30" s="195"/>
-      <c r="I30" s="195"/>
-      <c r="J30" s="195"/>
+      <c r="E30" s="192"/>
+      <c r="F30" s="192"/>
+      <c r="G30" s="192"/>
+      <c r="H30" s="192"/>
+      <c r="I30" s="192"/>
+      <c r="J30" s="192"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="195"/>
-      <c r="F31" s="195"/>
-      <c r="G31" s="195"/>
-      <c r="H31" s="195"/>
-      <c r="I31" s="195"/>
-      <c r="J31" s="195"/>
+      <c r="E31" s="192"/>
+      <c r="F31" s="192"/>
+      <c r="G31" s="192"/>
+      <c r="H31" s="192"/>
+      <c r="I31" s="192"/>
+      <c r="J31" s="192"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="195"/>
-      <c r="F32" s="195"/>
-      <c r="G32" s="195"/>
-      <c r="H32" s="195"/>
-      <c r="I32" s="195"/>
-      <c r="J32" s="195"/>
+      <c r="E32" s="192"/>
+      <c r="F32" s="192"/>
+      <c r="G32" s="192"/>
+      <c r="H32" s="192"/>
+      <c r="I32" s="192"/>
+      <c r="J32" s="192"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="195"/>
-      <c r="F33" s="195"/>
-      <c r="G33" s="195"/>
-      <c r="H33" s="195"/>
-      <c r="I33" s="195"/>
-      <c r="J33" s="195"/>
+      <c r="E33" s="192"/>
+      <c r="F33" s="192"/>
+      <c r="G33" s="192"/>
+      <c r="H33" s="192"/>
+      <c r="I33" s="192"/>
+      <c r="J33" s="192"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="195"/>
-      <c r="F34" s="195"/>
-      <c r="G34" s="195"/>
-      <c r="H34" s="195"/>
-      <c r="I34" s="195"/>
-      <c r="J34" s="195"/>
+      <c r="E34" s="192"/>
+      <c r="F34" s="192"/>
+      <c r="G34" s="192"/>
+      <c r="H34" s="192"/>
+      <c r="I34" s="192"/>
+      <c r="J34" s="192"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="195"/>
-      <c r="F35" s="195"/>
-      <c r="G35" s="195"/>
-      <c r="H35" s="195"/>
-      <c r="I35" s="195"/>
-      <c r="J35" s="195"/>
+      <c r="E35" s="192"/>
+      <c r="F35" s="192"/>
+      <c r="G35" s="192"/>
+      <c r="H35" s="192"/>
+      <c r="I35" s="192"/>
+      <c r="J35" s="192"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="195"/>
-      <c r="F36" s="195"/>
-      <c r="G36" s="195"/>
-      <c r="H36" s="195"/>
-      <c r="I36" s="195"/>
-      <c r="J36" s="195"/>
+      <c r="E36" s="192"/>
+      <c r="F36" s="192"/>
+      <c r="G36" s="192"/>
+      <c r="H36" s="192"/>
+      <c r="I36" s="192"/>
+      <c r="J36" s="192"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="195"/>
-      <c r="F37" s="195"/>
-      <c r="G37" s="195"/>
-      <c r="H37" s="195"/>
-      <c r="I37" s="195"/>
-      <c r="J37" s="195"/>
+      <c r="E37" s="192"/>
+      <c r="F37" s="192"/>
+      <c r="G37" s="192"/>
+      <c r="H37" s="192"/>
+      <c r="I37" s="192"/>
+      <c r="J37" s="192"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="195"/>
-      <c r="F38" s="195"/>
-      <c r="G38" s="195"/>
-      <c r="H38" s="195"/>
-      <c r="I38" s="195"/>
-      <c r="J38" s="195"/>
+      <c r="E38" s="192"/>
+      <c r="F38" s="192"/>
+      <c r="G38" s="192"/>
+      <c r="H38" s="192"/>
+      <c r="I38" s="192"/>
+      <c r="J38" s="192"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="195"/>
-      <c r="F39" s="195"/>
-      <c r="G39" s="195"/>
-      <c r="H39" s="195"/>
-      <c r="I39" s="195"/>
-      <c r="J39" s="195"/>
+      <c r="E39" s="192"/>
+      <c r="F39" s="192"/>
+      <c r="G39" s="192"/>
+      <c r="H39" s="192"/>
+      <c r="I39" s="192"/>
+      <c r="J39" s="192"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="195"/>
-      <c r="F40" s="195"/>
-      <c r="G40" s="195"/>
-      <c r="H40" s="195"/>
-      <c r="I40" s="195"/>
-      <c r="J40" s="195"/>
+      <c r="E40" s="192"/>
+      <c r="F40" s="192"/>
+      <c r="G40" s="192"/>
+      <c r="H40" s="192"/>
+      <c r="I40" s="192"/>
+      <c r="J40" s="192"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="195"/>
-      <c r="F41" s="195"/>
-      <c r="G41" s="195"/>
-      <c r="H41" s="195"/>
-      <c r="I41" s="195"/>
-      <c r="J41" s="195"/>
+      <c r="E41" s="192"/>
+      <c r="F41" s="192"/>
+      <c r="G41" s="192"/>
+      <c r="H41" s="192"/>
+      <c r="I41" s="192"/>
+      <c r="J41" s="192"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="195"/>
-      <c r="F42" s="195"/>
-      <c r="G42" s="195"/>
-      <c r="H42" s="195"/>
-      <c r="I42" s="195"/>
-      <c r="J42" s="195"/>
+      <c r="E42" s="192"/>
+      <c r="F42" s="192"/>
+      <c r="G42" s="192"/>
+      <c r="H42" s="192"/>
+      <c r="I42" s="192"/>
+      <c r="J42" s="192"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="E14:J14"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E19:J19"/>
     <mergeCell ref="E32:J32"/>
     <mergeCell ref="E21:J21"/>
     <mergeCell ref="E22:J22"/>
@@ -5052,24 +5205,16 @@
     <mergeCell ref="E29:J29"/>
     <mergeCell ref="E30:J30"/>
     <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E20:J20"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="E12:J12"/>
-    <mergeCell ref="E13:J13"/>
-    <mergeCell ref="E14:J14"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E38:J38"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
@@ -5259,7 +5404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="I6" sqref="I6:J6"/>
     </sheetView>
   </sheetViews>
@@ -5279,10 +5424,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="214" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="186"/>
+      <c r="B1" s="214"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -5307,14 +5452,14 @@
       <c r="I1" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="126">
+      <c r="J1" s="126" t="str">
         <f>'Update History'!J1</f>
-        <v>0</v>
+        <v>Thị Phượng</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="186"/>
-      <c r="B2" s="186"/>
+      <c r="A2" s="214"/>
+      <c r="B2" s="214"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -5341,7 +5486,7 @@
       </c>
       <c r="J2" s="15">
         <f>'Update History'!J2</f>
-        <v>0</v>
+        <v>42381</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -5357,76 +5502,76 @@
       <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="186" t="s">
+      <c r="A4" s="214" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="186"/>
-      <c r="C4" s="186"/>
-      <c r="D4" s="186"/>
-      <c r="E4" s="186"/>
-      <c r="F4" s="186"/>
-      <c r="G4" s="186"/>
-      <c r="H4" s="186"/>
-      <c r="I4" s="186" t="s">
+      <c r="B4" s="214"/>
+      <c r="C4" s="214"/>
+      <c r="D4" s="214"/>
+      <c r="E4" s="214"/>
+      <c r="F4" s="214"/>
+      <c r="G4" s="214"/>
+      <c r="H4" s="214"/>
+      <c r="I4" s="214" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="186"/>
+      <c r="J4" s="214"/>
     </row>
     <row r="5" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="222"/>
-      <c r="B5" s="223"/>
-      <c r="C5" s="223"/>
-      <c r="D5" s="223"/>
-      <c r="E5" s="223"/>
-      <c r="F5" s="223"/>
-      <c r="G5" s="223"/>
-      <c r="H5" s="224"/>
-      <c r="I5" s="214" t="s">
+      <c r="A5" s="226"/>
+      <c r="B5" s="227"/>
+      <c r="C5" s="227"/>
+      <c r="D5" s="227"/>
+      <c r="E5" s="227"/>
+      <c r="F5" s="227"/>
+      <c r="G5" s="227"/>
+      <c r="H5" s="228"/>
+      <c r="I5" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="215"/>
+      <c r="J5" s="233"/>
     </row>
     <row r="6" spans="1:10" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="225"/>
-      <c r="B6" s="226"/>
-      <c r="C6" s="226"/>
-      <c r="D6" s="226"/>
-      <c r="E6" s="226"/>
-      <c r="F6" s="226"/>
-      <c r="G6" s="226"/>
-      <c r="H6" s="227"/>
-      <c r="I6" s="216" t="s">
+      <c r="A6" s="229"/>
+      <c r="B6" s="230"/>
+      <c r="C6" s="230"/>
+      <c r="D6" s="230"/>
+      <c r="E6" s="230"/>
+      <c r="F6" s="230"/>
+      <c r="G6" s="230"/>
+      <c r="H6" s="231"/>
+      <c r="I6" s="234" t="s">
         <v>177</v>
       </c>
-      <c r="J6" s="217"/>
+      <c r="J6" s="235"/>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="225"/>
-      <c r="B7" s="226"/>
-      <c r="C7" s="226"/>
-      <c r="D7" s="226"/>
-      <c r="E7" s="226"/>
-      <c r="F7" s="226"/>
-      <c r="G7" s="226"/>
-      <c r="H7" s="227"/>
-      <c r="I7" s="218" t="s">
+      <c r="A7" s="229"/>
+      <c r="B7" s="230"/>
+      <c r="C7" s="230"/>
+      <c r="D7" s="230"/>
+      <c r="E7" s="230"/>
+      <c r="F7" s="230"/>
+      <c r="G7" s="230"/>
+      <c r="H7" s="231"/>
+      <c r="I7" s="236" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="219"/>
+      <c r="J7" s="237"/>
     </row>
     <row r="8" spans="1:10" ht="336" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="225"/>
-      <c r="B8" s="226"/>
-      <c r="C8" s="226"/>
-      <c r="D8" s="226"/>
-      <c r="E8" s="226"/>
-      <c r="F8" s="226"/>
-      <c r="G8" s="226"/>
-      <c r="H8" s="227"/>
-      <c r="I8" s="220" t="s">
+      <c r="A8" s="229"/>
+      <c r="B8" s="230"/>
+      <c r="C8" s="230"/>
+      <c r="D8" s="230"/>
+      <c r="E8" s="230"/>
+      <c r="F8" s="230"/>
+      <c r="G8" s="230"/>
+      <c r="H8" s="231"/>
+      <c r="I8" s="224" t="s">
         <v>171</v>
       </c>
-      <c r="J8" s="221"/>
+      <c r="J8" s="225"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
@@ -5505,359 +5650,339 @@
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="195"/>
-      <c r="F15" s="195"/>
-      <c r="G15" s="195"/>
-      <c r="H15" s="195"/>
-      <c r="I15" s="195"/>
-      <c r="J15" s="195"/>
+      <c r="E15" s="192"/>
+      <c r="F15" s="192"/>
+      <c r="G15" s="192"/>
+      <c r="H15" s="192"/>
+      <c r="I15" s="192"/>
+      <c r="J15" s="192"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="195"/>
-      <c r="F16" s="195"/>
-      <c r="G16" s="195"/>
-      <c r="H16" s="195"/>
-      <c r="I16" s="195"/>
-      <c r="J16" s="195"/>
+      <c r="E16" s="192"/>
+      <c r="F16" s="192"/>
+      <c r="G16" s="192"/>
+      <c r="H16" s="192"/>
+      <c r="I16" s="192"/>
+      <c r="J16" s="192"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="195"/>
-      <c r="F17" s="195"/>
-      <c r="G17" s="195"/>
-      <c r="H17" s="195"/>
-      <c r="I17" s="195"/>
-      <c r="J17" s="195"/>
+      <c r="E17" s="192"/>
+      <c r="F17" s="192"/>
+      <c r="G17" s="192"/>
+      <c r="H17" s="192"/>
+      <c r="I17" s="192"/>
+      <c r="J17" s="192"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="195"/>
-      <c r="F18" s="195"/>
-      <c r="G18" s="195"/>
-      <c r="H18" s="195"/>
-      <c r="I18" s="195"/>
-      <c r="J18" s="195"/>
+      <c r="E18" s="192"/>
+      <c r="F18" s="192"/>
+      <c r="G18" s="192"/>
+      <c r="H18" s="192"/>
+      <c r="I18" s="192"/>
+      <c r="J18" s="192"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="195"/>
-      <c r="F19" s="195"/>
-      <c r="G19" s="195"/>
-      <c r="H19" s="195"/>
-      <c r="I19" s="195"/>
-      <c r="J19" s="195"/>
+      <c r="E19" s="192"/>
+      <c r="F19" s="192"/>
+      <c r="G19" s="192"/>
+      <c r="H19" s="192"/>
+      <c r="I19" s="192"/>
+      <c r="J19" s="192"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="195"/>
-      <c r="F20" s="195"/>
-      <c r="G20" s="195"/>
-      <c r="H20" s="195"/>
-      <c r="I20" s="195"/>
-      <c r="J20" s="195"/>
+      <c r="E20" s="192"/>
+      <c r="F20" s="192"/>
+      <c r="G20" s="192"/>
+      <c r="H20" s="192"/>
+      <c r="I20" s="192"/>
+      <c r="J20" s="192"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="195"/>
-      <c r="F21" s="195"/>
-      <c r="G21" s="195"/>
-      <c r="H21" s="195"/>
-      <c r="I21" s="195"/>
-      <c r="J21" s="195"/>
+      <c r="E21" s="192"/>
+      <c r="F21" s="192"/>
+      <c r="G21" s="192"/>
+      <c r="H21" s="192"/>
+      <c r="I21" s="192"/>
+      <c r="J21" s="192"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="195"/>
-      <c r="F22" s="195"/>
-      <c r="G22" s="195"/>
-      <c r="H22" s="195"/>
-      <c r="I22" s="195"/>
-      <c r="J22" s="195"/>
+      <c r="E22" s="192"/>
+      <c r="F22" s="192"/>
+      <c r="G22" s="192"/>
+      <c r="H22" s="192"/>
+      <c r="I22" s="192"/>
+      <c r="J22" s="192"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="195"/>
-      <c r="F23" s="195"/>
-      <c r="G23" s="195"/>
-      <c r="H23" s="195"/>
-      <c r="I23" s="195"/>
-      <c r="J23" s="195"/>
+      <c r="E23" s="192"/>
+      <c r="F23" s="192"/>
+      <c r="G23" s="192"/>
+      <c r="H23" s="192"/>
+      <c r="I23" s="192"/>
+      <c r="J23" s="192"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="195"/>
-      <c r="F24" s="195"/>
-      <c r="G24" s="195"/>
-      <c r="H24" s="195"/>
-      <c r="I24" s="195"/>
-      <c r="J24" s="195"/>
+      <c r="E24" s="192"/>
+      <c r="F24" s="192"/>
+      <c r="G24" s="192"/>
+      <c r="H24" s="192"/>
+      <c r="I24" s="192"/>
+      <c r="J24" s="192"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="195"/>
-      <c r="F25" s="195"/>
-      <c r="G25" s="195"/>
-      <c r="H25" s="195"/>
-      <c r="I25" s="195"/>
-      <c r="J25" s="195"/>
+      <c r="E25" s="192"/>
+      <c r="F25" s="192"/>
+      <c r="G25" s="192"/>
+      <c r="H25" s="192"/>
+      <c r="I25" s="192"/>
+      <c r="J25" s="192"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="195"/>
-      <c r="F26" s="195"/>
-      <c r="G26" s="195"/>
-      <c r="H26" s="195"/>
-      <c r="I26" s="195"/>
-      <c r="J26" s="195"/>
+      <c r="E26" s="192"/>
+      <c r="F26" s="192"/>
+      <c r="G26" s="192"/>
+      <c r="H26" s="192"/>
+      <c r="I26" s="192"/>
+      <c r="J26" s="192"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="195"/>
-      <c r="F27" s="195"/>
-      <c r="G27" s="195"/>
-      <c r="H27" s="195"/>
-      <c r="I27" s="195"/>
-      <c r="J27" s="195"/>
+      <c r="E27" s="192"/>
+      <c r="F27" s="192"/>
+      <c r="G27" s="192"/>
+      <c r="H27" s="192"/>
+      <c r="I27" s="192"/>
+      <c r="J27" s="192"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="195"/>
-      <c r="F28" s="195"/>
-      <c r="G28" s="195"/>
-      <c r="H28" s="195"/>
-      <c r="I28" s="195"/>
-      <c r="J28" s="195"/>
+      <c r="E28" s="192"/>
+      <c r="F28" s="192"/>
+      <c r="G28" s="192"/>
+      <c r="H28" s="192"/>
+      <c r="I28" s="192"/>
+      <c r="J28" s="192"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="195"/>
-      <c r="F29" s="195"/>
-      <c r="G29" s="195"/>
-      <c r="H29" s="195"/>
-      <c r="I29" s="195"/>
-      <c r="J29" s="195"/>
+      <c r="E29" s="192"/>
+      <c r="F29" s="192"/>
+      <c r="G29" s="192"/>
+      <c r="H29" s="192"/>
+      <c r="I29" s="192"/>
+      <c r="J29" s="192"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="195"/>
-      <c r="F30" s="195"/>
-      <c r="G30" s="195"/>
-      <c r="H30" s="195"/>
-      <c r="I30" s="195"/>
-      <c r="J30" s="195"/>
+      <c r="E30" s="192"/>
+      <c r="F30" s="192"/>
+      <c r="G30" s="192"/>
+      <c r="H30" s="192"/>
+      <c r="I30" s="192"/>
+      <c r="J30" s="192"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="195"/>
-      <c r="F31" s="195"/>
-      <c r="G31" s="195"/>
-      <c r="H31" s="195"/>
-      <c r="I31" s="195"/>
-      <c r="J31" s="195"/>
+      <c r="E31" s="192"/>
+      <c r="F31" s="192"/>
+      <c r="G31" s="192"/>
+      <c r="H31" s="192"/>
+      <c r="I31" s="192"/>
+      <c r="J31" s="192"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="195"/>
-      <c r="F32" s="195"/>
-      <c r="G32" s="195"/>
-      <c r="H32" s="195"/>
-      <c r="I32" s="195"/>
-      <c r="J32" s="195"/>
+      <c r="E32" s="192"/>
+      <c r="F32" s="192"/>
+      <c r="G32" s="192"/>
+      <c r="H32" s="192"/>
+      <c r="I32" s="192"/>
+      <c r="J32" s="192"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="195"/>
-      <c r="F33" s="195"/>
-      <c r="G33" s="195"/>
-      <c r="H33" s="195"/>
-      <c r="I33" s="195"/>
-      <c r="J33" s="195"/>
+      <c r="E33" s="192"/>
+      <c r="F33" s="192"/>
+      <c r="G33" s="192"/>
+      <c r="H33" s="192"/>
+      <c r="I33" s="192"/>
+      <c r="J33" s="192"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="195"/>
-      <c r="F34" s="195"/>
-      <c r="G34" s="195"/>
-      <c r="H34" s="195"/>
-      <c r="I34" s="195"/>
-      <c r="J34" s="195"/>
+      <c r="E34" s="192"/>
+      <c r="F34" s="192"/>
+      <c r="G34" s="192"/>
+      <c r="H34" s="192"/>
+      <c r="I34" s="192"/>
+      <c r="J34" s="192"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="195"/>
-      <c r="F35" s="195"/>
-      <c r="G35" s="195"/>
-      <c r="H35" s="195"/>
-      <c r="I35" s="195"/>
-      <c r="J35" s="195"/>
+      <c r="E35" s="192"/>
+      <c r="F35" s="192"/>
+      <c r="G35" s="192"/>
+      <c r="H35" s="192"/>
+      <c r="I35" s="192"/>
+      <c r="J35" s="192"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="195"/>
-      <c r="F36" s="195"/>
-      <c r="G36" s="195"/>
-      <c r="H36" s="195"/>
-      <c r="I36" s="195"/>
-      <c r="J36" s="195"/>
+      <c r="E36" s="192"/>
+      <c r="F36" s="192"/>
+      <c r="G36" s="192"/>
+      <c r="H36" s="192"/>
+      <c r="I36" s="192"/>
+      <c r="J36" s="192"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="195"/>
-      <c r="F37" s="195"/>
-      <c r="G37" s="195"/>
-      <c r="H37" s="195"/>
-      <c r="I37" s="195"/>
-      <c r="J37" s="195"/>
+      <c r="E37" s="192"/>
+      <c r="F37" s="192"/>
+      <c r="G37" s="192"/>
+      <c r="H37" s="192"/>
+      <c r="I37" s="192"/>
+      <c r="J37" s="192"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="195"/>
-      <c r="F38" s="195"/>
-      <c r="G38" s="195"/>
-      <c r="H38" s="195"/>
-      <c r="I38" s="195"/>
-      <c r="J38" s="195"/>
+      <c r="E38" s="192"/>
+      <c r="F38" s="192"/>
+      <c r="G38" s="192"/>
+      <c r="H38" s="192"/>
+      <c r="I38" s="192"/>
+      <c r="J38" s="192"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="195"/>
-      <c r="F39" s="195"/>
-      <c r="G39" s="195"/>
-      <c r="H39" s="195"/>
-      <c r="I39" s="195"/>
-      <c r="J39" s="195"/>
+      <c r="E39" s="192"/>
+      <c r="F39" s="192"/>
+      <c r="G39" s="192"/>
+      <c r="H39" s="192"/>
+      <c r="I39" s="192"/>
+      <c r="J39" s="192"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="195"/>
-      <c r="F40" s="195"/>
-      <c r="G40" s="195"/>
-      <c r="H40" s="195"/>
-      <c r="I40" s="195"/>
-      <c r="J40" s="195"/>
+      <c r="E40" s="192"/>
+      <c r="F40" s="192"/>
+      <c r="G40" s="192"/>
+      <c r="H40" s="192"/>
+      <c r="I40" s="192"/>
+      <c r="J40" s="192"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="195"/>
-      <c r="F41" s="195"/>
-      <c r="G41" s="195"/>
-      <c r="H41" s="195"/>
-      <c r="I41" s="195"/>
-      <c r="J41" s="195"/>
+      <c r="E41" s="192"/>
+      <c r="F41" s="192"/>
+      <c r="G41" s="192"/>
+      <c r="H41" s="192"/>
+      <c r="I41" s="192"/>
+      <c r="J41" s="192"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="195"/>
-      <c r="F42" s="195"/>
-      <c r="G42" s="195"/>
-      <c r="H42" s="195"/>
-      <c r="I42" s="195"/>
-      <c r="J42" s="195"/>
+      <c r="E42" s="192"/>
+      <c r="F42" s="192"/>
+      <c r="G42" s="192"/>
+      <c r="H42" s="192"/>
+      <c r="I42" s="192"/>
+      <c r="J42" s="192"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="A5:H8"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E20:J20"/>
-    <mergeCell ref="E21:J21"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
     <mergeCell ref="E39:J39"/>
     <mergeCell ref="E40:J40"/>
     <mergeCell ref="E41:J41"/>
@@ -5874,6 +5999,26 @@
     <mergeCell ref="E37:J37"/>
     <mergeCell ref="E38:J38"/>
     <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="A5:H8"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E25:J25"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2">
@@ -5891,9 +6036,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N226"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F30" sqref="F30"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5915,10 +6060,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="214" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="228"/>
+      <c r="B1" s="238"/>
       <c r="C1" s="128" t="s">
         <v>1</v>
       </c>
@@ -5943,18 +6088,18 @@
       <c r="I1" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="229">
+      <c r="J1" s="239" t="str">
         <f>'Update History'!J1</f>
-        <v>0</v>
-      </c>
-      <c r="K1" s="230"/>
+        <v>Thị Phượng</v>
+      </c>
+      <c r="K1" s="240"/>
       <c r="L1" s="17"/>
       <c r="M1" s="17"/>
       <c r="N1" s="17"/>
     </row>
     <row r="2" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="186"/>
-      <c r="B2" s="228"/>
+      <c r="A2" s="214"/>
+      <c r="B2" s="238"/>
       <c r="C2" s="128" t="s">
         <v>7</v>
       </c>
@@ -5979,11 +6124,11 @@
       <c r="I2" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="231">
+      <c r="J2" s="241">
         <f>'Update History'!J2</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="232"/>
+        <v>42381</v>
+      </c>
+      <c r="K2" s="242"/>
       <c r="L2" s="17"/>
       <c r="M2" s="17"/>
       <c r="N2" s="17"/>
@@ -7683,8 +7828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:J19"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7702,10 +7847,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="214" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="186"/>
+      <c r="B1" s="214"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -7730,14 +7875,14 @@
       <c r="I1" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="126">
+      <c r="J1" s="126" t="str">
         <f>'Update History'!J1</f>
-        <v>0</v>
+        <v>Thị Phượng</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="186"/>
-      <c r="B2" s="186"/>
+      <c r="A2" s="214"/>
+      <c r="B2" s="214"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -7764,7 +7909,7 @@
       </c>
       <c r="J2" s="15">
         <f>'Update History'!J2</f>
-        <v>0</v>
+        <v>42381</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -7801,35 +7946,55 @@
       <c r="G4" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="236" t="s">
+      <c r="H4" s="246" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="236"/>
-      <c r="J4" s="236"/>
-    </row>
-    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="233"/>
-      <c r="I5" s="234"/>
-      <c r="J5" s="235"/>
-    </row>
-    <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="233"/>
-      <c r="I6" s="234"/>
-      <c r="J6" s="235"/>
+      <c r="I4" s="246"/>
+      <c r="J4" s="246"/>
+    </row>
+    <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="C5" s="277" t="s">
+        <v>251</v>
+      </c>
+      <c r="D5" s="278"/>
+      <c r="E5" s="271"/>
+      <c r="F5" s="270" t="s">
+        <v>252</v>
+      </c>
+      <c r="G5" s="270" t="s">
+        <v>253</v>
+      </c>
+      <c r="H5" s="272" t="s">
+        <v>255</v>
+      </c>
+      <c r="I5" s="273"/>
+      <c r="J5" s="274"/>
+    </row>
+    <row r="6" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="279"/>
+      <c r="B6" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="C6" s="280" t="s">
+        <v>251</v>
+      </c>
+      <c r="D6" s="281"/>
+      <c r="E6" s="282"/>
+      <c r="F6" s="283" t="s">
+        <v>252</v>
+      </c>
+      <c r="G6" s="283" t="s">
+        <v>253</v>
+      </c>
+      <c r="H6" s="272" t="s">
+        <v>254</v>
+      </c>
+      <c r="I6" s="273"/>
+      <c r="J6" s="274"/>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="56"/>
@@ -7839,9 +8004,9 @@
       <c r="E7" s="51"/>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
-      <c r="H7" s="233"/>
-      <c r="I7" s="234"/>
-      <c r="J7" s="235"/>
+      <c r="H7" s="243"/>
+      <c r="I7" s="244"/>
+      <c r="J7" s="245"/>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
@@ -7851,9 +8016,9 @@
       <c r="E8" s="50"/>
       <c r="F8" s="50"/>
       <c r="G8" s="50"/>
-      <c r="H8" s="233"/>
-      <c r="I8" s="234"/>
-      <c r="J8" s="235"/>
+      <c r="H8" s="243"/>
+      <c r="I8" s="244"/>
+      <c r="J8" s="245"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
@@ -7863,9 +8028,9 @@
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
-      <c r="H9" s="233"/>
-      <c r="I9" s="234"/>
-      <c r="J9" s="235"/>
+      <c r="H9" s="243"/>
+      <c r="I9" s="244"/>
+      <c r="J9" s="245"/>
     </row>
     <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="56"/>
@@ -7875,9 +8040,9 @@
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
-      <c r="H10" s="233"/>
-      <c r="I10" s="234"/>
-      <c r="J10" s="235"/>
+      <c r="H10" s="243"/>
+      <c r="I10" s="244"/>
+      <c r="J10" s="245"/>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="56"/>
@@ -7887,9 +8052,9 @@
       <c r="E11" s="51"/>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
-      <c r="H11" s="233"/>
-      <c r="I11" s="234"/>
-      <c r="J11" s="235"/>
+      <c r="H11" s="243"/>
+      <c r="I11" s="244"/>
+      <c r="J11" s="245"/>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="56"/>
@@ -7899,9 +8064,9 @@
       <c r="E12" s="51"/>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
-      <c r="H12" s="233"/>
-      <c r="I12" s="234"/>
-      <c r="J12" s="235"/>
+      <c r="H12" s="243"/>
+      <c r="I12" s="244"/>
+      <c r="J12" s="245"/>
     </row>
     <row r="13" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="56"/>
@@ -7911,9 +8076,9 @@
       <c r="E13" s="55"/>
       <c r="F13" s="55"/>
       <c r="G13" s="55"/>
-      <c r="H13" s="233"/>
-      <c r="I13" s="234"/>
-      <c r="J13" s="235"/>
+      <c r="H13" s="243"/>
+      <c r="I13" s="244"/>
+      <c r="J13" s="245"/>
     </row>
     <row r="14" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="56"/>
@@ -7923,372 +8088,348 @@
       <c r="E14" s="55"/>
       <c r="F14" s="55"/>
       <c r="G14" s="55"/>
-      <c r="H14" s="233"/>
-      <c r="I14" s="234"/>
-      <c r="J14" s="235"/>
+      <c r="H14" s="243"/>
+      <c r="I14" s="244"/>
+      <c r="J14" s="245"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="195"/>
-      <c r="F15" s="195"/>
-      <c r="G15" s="195"/>
-      <c r="H15" s="195"/>
-      <c r="I15" s="195"/>
-      <c r="J15" s="195"/>
+      <c r="E15" s="192"/>
+      <c r="F15" s="192"/>
+      <c r="G15" s="192"/>
+      <c r="H15" s="192"/>
+      <c r="I15" s="192"/>
+      <c r="J15" s="192"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="195"/>
-      <c r="F16" s="195"/>
-      <c r="G16" s="195"/>
-      <c r="H16" s="195"/>
-      <c r="I16" s="195"/>
-      <c r="J16" s="195"/>
+      <c r="E16" s="192"/>
+      <c r="F16" s="192"/>
+      <c r="G16" s="192"/>
+      <c r="H16" s="192"/>
+      <c r="I16" s="192"/>
+      <c r="J16" s="192"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="195"/>
-      <c r="F17" s="195"/>
-      <c r="G17" s="195"/>
-      <c r="H17" s="195"/>
-      <c r="I17" s="195"/>
-      <c r="J17" s="195"/>
+      <c r="E17" s="192"/>
+      <c r="F17" s="192"/>
+      <c r="G17" s="192"/>
+      <c r="H17" s="192"/>
+      <c r="I17" s="192"/>
+      <c r="J17" s="192"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="195"/>
-      <c r="F18" s="195"/>
-      <c r="G18" s="195"/>
-      <c r="H18" s="195"/>
-      <c r="I18" s="195"/>
-      <c r="J18" s="195"/>
+      <c r="E18" s="192"/>
+      <c r="F18" s="192"/>
+      <c r="G18" s="192"/>
+      <c r="H18" s="192"/>
+      <c r="I18" s="192"/>
+      <c r="J18" s="192"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="195"/>
-      <c r="F19" s="195"/>
-      <c r="G19" s="195"/>
-      <c r="H19" s="195"/>
-      <c r="I19" s="195"/>
-      <c r="J19" s="195"/>
+      <c r="E19" s="192"/>
+      <c r="F19" s="192"/>
+      <c r="G19" s="192"/>
+      <c r="H19" s="192"/>
+      <c r="I19" s="192"/>
+      <c r="J19" s="192"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="195"/>
-      <c r="F20" s="195"/>
-      <c r="G20" s="195"/>
-      <c r="H20" s="195"/>
-      <c r="I20" s="195"/>
-      <c r="J20" s="195"/>
+      <c r="E20" s="192"/>
+      <c r="F20" s="192"/>
+      <c r="G20" s="192"/>
+      <c r="H20" s="192"/>
+      <c r="I20" s="192"/>
+      <c r="J20" s="192"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="195"/>
-      <c r="F21" s="195"/>
-      <c r="G21" s="195"/>
-      <c r="H21" s="195"/>
-      <c r="I21" s="195"/>
-      <c r="J21" s="195"/>
+      <c r="E21" s="192"/>
+      <c r="F21" s="192"/>
+      <c r="G21" s="192"/>
+      <c r="H21" s="192"/>
+      <c r="I21" s="192"/>
+      <c r="J21" s="192"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="195"/>
-      <c r="F22" s="195"/>
-      <c r="G22" s="195"/>
-      <c r="H22" s="195"/>
-      <c r="I22" s="195"/>
-      <c r="J22" s="195"/>
+      <c r="E22" s="192"/>
+      <c r="F22" s="192"/>
+      <c r="G22" s="192"/>
+      <c r="H22" s="192"/>
+      <c r="I22" s="192"/>
+      <c r="J22" s="192"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="195"/>
-      <c r="F23" s="195"/>
-      <c r="G23" s="195"/>
-      <c r="H23" s="195"/>
-      <c r="I23" s="195"/>
-      <c r="J23" s="195"/>
+      <c r="E23" s="192"/>
+      <c r="F23" s="192"/>
+      <c r="G23" s="192"/>
+      <c r="H23" s="192"/>
+      <c r="I23" s="192"/>
+      <c r="J23" s="192"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="195"/>
-      <c r="F24" s="195"/>
-      <c r="G24" s="195"/>
-      <c r="H24" s="195"/>
-      <c r="I24" s="195"/>
-      <c r="J24" s="195"/>
+      <c r="E24" s="192"/>
+      <c r="F24" s="192"/>
+      <c r="G24" s="192"/>
+      <c r="H24" s="192"/>
+      <c r="I24" s="192"/>
+      <c r="J24" s="192"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="195"/>
-      <c r="F25" s="195"/>
-      <c r="G25" s="195"/>
-      <c r="H25" s="195"/>
-      <c r="I25" s="195"/>
-      <c r="J25" s="195"/>
+      <c r="E25" s="192"/>
+      <c r="F25" s="192"/>
+      <c r="G25" s="192"/>
+      <c r="H25" s="192"/>
+      <c r="I25" s="192"/>
+      <c r="J25" s="192"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="195"/>
-      <c r="F26" s="195"/>
-      <c r="G26" s="195"/>
-      <c r="H26" s="195"/>
-      <c r="I26" s="195"/>
-      <c r="J26" s="195"/>
+      <c r="E26" s="192"/>
+      <c r="F26" s="192"/>
+      <c r="G26" s="192"/>
+      <c r="H26" s="192"/>
+      <c r="I26" s="192"/>
+      <c r="J26" s="192"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="195"/>
-      <c r="F27" s="195"/>
-      <c r="G27" s="195"/>
-      <c r="H27" s="195"/>
-      <c r="I27" s="195"/>
-      <c r="J27" s="195"/>
+      <c r="E27" s="192"/>
+      <c r="F27" s="192"/>
+      <c r="G27" s="192"/>
+      <c r="H27" s="192"/>
+      <c r="I27" s="192"/>
+      <c r="J27" s="192"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="195"/>
-      <c r="F28" s="195"/>
-      <c r="G28" s="195"/>
-      <c r="H28" s="195"/>
-      <c r="I28" s="195"/>
-      <c r="J28" s="195"/>
+      <c r="E28" s="192"/>
+      <c r="F28" s="192"/>
+      <c r="G28" s="192"/>
+      <c r="H28" s="192"/>
+      <c r="I28" s="192"/>
+      <c r="J28" s="192"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="195"/>
-      <c r="F29" s="195"/>
-      <c r="G29" s="195"/>
-      <c r="H29" s="195"/>
-      <c r="I29" s="195"/>
-      <c r="J29" s="195"/>
+      <c r="E29" s="192"/>
+      <c r="F29" s="192"/>
+      <c r="G29" s="192"/>
+      <c r="H29" s="192"/>
+      <c r="I29" s="192"/>
+      <c r="J29" s="192"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="195"/>
-      <c r="F30" s="195"/>
-      <c r="G30" s="195"/>
-      <c r="H30" s="195"/>
-      <c r="I30" s="195"/>
-      <c r="J30" s="195"/>
+      <c r="E30" s="192"/>
+      <c r="F30" s="192"/>
+      <c r="G30" s="192"/>
+      <c r="H30" s="192"/>
+      <c r="I30" s="192"/>
+      <c r="J30" s="192"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="195"/>
-      <c r="F31" s="195"/>
-      <c r="G31" s="195"/>
-      <c r="H31" s="195"/>
-      <c r="I31" s="195"/>
-      <c r="J31" s="195"/>
+      <c r="E31" s="192"/>
+      <c r="F31" s="192"/>
+      <c r="G31" s="192"/>
+      <c r="H31" s="192"/>
+      <c r="I31" s="192"/>
+      <c r="J31" s="192"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="195"/>
-      <c r="F32" s="195"/>
-      <c r="G32" s="195"/>
-      <c r="H32" s="195"/>
-      <c r="I32" s="195"/>
-      <c r="J32" s="195"/>
+      <c r="E32" s="192"/>
+      <c r="F32" s="192"/>
+      <c r="G32" s="192"/>
+      <c r="H32" s="192"/>
+      <c r="I32" s="192"/>
+      <c r="J32" s="192"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="195"/>
-      <c r="F33" s="195"/>
-      <c r="G33" s="195"/>
-      <c r="H33" s="195"/>
-      <c r="I33" s="195"/>
-      <c r="J33" s="195"/>
+      <c r="E33" s="192"/>
+      <c r="F33" s="192"/>
+      <c r="G33" s="192"/>
+      <c r="H33" s="192"/>
+      <c r="I33" s="192"/>
+      <c r="J33" s="192"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="195"/>
-      <c r="F34" s="195"/>
-      <c r="G34" s="195"/>
-      <c r="H34" s="195"/>
-      <c r="I34" s="195"/>
-      <c r="J34" s="195"/>
+      <c r="E34" s="192"/>
+      <c r="F34" s="192"/>
+      <c r="G34" s="192"/>
+      <c r="H34" s="192"/>
+      <c r="I34" s="192"/>
+      <c r="J34" s="192"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="195"/>
-      <c r="F35" s="195"/>
-      <c r="G35" s="195"/>
-      <c r="H35" s="195"/>
-      <c r="I35" s="195"/>
-      <c r="J35" s="195"/>
+      <c r="E35" s="192"/>
+      <c r="F35" s="192"/>
+      <c r="G35" s="192"/>
+      <c r="H35" s="192"/>
+      <c r="I35" s="192"/>
+      <c r="J35" s="192"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="195"/>
-      <c r="F36" s="195"/>
-      <c r="G36" s="195"/>
-      <c r="H36" s="195"/>
-      <c r="I36" s="195"/>
-      <c r="J36" s="195"/>
+      <c r="E36" s="192"/>
+      <c r="F36" s="192"/>
+      <c r="G36" s="192"/>
+      <c r="H36" s="192"/>
+      <c r="I36" s="192"/>
+      <c r="J36" s="192"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="195"/>
-      <c r="F37" s="195"/>
-      <c r="G37" s="195"/>
-      <c r="H37" s="195"/>
-      <c r="I37" s="195"/>
-      <c r="J37" s="195"/>
+      <c r="E37" s="192"/>
+      <c r="F37" s="192"/>
+      <c r="G37" s="192"/>
+      <c r="H37" s="192"/>
+      <c r="I37" s="192"/>
+      <c r="J37" s="192"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="195"/>
-      <c r="F38" s="195"/>
-      <c r="G38" s="195"/>
-      <c r="H38" s="195"/>
-      <c r="I38" s="195"/>
-      <c r="J38" s="195"/>
+      <c r="E38" s="192"/>
+      <c r="F38" s="192"/>
+      <c r="G38" s="192"/>
+      <c r="H38" s="192"/>
+      <c r="I38" s="192"/>
+      <c r="J38" s="192"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="195"/>
-      <c r="F39" s="195"/>
-      <c r="G39" s="195"/>
-      <c r="H39" s="195"/>
-      <c r="I39" s="195"/>
-      <c r="J39" s="195"/>
+      <c r="E39" s="192"/>
+      <c r="F39" s="192"/>
+      <c r="G39" s="192"/>
+      <c r="H39" s="192"/>
+      <c r="I39" s="192"/>
+      <c r="J39" s="192"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="195"/>
-      <c r="F40" s="195"/>
-      <c r="G40" s="195"/>
-      <c r="H40" s="195"/>
-      <c r="I40" s="195"/>
-      <c r="J40" s="195"/>
+      <c r="E40" s="192"/>
+      <c r="F40" s="192"/>
+      <c r="G40" s="192"/>
+      <c r="H40" s="192"/>
+      <c r="I40" s="192"/>
+      <c r="J40" s="192"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="195"/>
-      <c r="F41" s="195"/>
-      <c r="G41" s="195"/>
-      <c r="H41" s="195"/>
-      <c r="I41" s="195"/>
-      <c r="J41" s="195"/>
+      <c r="E41" s="192"/>
+      <c r="F41" s="192"/>
+      <c r="G41" s="192"/>
+      <c r="H41" s="192"/>
+      <c r="I41" s="192"/>
+      <c r="J41" s="192"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="195"/>
-      <c r="F42" s="195"/>
-      <c r="G42" s="195"/>
-      <c r="H42" s="195"/>
-      <c r="I42" s="195"/>
-      <c r="J42" s="195"/>
+      <c r="E42" s="192"/>
+      <c r="F42" s="192"/>
+      <c r="G42" s="192"/>
+      <c r="H42" s="192"/>
+      <c r="I42" s="192"/>
+      <c r="J42" s="192"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="E39:J39"/>
     <mergeCell ref="E40:J40"/>
@@ -8305,6 +8446,30 @@
     <mergeCell ref="E20:J20"/>
     <mergeCell ref="E21:J21"/>
     <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H8:J8"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2">
@@ -8322,7 +8487,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:J2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8340,10 +8505,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="214" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="186"/>
+      <c r="B1" s="214"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -8368,14 +8533,14 @@
       <c r="I1" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="126">
+      <c r="J1" s="126" t="str">
         <f>'Update History'!J1</f>
-        <v>0</v>
+        <v>Thị Phượng</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="186"/>
-      <c r="B2" s="186"/>
+      <c r="A2" s="214"/>
+      <c r="B2" s="214"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -8402,20 +8567,20 @@
       </c>
       <c r="J2" s="15">
         <f>'Update History'!J2</f>
-        <v>0</v>
+        <v>42381</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="241"/>
-      <c r="B3" s="242"/>
-      <c r="C3" s="242"/>
-      <c r="D3" s="242"/>
-      <c r="E3" s="242"/>
-      <c r="F3" s="242"/>
-      <c r="G3" s="242"/>
-      <c r="H3" s="242"/>
-      <c r="I3" s="242"/>
-      <c r="J3" s="243"/>
+      <c r="A3" s="251"/>
+      <c r="B3" s="252"/>
+      <c r="C3" s="252"/>
+      <c r="D3" s="252"/>
+      <c r="E3" s="252"/>
+      <c r="F3" s="252"/>
+      <c r="G3" s="252"/>
+      <c r="H3" s="252"/>
+      <c r="I3" s="252"/>
+      <c r="J3" s="253"/>
     </row>
     <row r="4" spans="1:10" s="45" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="66" t="s">
@@ -8430,16 +8595,16 @@
       <c r="D4" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="237" t="s">
+      <c r="E4" s="247" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="237"/>
-      <c r="G4" s="238" t="s">
+      <c r="F4" s="247"/>
+      <c r="G4" s="248" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="239"/>
-      <c r="I4" s="239"/>
-      <c r="J4" s="240"/>
+      <c r="H4" s="249"/>
+      <c r="I4" s="249"/>
+      <c r="J4" s="250"/>
     </row>
     <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
@@ -8566,347 +8731,351 @@
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="195"/>
-      <c r="F15" s="195"/>
-      <c r="G15" s="195"/>
-      <c r="H15" s="195"/>
-      <c r="I15" s="195"/>
-      <c r="J15" s="195"/>
+      <c r="E15" s="192"/>
+      <c r="F15" s="192"/>
+      <c r="G15" s="192"/>
+      <c r="H15" s="192"/>
+      <c r="I15" s="192"/>
+      <c r="J15" s="192"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="195"/>
-      <c r="F16" s="195"/>
-      <c r="G16" s="195"/>
-      <c r="H16" s="195"/>
-      <c r="I16" s="195"/>
-      <c r="J16" s="195"/>
+      <c r="E16" s="192"/>
+      <c r="F16" s="192"/>
+      <c r="G16" s="192"/>
+      <c r="H16" s="192"/>
+      <c r="I16" s="192"/>
+      <c r="J16" s="192"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="195"/>
-      <c r="F17" s="195"/>
-      <c r="G17" s="195"/>
-      <c r="H17" s="195"/>
-      <c r="I17" s="195"/>
-      <c r="J17" s="195"/>
+      <c r="E17" s="192"/>
+      <c r="F17" s="192"/>
+      <c r="G17" s="192"/>
+      <c r="H17" s="192"/>
+      <c r="I17" s="192"/>
+      <c r="J17" s="192"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="195"/>
-      <c r="F18" s="195"/>
-      <c r="G18" s="195"/>
-      <c r="H18" s="195"/>
-      <c r="I18" s="195"/>
-      <c r="J18" s="195"/>
+      <c r="E18" s="192"/>
+      <c r="F18" s="192"/>
+      <c r="G18" s="192"/>
+      <c r="H18" s="192"/>
+      <c r="I18" s="192"/>
+      <c r="J18" s="192"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="195"/>
-      <c r="F19" s="195"/>
-      <c r="G19" s="195"/>
-      <c r="H19" s="195"/>
-      <c r="I19" s="195"/>
-      <c r="J19" s="195"/>
+      <c r="E19" s="192"/>
+      <c r="F19" s="192"/>
+      <c r="G19" s="192"/>
+      <c r="H19" s="192"/>
+      <c r="I19" s="192"/>
+      <c r="J19" s="192"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="195"/>
-      <c r="F20" s="195"/>
-      <c r="G20" s="195"/>
-      <c r="H20" s="195"/>
-      <c r="I20" s="195"/>
-      <c r="J20" s="195"/>
+      <c r="E20" s="192"/>
+      <c r="F20" s="192"/>
+      <c r="G20" s="192"/>
+      <c r="H20" s="192"/>
+      <c r="I20" s="192"/>
+      <c r="J20" s="192"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="195"/>
-      <c r="F21" s="195"/>
-      <c r="G21" s="195"/>
-      <c r="H21" s="195"/>
-      <c r="I21" s="195"/>
-      <c r="J21" s="195"/>
+      <c r="E21" s="192"/>
+      <c r="F21" s="192"/>
+      <c r="G21" s="192"/>
+      <c r="H21" s="192"/>
+      <c r="I21" s="192"/>
+      <c r="J21" s="192"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="195"/>
-      <c r="F22" s="195"/>
-      <c r="G22" s="195"/>
-      <c r="H22" s="195"/>
-      <c r="I22" s="195"/>
-      <c r="J22" s="195"/>
+      <c r="E22" s="192"/>
+      <c r="F22" s="192"/>
+      <c r="G22" s="192"/>
+      <c r="H22" s="192"/>
+      <c r="I22" s="192"/>
+      <c r="J22" s="192"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="195"/>
-      <c r="F23" s="195"/>
-      <c r="G23" s="195"/>
-      <c r="H23" s="195"/>
-      <c r="I23" s="195"/>
-      <c r="J23" s="195"/>
+      <c r="E23" s="192"/>
+      <c r="F23" s="192"/>
+      <c r="G23" s="192"/>
+      <c r="H23" s="192"/>
+      <c r="I23" s="192"/>
+      <c r="J23" s="192"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="195"/>
-      <c r="F24" s="195"/>
-      <c r="G24" s="195"/>
-      <c r="H24" s="195"/>
-      <c r="I24" s="195"/>
-      <c r="J24" s="195"/>
+      <c r="E24" s="192"/>
+      <c r="F24" s="192"/>
+      <c r="G24" s="192"/>
+      <c r="H24" s="192"/>
+      <c r="I24" s="192"/>
+      <c r="J24" s="192"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="195"/>
-      <c r="F25" s="195"/>
-      <c r="G25" s="195"/>
-      <c r="H25" s="195"/>
-      <c r="I25" s="195"/>
-      <c r="J25" s="195"/>
+      <c r="E25" s="192"/>
+      <c r="F25" s="192"/>
+      <c r="G25" s="192"/>
+      <c r="H25" s="192"/>
+      <c r="I25" s="192"/>
+      <c r="J25" s="192"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="195"/>
-      <c r="F26" s="195"/>
-      <c r="G26" s="195"/>
-      <c r="H26" s="195"/>
-      <c r="I26" s="195"/>
-      <c r="J26" s="195"/>
+      <c r="E26" s="192"/>
+      <c r="F26" s="192"/>
+      <c r="G26" s="192"/>
+      <c r="H26" s="192"/>
+      <c r="I26" s="192"/>
+      <c r="J26" s="192"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="195"/>
-      <c r="F27" s="195"/>
-      <c r="G27" s="195"/>
-      <c r="H27" s="195"/>
-      <c r="I27" s="195"/>
-      <c r="J27" s="195"/>
+      <c r="E27" s="192"/>
+      <c r="F27" s="192"/>
+      <c r="G27" s="192"/>
+      <c r="H27" s="192"/>
+      <c r="I27" s="192"/>
+      <c r="J27" s="192"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="195"/>
-      <c r="F28" s="195"/>
-      <c r="G28" s="195"/>
-      <c r="H28" s="195"/>
-      <c r="I28" s="195"/>
-      <c r="J28" s="195"/>
+      <c r="E28" s="192"/>
+      <c r="F28" s="192"/>
+      <c r="G28" s="192"/>
+      <c r="H28" s="192"/>
+      <c r="I28" s="192"/>
+      <c r="J28" s="192"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="195"/>
-      <c r="F29" s="195"/>
-      <c r="G29" s="195"/>
-      <c r="H29" s="195"/>
-      <c r="I29" s="195"/>
-      <c r="J29" s="195"/>
+      <c r="E29" s="192"/>
+      <c r="F29" s="192"/>
+      <c r="G29" s="192"/>
+      <c r="H29" s="192"/>
+      <c r="I29" s="192"/>
+      <c r="J29" s="192"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="195"/>
-      <c r="F30" s="195"/>
-      <c r="G30" s="195"/>
-      <c r="H30" s="195"/>
-      <c r="I30" s="195"/>
-      <c r="J30" s="195"/>
+      <c r="E30" s="192"/>
+      <c r="F30" s="192"/>
+      <c r="G30" s="192"/>
+      <c r="H30" s="192"/>
+      <c r="I30" s="192"/>
+      <c r="J30" s="192"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="195"/>
-      <c r="F31" s="195"/>
-      <c r="G31" s="195"/>
-      <c r="H31" s="195"/>
-      <c r="I31" s="195"/>
-      <c r="J31" s="195"/>
+      <c r="E31" s="192"/>
+      <c r="F31" s="192"/>
+      <c r="G31" s="192"/>
+      <c r="H31" s="192"/>
+      <c r="I31" s="192"/>
+      <c r="J31" s="192"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="195"/>
-      <c r="F32" s="195"/>
-      <c r="G32" s="195"/>
-      <c r="H32" s="195"/>
-      <c r="I32" s="195"/>
-      <c r="J32" s="195"/>
+      <c r="E32" s="192"/>
+      <c r="F32" s="192"/>
+      <c r="G32" s="192"/>
+      <c r="H32" s="192"/>
+      <c r="I32" s="192"/>
+      <c r="J32" s="192"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="195"/>
-      <c r="F33" s="195"/>
-      <c r="G33" s="195"/>
-      <c r="H33" s="195"/>
-      <c r="I33" s="195"/>
-      <c r="J33" s="195"/>
+      <c r="E33" s="192"/>
+      <c r="F33" s="192"/>
+      <c r="G33" s="192"/>
+      <c r="H33" s="192"/>
+      <c r="I33" s="192"/>
+      <c r="J33" s="192"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="195"/>
-      <c r="F34" s="195"/>
-      <c r="G34" s="195"/>
-      <c r="H34" s="195"/>
-      <c r="I34" s="195"/>
-      <c r="J34" s="195"/>
+      <c r="E34" s="192"/>
+      <c r="F34" s="192"/>
+      <c r="G34" s="192"/>
+      <c r="H34" s="192"/>
+      <c r="I34" s="192"/>
+      <c r="J34" s="192"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="195"/>
-      <c r="F35" s="195"/>
-      <c r="G35" s="195"/>
-      <c r="H35" s="195"/>
-      <c r="I35" s="195"/>
-      <c r="J35" s="195"/>
+      <c r="E35" s="192"/>
+      <c r="F35" s="192"/>
+      <c r="G35" s="192"/>
+      <c r="H35" s="192"/>
+      <c r="I35" s="192"/>
+      <c r="J35" s="192"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="195"/>
-      <c r="F36" s="195"/>
-      <c r="G36" s="195"/>
-      <c r="H36" s="195"/>
-      <c r="I36" s="195"/>
-      <c r="J36" s="195"/>
+      <c r="E36" s="192"/>
+      <c r="F36" s="192"/>
+      <c r="G36" s="192"/>
+      <c r="H36" s="192"/>
+      <c r="I36" s="192"/>
+      <c r="J36" s="192"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="195"/>
-      <c r="F37" s="195"/>
-      <c r="G37" s="195"/>
-      <c r="H37" s="195"/>
-      <c r="I37" s="195"/>
-      <c r="J37" s="195"/>
+      <c r="E37" s="192"/>
+      <c r="F37" s="192"/>
+      <c r="G37" s="192"/>
+      <c r="H37" s="192"/>
+      <c r="I37" s="192"/>
+      <c r="J37" s="192"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="195"/>
-      <c r="F38" s="195"/>
-      <c r="G38" s="195"/>
-      <c r="H38" s="195"/>
-      <c r="I38" s="195"/>
-      <c r="J38" s="195"/>
+      <c r="E38" s="192"/>
+      <c r="F38" s="192"/>
+      <c r="G38" s="192"/>
+      <c r="H38" s="192"/>
+      <c r="I38" s="192"/>
+      <c r="J38" s="192"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="195"/>
-      <c r="F39" s="195"/>
-      <c r="G39" s="195"/>
-      <c r="H39" s="195"/>
-      <c r="I39" s="195"/>
-      <c r="J39" s="195"/>
+      <c r="E39" s="192"/>
+      <c r="F39" s="192"/>
+      <c r="G39" s="192"/>
+      <c r="H39" s="192"/>
+      <c r="I39" s="192"/>
+      <c r="J39" s="192"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="195"/>
-      <c r="F40" s="195"/>
-      <c r="G40" s="195"/>
-      <c r="H40" s="195"/>
-      <c r="I40" s="195"/>
-      <c r="J40" s="195"/>
+      <c r="E40" s="192"/>
+      <c r="F40" s="192"/>
+      <c r="G40" s="192"/>
+      <c r="H40" s="192"/>
+      <c r="I40" s="192"/>
+      <c r="J40" s="192"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="195"/>
-      <c r="F41" s="195"/>
-      <c r="G41" s="195"/>
-      <c r="H41" s="195"/>
-      <c r="I41" s="195"/>
-      <c r="J41" s="195"/>
+      <c r="E41" s="192"/>
+      <c r="F41" s="192"/>
+      <c r="G41" s="192"/>
+      <c r="H41" s="192"/>
+      <c r="I41" s="192"/>
+      <c r="J41" s="192"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="195"/>
-      <c r="F42" s="195"/>
-      <c r="G42" s="195"/>
-      <c r="H42" s="195"/>
-      <c r="I42" s="195"/>
-      <c r="J42" s="195"/>
+      <c r="E42" s="192"/>
+      <c r="F42" s="192"/>
+      <c r="G42" s="192"/>
+      <c r="H42" s="192"/>
+      <c r="I42" s="192"/>
+      <c r="J42" s="192"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E24:J24"/>
     <mergeCell ref="E41:J41"/>
     <mergeCell ref="E42:J42"/>
     <mergeCell ref="E31:J31"/>
@@ -8919,18 +9088,14 @@
     <mergeCell ref="E38:J38"/>
     <mergeCell ref="E39:J39"/>
     <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E20:J20"/>
-    <mergeCell ref="E21:J21"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2">
@@ -8947,8 +9112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8974,10 +9139,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="214" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="186"/>
+      <c r="B1" s="214"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -9002,9 +9167,9 @@
       <c r="I1" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="126">
+      <c r="J1" s="126" t="str">
         <f>'Update History'!J1</f>
-        <v>0</v>
+        <v>Thị Phượng</v>
       </c>
       <c r="K1" s="17"/>
       <c r="L1" s="17"/>
@@ -9015,8 +9180,8 @@
       <c r="Q1" s="17"/>
     </row>
     <row r="2" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="186"/>
-      <c r="B2" s="186"/>
+      <c r="A2" s="214"/>
+      <c r="B2" s="214"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -9043,7 +9208,7 @@
       </c>
       <c r="J2" s="15">
         <f>'Update History'!J2</f>
-        <v>0</v>
+        <v>42381</v>
       </c>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
@@ -9054,16 +9219,16 @@
       <c r="Q2" s="17"/>
     </row>
     <row r="3" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="241"/>
-      <c r="B3" s="242"/>
-      <c r="C3" s="242"/>
-      <c r="D3" s="242"/>
-      <c r="E3" s="242"/>
-      <c r="F3" s="242"/>
-      <c r="G3" s="242"/>
-      <c r="H3" s="242"/>
-      <c r="I3" s="242"/>
-      <c r="J3" s="243"/>
+      <c r="A3" s="251"/>
+      <c r="B3" s="252"/>
+      <c r="C3" s="252"/>
+      <c r="D3" s="252"/>
+      <c r="E3" s="252"/>
+      <c r="F3" s="252"/>
+      <c r="G3" s="252"/>
+      <c r="H3" s="252"/>
+      <c r="I3" s="252"/>
+      <c r="J3" s="253"/>
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
@@ -9097,12 +9262,12 @@
       <c r="H4" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="238" t="s">
+      <c r="I4" s="248" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="239"/>
-      <c r="K4" s="239"/>
-      <c r="L4" s="240"/>
+      <c r="J4" s="249"/>
+      <c r="K4" s="249"/>
+      <c r="L4" s="250"/>
       <c r="M4" s="66" t="s">
         <v>44</v>
       </c>
@@ -9136,12 +9301,12 @@
       <c r="H5" s="166" t="s">
         <v>231</v>
       </c>
-      <c r="I5" s="247" t="s">
+      <c r="I5" s="257" t="s">
         <v>232</v>
       </c>
-      <c r="J5" s="248"/>
-      <c r="K5" s="248"/>
-      <c r="L5" s="249"/>
+      <c r="J5" s="258"/>
+      <c r="K5" s="258"/>
+      <c r="L5" s="259"/>
       <c r="M5" s="151"/>
       <c r="N5" s="151"/>
       <c r="O5" s="151"/>
@@ -9165,63 +9330,83 @@
       <c r="H6" s="166" t="s">
         <v>175</v>
       </c>
-      <c r="I6" s="244" t="s">
+      <c r="I6" s="260" t="s">
         <v>228</v>
       </c>
-      <c r="J6" s="245"/>
-      <c r="K6" s="245"/>
-      <c r="L6" s="246"/>
+      <c r="J6" s="261"/>
+      <c r="K6" s="261"/>
+      <c r="L6" s="262"/>
       <c r="M6" s="151"/>
       <c r="N6" s="151"/>
       <c r="O6" s="151"/>
       <c r="P6" s="151"/>
       <c r="Q6" s="151"/>
     </row>
-    <row r="7" spans="1:17" s="266" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="255"/>
-      <c r="B7" s="256"/>
-      <c r="C7" s="257"/>
-      <c r="D7" s="258"/>
-      <c r="E7" s="259" t="s">
+    <row r="7" spans="1:17" s="191" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="183"/>
+      <c r="B7" s="184"/>
+      <c r="C7" s="185"/>
+      <c r="D7" s="186"/>
+      <c r="E7" s="187" t="s">
         <v>235</v>
       </c>
-      <c r="F7" s="260"/>
-      <c r="G7" s="260" t="s">
+      <c r="F7" s="188"/>
+      <c r="G7" s="188" t="s">
         <v>236</v>
       </c>
-      <c r="H7" s="261" t="s">
+      <c r="H7" s="189" t="s">
         <v>238</v>
       </c>
-      <c r="I7" s="262" t="s">
+      <c r="I7" s="254" t="s">
         <v>237</v>
       </c>
-      <c r="J7" s="263"/>
-      <c r="K7" s="263"/>
-      <c r="L7" s="264"/>
-      <c r="M7" s="265"/>
-      <c r="N7" s="265"/>
-      <c r="O7" s="265"/>
-      <c r="P7" s="265"/>
-      <c r="Q7" s="265"/>
-    </row>
-    <row r="8" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="233"/>
-      <c r="J8" s="234"/>
-      <c r="K8" s="234"/>
-      <c r="L8" s="235"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
-      <c r="O8" s="60"/>
-      <c r="P8" s="60"/>
-      <c r="Q8" s="60"/>
+      <c r="J7" s="255"/>
+      <c r="K7" s="255"/>
+      <c r="L7" s="256"/>
+      <c r="M7" s="190"/>
+      <c r="N7" s="190"/>
+      <c r="O7" s="190"/>
+      <c r="P7" s="190"/>
+      <c r="Q7" s="190"/>
+    </row>
+    <row r="8" spans="1:17" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="269"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="270" t="s">
+        <v>243</v>
+      </c>
+      <c r="F8" s="268" t="s">
+        <v>172</v>
+      </c>
+      <c r="G8" s="268" t="s">
+        <v>236</v>
+      </c>
+      <c r="H8" s="271" t="s">
+        <v>242</v>
+      </c>
+      <c r="I8" s="272" t="s">
+        <v>244</v>
+      </c>
+      <c r="J8" s="273"/>
+      <c r="K8" s="273"/>
+      <c r="L8" s="274"/>
+      <c r="M8" s="275" t="s">
+        <v>245</v>
+      </c>
+      <c r="N8" s="271" t="s">
+        <v>246</v>
+      </c>
+      <c r="O8" s="276" t="s">
+        <v>249</v>
+      </c>
+      <c r="P8" s="276" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q8" s="270" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="56"/>
@@ -9232,10 +9417,10 @@
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
       <c r="H9" s="51"/>
-      <c r="I9" s="233"/>
-      <c r="J9" s="234"/>
-      <c r="K9" s="234"/>
-      <c r="L9" s="235"/>
+      <c r="I9" s="243"/>
+      <c r="J9" s="244"/>
+      <c r="K9" s="244"/>
+      <c r="L9" s="245"/>
       <c r="M9" s="60"/>
       <c r="N9" s="60"/>
       <c r="O9" s="60"/>
@@ -9251,10 +9436,10 @@
       <c r="F10" s="55"/>
       <c r="G10" s="55"/>
       <c r="H10" s="55"/>
-      <c r="I10" s="233"/>
-      <c r="J10" s="234"/>
-      <c r="K10" s="234"/>
-      <c r="L10" s="235"/>
+      <c r="I10" s="243"/>
+      <c r="J10" s="244"/>
+      <c r="K10" s="244"/>
+      <c r="L10" s="245"/>
       <c r="M10" s="60"/>
       <c r="N10" s="60"/>
       <c r="O10" s="60"/>
@@ -9270,10 +9455,10 @@
       <c r="F11" s="55"/>
       <c r="G11" s="55"/>
       <c r="H11" s="55"/>
-      <c r="I11" s="233"/>
-      <c r="J11" s="234"/>
-      <c r="K11" s="234"/>
-      <c r="L11" s="235"/>
+      <c r="I11" s="243"/>
+      <c r="J11" s="244"/>
+      <c r="K11" s="244"/>
+      <c r="L11" s="245"/>
       <c r="M11" s="60"/>
       <c r="N11" s="60"/>
       <c r="O11" s="60"/>
@@ -9285,361 +9470,339 @@
       <c r="B12" s="35"/>
       <c r="C12" s="36"/>
       <c r="D12" s="34"/>
-      <c r="E12" s="195"/>
-      <c r="F12" s="195"/>
-      <c r="G12" s="195"/>
-      <c r="H12" s="195"/>
-      <c r="I12" s="195"/>
-      <c r="J12" s="195"/>
+      <c r="E12" s="192"/>
+      <c r="F12" s="192"/>
+      <c r="G12" s="192"/>
+      <c r="H12" s="192"/>
+      <c r="I12" s="192"/>
+      <c r="J12" s="192"/>
     </row>
     <row r="13" spans="1:17" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="35"/>
       <c r="C13" s="36"/>
       <c r="D13" s="34"/>
-      <c r="E13" s="195"/>
-      <c r="F13" s="195"/>
-      <c r="G13" s="195"/>
-      <c r="H13" s="195"/>
-      <c r="I13" s="195"/>
-      <c r="J13" s="195"/>
+      <c r="E13" s="192"/>
+      <c r="F13" s="192"/>
+      <c r="G13" s="192"/>
+      <c r="H13" s="192"/>
+      <c r="I13" s="192"/>
+      <c r="J13" s="192"/>
     </row>
     <row r="14" spans="1:17" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="35"/>
       <c r="C14" s="36"/>
       <c r="D14" s="34"/>
-      <c r="E14" s="195"/>
-      <c r="F14" s="195"/>
-      <c r="G14" s="195"/>
-      <c r="H14" s="195"/>
-      <c r="I14" s="195"/>
-      <c r="J14" s="195"/>
+      <c r="E14" s="192"/>
+      <c r="F14" s="192"/>
+      <c r="G14" s="192"/>
+      <c r="H14" s="192"/>
+      <c r="I14" s="192"/>
+      <c r="J14" s="192"/>
     </row>
     <row r="15" spans="1:17" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="195"/>
-      <c r="F15" s="195"/>
-      <c r="G15" s="195"/>
-      <c r="H15" s="195"/>
-      <c r="I15" s="195"/>
-      <c r="J15" s="195"/>
+      <c r="E15" s="192"/>
+      <c r="F15" s="192"/>
+      <c r="G15" s="192"/>
+      <c r="H15" s="192"/>
+      <c r="I15" s="192"/>
+      <c r="J15" s="192"/>
     </row>
     <row r="16" spans="1:17" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="195"/>
-      <c r="F16" s="195"/>
-      <c r="G16" s="195"/>
-      <c r="H16" s="195"/>
-      <c r="I16" s="195"/>
-      <c r="J16" s="195"/>
+      <c r="E16" s="192"/>
+      <c r="F16" s="192"/>
+      <c r="G16" s="192"/>
+      <c r="H16" s="192"/>
+      <c r="I16" s="192"/>
+      <c r="J16" s="192"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="195"/>
-      <c r="F17" s="195"/>
-      <c r="G17" s="195"/>
-      <c r="H17" s="195"/>
-      <c r="I17" s="195"/>
-      <c r="J17" s="195"/>
+      <c r="E17" s="192"/>
+      <c r="F17" s="192"/>
+      <c r="G17" s="192"/>
+      <c r="H17" s="192"/>
+      <c r="I17" s="192"/>
+      <c r="J17" s="192"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="195"/>
-      <c r="F18" s="195"/>
-      <c r="G18" s="195"/>
-      <c r="H18" s="195"/>
-      <c r="I18" s="195"/>
-      <c r="J18" s="195"/>
+      <c r="E18" s="192"/>
+      <c r="F18" s="192"/>
+      <c r="G18" s="192"/>
+      <c r="H18" s="192"/>
+      <c r="I18" s="192"/>
+      <c r="J18" s="192"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="195"/>
-      <c r="F19" s="195"/>
-      <c r="G19" s="195"/>
-      <c r="H19" s="195"/>
-      <c r="I19" s="195"/>
-      <c r="J19" s="195"/>
+      <c r="E19" s="192"/>
+      <c r="F19" s="192"/>
+      <c r="G19" s="192"/>
+      <c r="H19" s="192"/>
+      <c r="I19" s="192"/>
+      <c r="J19" s="192"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="195"/>
-      <c r="F20" s="195"/>
-      <c r="G20" s="195"/>
-      <c r="H20" s="195"/>
-      <c r="I20" s="195"/>
-      <c r="J20" s="195"/>
+      <c r="E20" s="192"/>
+      <c r="F20" s="192"/>
+      <c r="G20" s="192"/>
+      <c r="H20" s="192"/>
+      <c r="I20" s="192"/>
+      <c r="J20" s="192"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="195"/>
-      <c r="F21" s="195"/>
-      <c r="G21" s="195"/>
-      <c r="H21" s="195"/>
-      <c r="I21" s="195"/>
-      <c r="J21" s="195"/>
+      <c r="E21" s="192"/>
+      <c r="F21" s="192"/>
+      <c r="G21" s="192"/>
+      <c r="H21" s="192"/>
+      <c r="I21" s="192"/>
+      <c r="J21" s="192"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="34"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="195"/>
-      <c r="F22" s="195"/>
-      <c r="G22" s="195"/>
-      <c r="H22" s="195"/>
-      <c r="I22" s="195"/>
-      <c r="J22" s="195"/>
+      <c r="E22" s="192"/>
+      <c r="F22" s="192"/>
+      <c r="G22" s="192"/>
+      <c r="H22" s="192"/>
+      <c r="I22" s="192"/>
+      <c r="J22" s="192"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="195"/>
-      <c r="F23" s="195"/>
-      <c r="G23" s="195"/>
-      <c r="H23" s="195"/>
-      <c r="I23" s="195"/>
-      <c r="J23" s="195"/>
+      <c r="E23" s="192"/>
+      <c r="F23" s="192"/>
+      <c r="G23" s="192"/>
+      <c r="H23" s="192"/>
+      <c r="I23" s="192"/>
+      <c r="J23" s="192"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="195"/>
-      <c r="F24" s="195"/>
-      <c r="G24" s="195"/>
-      <c r="H24" s="195"/>
-      <c r="I24" s="195"/>
-      <c r="J24" s="195"/>
+      <c r="E24" s="192"/>
+      <c r="F24" s="192"/>
+      <c r="G24" s="192"/>
+      <c r="H24" s="192"/>
+      <c r="I24" s="192"/>
+      <c r="J24" s="192"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="195"/>
-      <c r="F25" s="195"/>
-      <c r="G25" s="195"/>
-      <c r="H25" s="195"/>
-      <c r="I25" s="195"/>
-      <c r="J25" s="195"/>
+      <c r="E25" s="192"/>
+      <c r="F25" s="192"/>
+      <c r="G25" s="192"/>
+      <c r="H25" s="192"/>
+      <c r="I25" s="192"/>
+      <c r="J25" s="192"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="195"/>
-      <c r="F26" s="195"/>
-      <c r="G26" s="195"/>
-      <c r="H26" s="195"/>
-      <c r="I26" s="195"/>
-      <c r="J26" s="195"/>
+      <c r="E26" s="192"/>
+      <c r="F26" s="192"/>
+      <c r="G26" s="192"/>
+      <c r="H26" s="192"/>
+      <c r="I26" s="192"/>
+      <c r="J26" s="192"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="195"/>
-      <c r="F27" s="195"/>
-      <c r="G27" s="195"/>
-      <c r="H27" s="195"/>
-      <c r="I27" s="195"/>
-      <c r="J27" s="195"/>
+      <c r="E27" s="192"/>
+      <c r="F27" s="192"/>
+      <c r="G27" s="192"/>
+      <c r="H27" s="192"/>
+      <c r="I27" s="192"/>
+      <c r="J27" s="192"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="195"/>
-      <c r="F28" s="195"/>
-      <c r="G28" s="195"/>
-      <c r="H28" s="195"/>
-      <c r="I28" s="195"/>
-      <c r="J28" s="195"/>
+      <c r="E28" s="192"/>
+      <c r="F28" s="192"/>
+      <c r="G28" s="192"/>
+      <c r="H28" s="192"/>
+      <c r="I28" s="192"/>
+      <c r="J28" s="192"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="195"/>
-      <c r="F29" s="195"/>
-      <c r="G29" s="195"/>
-      <c r="H29" s="195"/>
-      <c r="I29" s="195"/>
-      <c r="J29" s="195"/>
+      <c r="E29" s="192"/>
+      <c r="F29" s="192"/>
+      <c r="G29" s="192"/>
+      <c r="H29" s="192"/>
+      <c r="I29" s="192"/>
+      <c r="J29" s="192"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="195"/>
-      <c r="F30" s="195"/>
-      <c r="G30" s="195"/>
-      <c r="H30" s="195"/>
-      <c r="I30" s="195"/>
-      <c r="J30" s="195"/>
+      <c r="E30" s="192"/>
+      <c r="F30" s="192"/>
+      <c r="G30" s="192"/>
+      <c r="H30" s="192"/>
+      <c r="I30" s="192"/>
+      <c r="J30" s="192"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="195"/>
-      <c r="F31" s="195"/>
-      <c r="G31" s="195"/>
-      <c r="H31" s="195"/>
-      <c r="I31" s="195"/>
-      <c r="J31" s="195"/>
+      <c r="E31" s="192"/>
+      <c r="F31" s="192"/>
+      <c r="G31" s="192"/>
+      <c r="H31" s="192"/>
+      <c r="I31" s="192"/>
+      <c r="J31" s="192"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="34"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="195"/>
-      <c r="F32" s="195"/>
-      <c r="G32" s="195"/>
-      <c r="H32" s="195"/>
-      <c r="I32" s="195"/>
-      <c r="J32" s="195"/>
+      <c r="E32" s="192"/>
+      <c r="F32" s="192"/>
+      <c r="G32" s="192"/>
+      <c r="H32" s="192"/>
+      <c r="I32" s="192"/>
+      <c r="J32" s="192"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="195"/>
-      <c r="F33" s="195"/>
-      <c r="G33" s="195"/>
-      <c r="H33" s="195"/>
-      <c r="I33" s="195"/>
-      <c r="J33" s="195"/>
+      <c r="E33" s="192"/>
+      <c r="F33" s="192"/>
+      <c r="G33" s="192"/>
+      <c r="H33" s="192"/>
+      <c r="I33" s="192"/>
+      <c r="J33" s="192"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="195"/>
-      <c r="F34" s="195"/>
-      <c r="G34" s="195"/>
-      <c r="H34" s="195"/>
-      <c r="I34" s="195"/>
-      <c r="J34" s="195"/>
+      <c r="E34" s="192"/>
+      <c r="F34" s="192"/>
+      <c r="G34" s="192"/>
+      <c r="H34" s="192"/>
+      <c r="I34" s="192"/>
+      <c r="J34" s="192"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="195"/>
-      <c r="F35" s="195"/>
-      <c r="G35" s="195"/>
-      <c r="H35" s="195"/>
-      <c r="I35" s="195"/>
-      <c r="J35" s="195"/>
+      <c r="E35" s="192"/>
+      <c r="F35" s="192"/>
+      <c r="G35" s="192"/>
+      <c r="H35" s="192"/>
+      <c r="I35" s="192"/>
+      <c r="J35" s="192"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="195"/>
-      <c r="F36" s="195"/>
-      <c r="G36" s="195"/>
-      <c r="H36" s="195"/>
-      <c r="I36" s="195"/>
-      <c r="J36" s="195"/>
+      <c r="E36" s="192"/>
+      <c r="F36" s="192"/>
+      <c r="G36" s="192"/>
+      <c r="H36" s="192"/>
+      <c r="I36" s="192"/>
+      <c r="J36" s="192"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="195"/>
-      <c r="F37" s="195"/>
-      <c r="G37" s="195"/>
-      <c r="H37" s="195"/>
-      <c r="I37" s="195"/>
-      <c r="J37" s="195"/>
+      <c r="E37" s="192"/>
+      <c r="F37" s="192"/>
+      <c r="G37" s="192"/>
+      <c r="H37" s="192"/>
+      <c r="I37" s="192"/>
+      <c r="J37" s="192"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="195"/>
-      <c r="F38" s="195"/>
-      <c r="G38" s="195"/>
-      <c r="H38" s="195"/>
-      <c r="I38" s="195"/>
-      <c r="J38" s="195"/>
+      <c r="E38" s="192"/>
+      <c r="F38" s="192"/>
+      <c r="G38" s="192"/>
+      <c r="H38" s="192"/>
+      <c r="I38" s="192"/>
+      <c r="J38" s="192"/>
     </row>
     <row r="39" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="195"/>
-      <c r="F39" s="195"/>
-      <c r="G39" s="195"/>
-      <c r="H39" s="195"/>
-      <c r="I39" s="195"/>
-      <c r="J39" s="195"/>
+      <c r="E39" s="192"/>
+      <c r="F39" s="192"/>
+      <c r="G39" s="192"/>
+      <c r="H39" s="192"/>
+      <c r="I39" s="192"/>
+      <c r="J39" s="192"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E14:J14"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="E12:J12"/>
-    <mergeCell ref="E13:J13"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
-    <mergeCell ref="I5:L5"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E20:J20"/>
-    <mergeCell ref="E21:J21"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
     <mergeCell ref="E39:J39"/>
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="I6:L6"/>
@@ -9656,15 +9819,37 @@
     <mergeCell ref="E31:J31"/>
     <mergeCell ref="E25:J25"/>
     <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E14:J14"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="I5:L5"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2">
       <formula1>"ASOFT - ERP.NET,ASOFT - ACC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5 G7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5 G7:G8">
       <formula1>"SQL Script, ID SQL, ID Store, ID Function, ID Trigger"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5 F7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5 F7:F8">
       <formula1>"Select,Insert,Update,Delete"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9678,8 +9863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A18" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9698,11 +9883,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="214" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="186"/>
-      <c r="C1" s="186"/>
+      <c r="B1" s="214"/>
+      <c r="C1" s="214"/>
       <c r="D1" s="46" t="s">
         <v>1</v>
       </c>
@@ -9727,15 +9912,15 @@
       <c r="J1" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="126">
+      <c r="K1" s="126" t="str">
         <f>'Update History'!J1</f>
-        <v>0</v>
+        <v>Thị Phượng</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="186"/>
-      <c r="B2" s="186"/>
-      <c r="C2" s="186"/>
+      <c r="A2" s="214"/>
+      <c r="B2" s="214"/>
+      <c r="C2" s="214"/>
       <c r="D2" s="46" t="s">
         <v>7</v>
       </c>
@@ -9762,7 +9947,7 @@
       </c>
       <c r="K2" s="15">
         <f>'Update History'!J2</f>
-        <v>0</v>
+        <v>42381</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -10075,18 +10260,20 @@
       <c r="J23" s="181"/>
       <c r="K23" s="182"/>
     </row>
-    <row r="24" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="157"/>
-      <c r="B24" s="156"/>
-      <c r="C24" s="161"/>
-      <c r="D24" s="155"/>
-      <c r="E24" s="156"/>
-      <c r="F24" s="156"/>
-      <c r="G24" s="156"/>
-      <c r="H24" s="160"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="68"/>
+    <row r="24" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="286"/>
+      <c r="B24" s="287"/>
+      <c r="C24" s="288" t="s">
+        <v>256</v>
+      </c>
+      <c r="D24" s="284"/>
+      <c r="E24" s="284"/>
+      <c r="F24" s="284"/>
+      <c r="G24" s="284"/>
+      <c r="H24" s="284"/>
+      <c r="I24" s="284"/>
+      <c r="J24" s="284"/>
+      <c r="K24" s="285"/>
       <c r="L24" s="17"/>
     </row>
     <row r="25" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -10171,12 +10358,12 @@
       <c r="C30" s="39"/>
       <c r="D30" s="42"/>
       <c r="E30" s="38"/>
-      <c r="F30" s="250"/>
-      <c r="G30" s="250"/>
-      <c r="H30" s="250"/>
-      <c r="I30" s="250"/>
-      <c r="J30" s="250"/>
-      <c r="K30" s="250"/>
+      <c r="F30" s="263"/>
+      <c r="G30" s="263"/>
+      <c r="H30" s="263"/>
+      <c r="I30" s="263"/>
+      <c r="J30" s="263"/>
+      <c r="K30" s="263"/>
       <c r="L30" s="17"/>
     </row>
     <row r="31" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -10185,12 +10372,12 @@
       <c r="C31" s="39"/>
       <c r="D31" s="42"/>
       <c r="E31" s="38"/>
-      <c r="F31" s="250"/>
-      <c r="G31" s="250"/>
-      <c r="H31" s="250"/>
-      <c r="I31" s="250"/>
-      <c r="J31" s="250"/>
-      <c r="K31" s="250"/>
+      <c r="F31" s="263"/>
+      <c r="G31" s="263"/>
+      <c r="H31" s="263"/>
+      <c r="I31" s="263"/>
+      <c r="J31" s="263"/>
+      <c r="K31" s="263"/>
       <c r="L31" s="17"/>
     </row>
     <row r="32" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -10199,12 +10386,12 @@
       <c r="C32" s="39"/>
       <c r="D32" s="42"/>
       <c r="E32" s="38"/>
-      <c r="F32" s="250"/>
-      <c r="G32" s="250"/>
-      <c r="H32" s="250"/>
-      <c r="I32" s="250"/>
-      <c r="J32" s="250"/>
-      <c r="K32" s="250"/>
+      <c r="F32" s="263"/>
+      <c r="G32" s="263"/>
+      <c r="H32" s="263"/>
+      <c r="I32" s="263"/>
+      <c r="J32" s="263"/>
+      <c r="K32" s="263"/>
       <c r="L32" s="17"/>
     </row>
     <row r="33" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10213,12 +10400,12 @@
       <c r="C33" s="39"/>
       <c r="D33" s="42"/>
       <c r="E33" s="38"/>
-      <c r="F33" s="250"/>
-      <c r="G33" s="250"/>
-      <c r="H33" s="250"/>
-      <c r="I33" s="250"/>
-      <c r="J33" s="250"/>
-      <c r="K33" s="250"/>
+      <c r="F33" s="263"/>
+      <c r="G33" s="263"/>
+      <c r="H33" s="263"/>
+      <c r="I33" s="263"/>
+      <c r="J33" s="263"/>
+      <c r="K33" s="263"/>
       <c r="L33" s="17"/>
     </row>
     <row r="34" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -10404,12 +10591,13 @@
       <c r="L46" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="F30:K30"/>
     <mergeCell ref="F31:K31"/>
     <mergeCell ref="F32:K32"/>
     <mergeCell ref="F33:K33"/>
     <mergeCell ref="A1:C2"/>
+    <mergeCell ref="C24:K24"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
@@ -10446,11 +10634,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="214" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="186"/>
-      <c r="C1" s="186"/>
+      <c r="B1" s="214"/>
+      <c r="C1" s="214"/>
       <c r="D1" s="46" t="s">
         <v>1</v>
       </c>
@@ -10473,9 +10661,9 @@
       <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="186"/>
-      <c r="B2" s="186"/>
-      <c r="C2" s="186"/>
+      <c r="A2" s="214"/>
+      <c r="B2" s="214"/>
+      <c r="C2" s="214"/>
       <c r="D2" s="46" t="s">
         <v>7</v>
       </c>
@@ -10845,12 +11033,12 @@
       <c r="C28" s="39"/>
       <c r="D28" s="42"/>
       <c r="E28" s="38"/>
-      <c r="F28" s="250"/>
-      <c r="G28" s="250"/>
-      <c r="H28" s="250"/>
-      <c r="I28" s="250"/>
-      <c r="J28" s="250"/>
-      <c r="K28" s="250"/>
+      <c r="F28" s="263"/>
+      <c r="G28" s="263"/>
+      <c r="H28" s="263"/>
+      <c r="I28" s="263"/>
+      <c r="J28" s="263"/>
+      <c r="K28" s="263"/>
       <c r="L28" s="17"/>
     </row>
     <row r="29" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -10859,12 +11047,12 @@
       <c r="C29" s="39"/>
       <c r="D29" s="42"/>
       <c r="E29" s="38"/>
-      <c r="F29" s="250"/>
-      <c r="G29" s="250"/>
-      <c r="H29" s="250"/>
-      <c r="I29" s="250"/>
-      <c r="J29" s="250"/>
-      <c r="K29" s="250"/>
+      <c r="F29" s="263"/>
+      <c r="G29" s="263"/>
+      <c r="H29" s="263"/>
+      <c r="I29" s="263"/>
+      <c r="J29" s="263"/>
+      <c r="K29" s="263"/>
       <c r="L29" s="17"/>
     </row>
     <row r="30" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -10873,12 +11061,12 @@
       <c r="C30" s="39"/>
       <c r="D30" s="42"/>
       <c r="E30" s="38"/>
-      <c r="F30" s="250"/>
-      <c r="G30" s="250"/>
-      <c r="H30" s="250"/>
-      <c r="I30" s="250"/>
-      <c r="J30" s="250"/>
-      <c r="K30" s="250"/>
+      <c r="F30" s="263"/>
+      <c r="G30" s="263"/>
+      <c r="H30" s="263"/>
+      <c r="I30" s="263"/>
+      <c r="J30" s="263"/>
+      <c r="K30" s="263"/>
       <c r="L30" s="17"/>
     </row>
     <row r="31" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10887,12 +11075,12 @@
       <c r="C31" s="39"/>
       <c r="D31" s="42"/>
       <c r="E31" s="38"/>
-      <c r="F31" s="250"/>
-      <c r="G31" s="250"/>
-      <c r="H31" s="250"/>
-      <c r="I31" s="250"/>
-      <c r="J31" s="250"/>
-      <c r="K31" s="250"/>
+      <c r="F31" s="263"/>
+      <c r="G31" s="263"/>
+      <c r="H31" s="263"/>
+      <c r="I31" s="263"/>
+      <c r="J31" s="263"/>
+      <c r="K31" s="263"/>
       <c r="L31" s="17"/>
     </row>
     <row r="32" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -11112,14 +11300,14 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="78"/>
-      <c r="E2" s="251" t="s">
+      <c r="E2" s="264" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="251"/>
-      <c r="G2" s="251"/>
-      <c r="H2" s="251"/>
-      <c r="I2" s="251"/>
-      <c r="J2" s="251"/>
+      <c r="F2" s="264"/>
+      <c r="G2" s="264"/>
+      <c r="H2" s="264"/>
+      <c r="I2" s="264"/>
+      <c r="J2" s="264"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="79"/>
@@ -11540,11 +11728,11 @@
       <c r="B28" s="78"/>
       <c r="C28" s="78"/>
       <c r="D28" s="78"/>
-      <c r="E28" s="252" t="s">
+      <c r="E28" s="265" t="s">
         <v>107</v>
       </c>
-      <c r="F28" s="253"/>
-      <c r="G28" s="254"/>
+      <c r="F28" s="266"/>
+      <c r="G28" s="267"/>
       <c r="H28" s="78"/>
       <c r="I28" s="78"/>
       <c r="J28" s="78"/>

</xml_diff>

<commit_message>
Bổ sung nội dung cho Customize Hoàng Trần
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/WF0008 Danh muc phieu nhap xuat vcnb.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/WF0008 Danh muc phieu nhap xuat vcnb.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Update History" sheetId="1" r:id="rId1"/>
@@ -2903,9 +2903,6 @@
 1</t>
   </si>
   <si>
-    <t>Thực hiện câu @SQL004 để kiểm tra điệu kiện để load màn hình Cập nhật khi thực hiện Click LinkEdit</t>
-  </si>
-  <si>
     <t>Load</t>
   </si>
   <si>
@@ -2935,9 +2932,13 @@
 - Nếu =0 thực thi @SQL002 load form Detail</t>
   </si>
   <si>
-    <t>- Thêm câu @SQL004 trong sheet Data Input
+    <t>CustomizeIndex = 51 (Hoàng Trần): kiểm tra điều kiện phiếu nhập xuất VCNB
+- Thêm câu @SQL004 trong sheet Data Input
 - Thêm WFML000185 và WFML000186 trong sheet Input Check
 - Thêm sự kiện Sửa trong sheet Form Func Spec</t>
+  </si>
+  <si>
+    <t>Thực hiện câu @SQL004 để kiểm tra điệu kiện để load màn hình Cập nhật khi thực hiện Click LinkEdit cho Cus Hoàng Trần</t>
   </si>
 </sst>
 </file>
@@ -3912,6 +3913,90 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3969,44 +4054,23 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4032,24 +4096,6 @@
     <xf numFmtId="14" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4077,6 +4123,15 @@
     <xf numFmtId="0" fontId="10" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4098,6 +4153,15 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4116,18 +4180,18 @@
     <xf numFmtId="0" fontId="7" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4138,69 +4202,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4541,7 +4542,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4560,10 +4561,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="214" t="s">
+      <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="214"/>
+      <c r="B1" s="210"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -4590,8 +4591,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="214"/>
-      <c r="B2" s="214"/>
+      <c r="A2" s="210"/>
+      <c r="B2" s="210"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -4642,14 +4643,14 @@
       <c r="D4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="215" t="s">
+      <c r="E4" s="211" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="215"/>
-      <c r="G4" s="215"/>
-      <c r="H4" s="215"/>
-      <c r="I4" s="215"/>
-      <c r="J4" s="215"/>
+      <c r="F4" s="211"/>
+      <c r="G4" s="211"/>
+      <c r="H4" s="211"/>
+      <c r="I4" s="211"/>
+      <c r="J4" s="211"/>
     </row>
     <row r="5" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
@@ -4666,14 +4667,14 @@
         <f>H1</f>
         <v>Thanh Sơn</v>
       </c>
-      <c r="E5" s="216" t="s">
+      <c r="E5" s="212" t="s">
         <v>176</v>
       </c>
-      <c r="F5" s="217"/>
-      <c r="G5" s="217"/>
-      <c r="H5" s="217"/>
-      <c r="I5" s="217"/>
-      <c r="J5" s="217"/>
+      <c r="F5" s="213"/>
+      <c r="G5" s="213"/>
+      <c r="H5" s="213"/>
+      <c r="I5" s="213"/>
+      <c r="J5" s="213"/>
     </row>
     <row r="6" spans="1:10" s="111" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
@@ -4688,14 +4689,14 @@
       <c r="D6" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="218" t="s">
+      <c r="E6" s="214" t="s">
         <v>179</v>
       </c>
-      <c r="F6" s="219"/>
-      <c r="G6" s="219"/>
-      <c r="H6" s="219"/>
-      <c r="I6" s="219"/>
-      <c r="J6" s="220"/>
+      <c r="F6" s="215"/>
+      <c r="G6" s="215"/>
+      <c r="H6" s="215"/>
+      <c r="I6" s="215"/>
+      <c r="J6" s="216"/>
     </row>
     <row r="7" spans="1:10" s="111" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="112">
@@ -4710,14 +4711,14 @@
       <c r="D7" s="115" t="s">
         <v>239</v>
       </c>
-      <c r="E7" s="221" t="s">
+      <c r="E7" s="217" t="s">
         <v>240</v>
       </c>
-      <c r="F7" s="222"/>
-      <c r="G7" s="222"/>
-      <c r="H7" s="222"/>
-      <c r="I7" s="222"/>
-      <c r="J7" s="223"/>
+      <c r="F7" s="218"/>
+      <c r="G7" s="218"/>
+      <c r="H7" s="218"/>
+      <c r="I7" s="218"/>
+      <c r="J7" s="219"/>
     </row>
     <row r="8" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -4732,14 +4733,14 @@
       <c r="D8" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="E8" s="211" t="s">
-        <v>257</v>
-      </c>
-      <c r="F8" s="212"/>
-      <c r="G8" s="212"/>
-      <c r="H8" s="212"/>
-      <c r="I8" s="212"/>
-      <c r="J8" s="213"/>
+      <c r="E8" s="207" t="s">
+        <v>256</v>
+      </c>
+      <c r="F8" s="208"/>
+      <c r="G8" s="208"/>
+      <c r="H8" s="208"/>
+      <c r="I8" s="208"/>
+      <c r="J8" s="209"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -4750,12 +4751,12 @@
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="26"/>
-      <c r="E9" s="193"/>
-      <c r="F9" s="194"/>
-      <c r="G9" s="194"/>
-      <c r="H9" s="194"/>
-      <c r="I9" s="194"/>
-      <c r="J9" s="195"/>
+      <c r="E9" s="221"/>
+      <c r="F9" s="222"/>
+      <c r="G9" s="222"/>
+      <c r="H9" s="222"/>
+      <c r="I9" s="222"/>
+      <c r="J9" s="223"/>
     </row>
     <row r="10" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -4766,12 +4767,12 @@
       </c>
       <c r="C10" s="117"/>
       <c r="D10" s="118"/>
-      <c r="E10" s="196"/>
-      <c r="F10" s="197"/>
-      <c r="G10" s="197"/>
-      <c r="H10" s="197"/>
-      <c r="I10" s="197"/>
-      <c r="J10" s="198"/>
+      <c r="E10" s="224"/>
+      <c r="F10" s="225"/>
+      <c r="G10" s="225"/>
+      <c r="H10" s="225"/>
+      <c r="I10" s="225"/>
+      <c r="J10" s="226"/>
     </row>
     <row r="11" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -4782,12 +4783,12 @@
       </c>
       <c r="C11" s="120"/>
       <c r="D11" s="121"/>
-      <c r="E11" s="199"/>
-      <c r="F11" s="200"/>
-      <c r="G11" s="200"/>
-      <c r="H11" s="200"/>
-      <c r="I11" s="200"/>
-      <c r="J11" s="201"/>
+      <c r="E11" s="227"/>
+      <c r="F11" s="228"/>
+      <c r="G11" s="228"/>
+      <c r="H11" s="228"/>
+      <c r="I11" s="228"/>
+      <c r="J11" s="229"/>
     </row>
     <row r="12" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -4798,12 +4799,12 @@
       </c>
       <c r="C12" s="123"/>
       <c r="D12" s="124"/>
-      <c r="E12" s="202"/>
-      <c r="F12" s="203"/>
-      <c r="G12" s="203"/>
-      <c r="H12" s="203"/>
-      <c r="I12" s="203"/>
-      <c r="J12" s="204"/>
+      <c r="E12" s="230"/>
+      <c r="F12" s="231"/>
+      <c r="G12" s="231"/>
+      <c r="H12" s="231"/>
+      <c r="I12" s="231"/>
+      <c r="J12" s="232"/>
     </row>
     <row r="13" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -4814,12 +4815,12 @@
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="29"/>
-      <c r="E13" s="205"/>
-      <c r="F13" s="206"/>
-      <c r="G13" s="206"/>
-      <c r="H13" s="206"/>
-      <c r="I13" s="206"/>
-      <c r="J13" s="207"/>
+      <c r="E13" s="233"/>
+      <c r="F13" s="234"/>
+      <c r="G13" s="234"/>
+      <c r="H13" s="234"/>
+      <c r="I13" s="234"/>
+      <c r="J13" s="235"/>
     </row>
     <row r="14" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
@@ -4830,357 +4831,373 @@
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="33"/>
-      <c r="E14" s="208"/>
-      <c r="F14" s="209"/>
-      <c r="G14" s="209"/>
-      <c r="H14" s="209"/>
-      <c r="I14" s="209"/>
-      <c r="J14" s="210"/>
+      <c r="E14" s="236"/>
+      <c r="F14" s="237"/>
+      <c r="G14" s="237"/>
+      <c r="H14" s="237"/>
+      <c r="I14" s="237"/>
+      <c r="J14" s="238"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="192"/>
-      <c r="F15" s="192"/>
-      <c r="G15" s="192"/>
-      <c r="H15" s="192"/>
-      <c r="I15" s="192"/>
-      <c r="J15" s="192"/>
+      <c r="E15" s="220"/>
+      <c r="F15" s="220"/>
+      <c r="G15" s="220"/>
+      <c r="H15" s="220"/>
+      <c r="I15" s="220"/>
+      <c r="J15" s="220"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="192"/>
-      <c r="F16" s="192"/>
-      <c r="G16" s="192"/>
-      <c r="H16" s="192"/>
-      <c r="I16" s="192"/>
-      <c r="J16" s="192"/>
+      <c r="E16" s="220"/>
+      <c r="F16" s="220"/>
+      <c r="G16" s="220"/>
+      <c r="H16" s="220"/>
+      <c r="I16" s="220"/>
+      <c r="J16" s="220"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="192"/>
-      <c r="F17" s="192"/>
-      <c r="G17" s="192"/>
-      <c r="H17" s="192"/>
-      <c r="I17" s="192"/>
-      <c r="J17" s="192"/>
+      <c r="E17" s="220"/>
+      <c r="F17" s="220"/>
+      <c r="G17" s="220"/>
+      <c r="H17" s="220"/>
+      <c r="I17" s="220"/>
+      <c r="J17" s="220"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="192"/>
-      <c r="F18" s="192"/>
-      <c r="G18" s="192"/>
-      <c r="H18" s="192"/>
-      <c r="I18" s="192"/>
-      <c r="J18" s="192"/>
+      <c r="E18" s="220"/>
+      <c r="F18" s="220"/>
+      <c r="G18" s="220"/>
+      <c r="H18" s="220"/>
+      <c r="I18" s="220"/>
+      <c r="J18" s="220"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="192"/>
-      <c r="F19" s="192"/>
-      <c r="G19" s="192"/>
-      <c r="H19" s="192"/>
-      <c r="I19" s="192"/>
-      <c r="J19" s="192"/>
+      <c r="E19" s="220"/>
+      <c r="F19" s="220"/>
+      <c r="G19" s="220"/>
+      <c r="H19" s="220"/>
+      <c r="I19" s="220"/>
+      <c r="J19" s="220"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="192"/>
-      <c r="F20" s="192"/>
-      <c r="G20" s="192"/>
-      <c r="H20" s="192"/>
-      <c r="I20" s="192"/>
-      <c r="J20" s="192"/>
+      <c r="E20" s="220"/>
+      <c r="F20" s="220"/>
+      <c r="G20" s="220"/>
+      <c r="H20" s="220"/>
+      <c r="I20" s="220"/>
+      <c r="J20" s="220"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="192"/>
-      <c r="F21" s="192"/>
-      <c r="G21" s="192"/>
-      <c r="H21" s="192"/>
-      <c r="I21" s="192"/>
-      <c r="J21" s="192"/>
+      <c r="E21" s="220"/>
+      <c r="F21" s="220"/>
+      <c r="G21" s="220"/>
+      <c r="H21" s="220"/>
+      <c r="I21" s="220"/>
+      <c r="J21" s="220"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="192"/>
-      <c r="F22" s="192"/>
-      <c r="G22" s="192"/>
-      <c r="H22" s="192"/>
-      <c r="I22" s="192"/>
-      <c r="J22" s="192"/>
+      <c r="E22" s="220"/>
+      <c r="F22" s="220"/>
+      <c r="G22" s="220"/>
+      <c r="H22" s="220"/>
+      <c r="I22" s="220"/>
+      <c r="J22" s="220"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="192"/>
-      <c r="F23" s="192"/>
-      <c r="G23" s="192"/>
-      <c r="H23" s="192"/>
-      <c r="I23" s="192"/>
-      <c r="J23" s="192"/>
+      <c r="E23" s="220"/>
+      <c r="F23" s="220"/>
+      <c r="G23" s="220"/>
+      <c r="H23" s="220"/>
+      <c r="I23" s="220"/>
+      <c r="J23" s="220"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="192"/>
-      <c r="F24" s="192"/>
-      <c r="G24" s="192"/>
-      <c r="H24" s="192"/>
-      <c r="I24" s="192"/>
-      <c r="J24" s="192"/>
+      <c r="E24" s="220"/>
+      <c r="F24" s="220"/>
+      <c r="G24" s="220"/>
+      <c r="H24" s="220"/>
+      <c r="I24" s="220"/>
+      <c r="J24" s="220"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="192"/>
-      <c r="F25" s="192"/>
-      <c r="G25" s="192"/>
-      <c r="H25" s="192"/>
-      <c r="I25" s="192"/>
-      <c r="J25" s="192"/>
+      <c r="E25" s="220"/>
+      <c r="F25" s="220"/>
+      <c r="G25" s="220"/>
+      <c r="H25" s="220"/>
+      <c r="I25" s="220"/>
+      <c r="J25" s="220"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="192"/>
-      <c r="F26" s="192"/>
-      <c r="G26" s="192"/>
-      <c r="H26" s="192"/>
-      <c r="I26" s="192"/>
-      <c r="J26" s="192"/>
+      <c r="E26" s="220"/>
+      <c r="F26" s="220"/>
+      <c r="G26" s="220"/>
+      <c r="H26" s="220"/>
+      <c r="I26" s="220"/>
+      <c r="J26" s="220"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="192"/>
-      <c r="F27" s="192"/>
-      <c r="G27" s="192"/>
-      <c r="H27" s="192"/>
-      <c r="I27" s="192"/>
-      <c r="J27" s="192"/>
+      <c r="E27" s="220"/>
+      <c r="F27" s="220"/>
+      <c r="G27" s="220"/>
+      <c r="H27" s="220"/>
+      <c r="I27" s="220"/>
+      <c r="J27" s="220"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="192"/>
-      <c r="F28" s="192"/>
-      <c r="G28" s="192"/>
-      <c r="H28" s="192"/>
-      <c r="I28" s="192"/>
-      <c r="J28" s="192"/>
+      <c r="E28" s="220"/>
+      <c r="F28" s="220"/>
+      <c r="G28" s="220"/>
+      <c r="H28" s="220"/>
+      <c r="I28" s="220"/>
+      <c r="J28" s="220"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="192"/>
-      <c r="F29" s="192"/>
-      <c r="G29" s="192"/>
-      <c r="H29" s="192"/>
-      <c r="I29" s="192"/>
-      <c r="J29" s="192"/>
+      <c r="E29" s="220"/>
+      <c r="F29" s="220"/>
+      <c r="G29" s="220"/>
+      <c r="H29" s="220"/>
+      <c r="I29" s="220"/>
+      <c r="J29" s="220"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="192"/>
-      <c r="F30" s="192"/>
-      <c r="G30" s="192"/>
-      <c r="H30" s="192"/>
-      <c r="I30" s="192"/>
-      <c r="J30" s="192"/>
+      <c r="E30" s="220"/>
+      <c r="F30" s="220"/>
+      <c r="G30" s="220"/>
+      <c r="H30" s="220"/>
+      <c r="I30" s="220"/>
+      <c r="J30" s="220"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="192"/>
-      <c r="F31" s="192"/>
-      <c r="G31" s="192"/>
-      <c r="H31" s="192"/>
-      <c r="I31" s="192"/>
-      <c r="J31" s="192"/>
+      <c r="E31" s="220"/>
+      <c r="F31" s="220"/>
+      <c r="G31" s="220"/>
+      <c r="H31" s="220"/>
+      <c r="I31" s="220"/>
+      <c r="J31" s="220"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="192"/>
-      <c r="F32" s="192"/>
-      <c r="G32" s="192"/>
-      <c r="H32" s="192"/>
-      <c r="I32" s="192"/>
-      <c r="J32" s="192"/>
+      <c r="E32" s="220"/>
+      <c r="F32" s="220"/>
+      <c r="G32" s="220"/>
+      <c r="H32" s="220"/>
+      <c r="I32" s="220"/>
+      <c r="J32" s="220"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="192"/>
-      <c r="F33" s="192"/>
-      <c r="G33" s="192"/>
-      <c r="H33" s="192"/>
-      <c r="I33" s="192"/>
-      <c r="J33" s="192"/>
+      <c r="E33" s="220"/>
+      <c r="F33" s="220"/>
+      <c r="G33" s="220"/>
+      <c r="H33" s="220"/>
+      <c r="I33" s="220"/>
+      <c r="J33" s="220"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="192"/>
-      <c r="F34" s="192"/>
-      <c r="G34" s="192"/>
-      <c r="H34" s="192"/>
-      <c r="I34" s="192"/>
-      <c r="J34" s="192"/>
+      <c r="E34" s="220"/>
+      <c r="F34" s="220"/>
+      <c r="G34" s="220"/>
+      <c r="H34" s="220"/>
+      <c r="I34" s="220"/>
+      <c r="J34" s="220"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="192"/>
-      <c r="F35" s="192"/>
-      <c r="G35" s="192"/>
-      <c r="H35" s="192"/>
-      <c r="I35" s="192"/>
-      <c r="J35" s="192"/>
+      <c r="E35" s="220"/>
+      <c r="F35" s="220"/>
+      <c r="G35" s="220"/>
+      <c r="H35" s="220"/>
+      <c r="I35" s="220"/>
+      <c r="J35" s="220"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="192"/>
-      <c r="F36" s="192"/>
-      <c r="G36" s="192"/>
-      <c r="H36" s="192"/>
-      <c r="I36" s="192"/>
-      <c r="J36" s="192"/>
+      <c r="E36" s="220"/>
+      <c r="F36" s="220"/>
+      <c r="G36" s="220"/>
+      <c r="H36" s="220"/>
+      <c r="I36" s="220"/>
+      <c r="J36" s="220"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="192"/>
-      <c r="F37" s="192"/>
-      <c r="G37" s="192"/>
-      <c r="H37" s="192"/>
-      <c r="I37" s="192"/>
-      <c r="J37" s="192"/>
+      <c r="E37" s="220"/>
+      <c r="F37" s="220"/>
+      <c r="G37" s="220"/>
+      <c r="H37" s="220"/>
+      <c r="I37" s="220"/>
+      <c r="J37" s="220"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="192"/>
-      <c r="F38" s="192"/>
-      <c r="G38" s="192"/>
-      <c r="H38" s="192"/>
-      <c r="I38" s="192"/>
-      <c r="J38" s="192"/>
+      <c r="E38" s="220"/>
+      <c r="F38" s="220"/>
+      <c r="G38" s="220"/>
+      <c r="H38" s="220"/>
+      <c r="I38" s="220"/>
+      <c r="J38" s="220"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="192"/>
-      <c r="F39" s="192"/>
-      <c r="G39" s="192"/>
-      <c r="H39" s="192"/>
-      <c r="I39" s="192"/>
-      <c r="J39" s="192"/>
+      <c r="E39" s="220"/>
+      <c r="F39" s="220"/>
+      <c r="G39" s="220"/>
+      <c r="H39" s="220"/>
+      <c r="I39" s="220"/>
+      <c r="J39" s="220"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="192"/>
-      <c r="F40" s="192"/>
-      <c r="G40" s="192"/>
-      <c r="H40" s="192"/>
-      <c r="I40" s="192"/>
-      <c r="J40" s="192"/>
+      <c r="E40" s="220"/>
+      <c r="F40" s="220"/>
+      <c r="G40" s="220"/>
+      <c r="H40" s="220"/>
+      <c r="I40" s="220"/>
+      <c r="J40" s="220"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="192"/>
-      <c r="F41" s="192"/>
-      <c r="G41" s="192"/>
-      <c r="H41" s="192"/>
-      <c r="I41" s="192"/>
-      <c r="J41" s="192"/>
+      <c r="E41" s="220"/>
+      <c r="F41" s="220"/>
+      <c r="G41" s="220"/>
+      <c r="H41" s="220"/>
+      <c r="I41" s="220"/>
+      <c r="J41" s="220"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="192"/>
-      <c r="F42" s="192"/>
-      <c r="G42" s="192"/>
-      <c r="H42" s="192"/>
-      <c r="I42" s="192"/>
-      <c r="J42" s="192"/>
+      <c r="E42" s="220"/>
+      <c r="F42" s="220"/>
+      <c r="G42" s="220"/>
+      <c r="H42" s="220"/>
+      <c r="I42" s="220"/>
+      <c r="J42" s="220"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E31:J31"/>
     <mergeCell ref="E20:J20"/>
     <mergeCell ref="E9:J9"/>
     <mergeCell ref="E10:J10"/>
@@ -5193,28 +5210,12 @@
     <mergeCell ref="E17:J17"/>
     <mergeCell ref="E18:J18"/>
     <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E21:J21"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E7:J7"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
@@ -5424,10 +5425,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="214" t="s">
+      <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="214"/>
+      <c r="B1" s="210"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -5458,8 +5459,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="214"/>
-      <c r="B2" s="214"/>
+      <c r="A2" s="210"/>
+      <c r="B2" s="210"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -5502,76 +5503,76 @@
       <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="214" t="s">
+      <c r="A4" s="210" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="214"/>
-      <c r="C4" s="214"/>
-      <c r="D4" s="214"/>
-      <c r="E4" s="214"/>
-      <c r="F4" s="214"/>
-      <c r="G4" s="214"/>
-      <c r="H4" s="214"/>
-      <c r="I4" s="214" t="s">
+      <c r="B4" s="210"/>
+      <c r="C4" s="210"/>
+      <c r="D4" s="210"/>
+      <c r="E4" s="210"/>
+      <c r="F4" s="210"/>
+      <c r="G4" s="210"/>
+      <c r="H4" s="210"/>
+      <c r="I4" s="210" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="214"/>
+      <c r="J4" s="210"/>
     </row>
     <row r="5" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="226"/>
-      <c r="B5" s="227"/>
-      <c r="C5" s="227"/>
-      <c r="D5" s="227"/>
-      <c r="E5" s="227"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="227"/>
-      <c r="H5" s="228"/>
-      <c r="I5" s="232" t="s">
+      <c r="A5" s="247"/>
+      <c r="B5" s="248"/>
+      <c r="C5" s="248"/>
+      <c r="D5" s="248"/>
+      <c r="E5" s="248"/>
+      <c r="F5" s="248"/>
+      <c r="G5" s="248"/>
+      <c r="H5" s="249"/>
+      <c r="I5" s="239" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="233"/>
+      <c r="J5" s="240"/>
     </row>
     <row r="6" spans="1:10" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="229"/>
-      <c r="B6" s="230"/>
-      <c r="C6" s="230"/>
-      <c r="D6" s="230"/>
-      <c r="E6" s="230"/>
-      <c r="F6" s="230"/>
-      <c r="G6" s="230"/>
-      <c r="H6" s="231"/>
-      <c r="I6" s="234" t="s">
+      <c r="A6" s="250"/>
+      <c r="B6" s="251"/>
+      <c r="C6" s="251"/>
+      <c r="D6" s="251"/>
+      <c r="E6" s="251"/>
+      <c r="F6" s="251"/>
+      <c r="G6" s="251"/>
+      <c r="H6" s="252"/>
+      <c r="I6" s="241" t="s">
         <v>177</v>
       </c>
-      <c r="J6" s="235"/>
+      <c r="J6" s="242"/>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="229"/>
-      <c r="B7" s="230"/>
-      <c r="C7" s="230"/>
-      <c r="D7" s="230"/>
-      <c r="E7" s="230"/>
-      <c r="F7" s="230"/>
-      <c r="G7" s="230"/>
-      <c r="H7" s="231"/>
-      <c r="I7" s="236" t="s">
+      <c r="A7" s="250"/>
+      <c r="B7" s="251"/>
+      <c r="C7" s="251"/>
+      <c r="D7" s="251"/>
+      <c r="E7" s="251"/>
+      <c r="F7" s="251"/>
+      <c r="G7" s="251"/>
+      <c r="H7" s="252"/>
+      <c r="I7" s="243" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="237"/>
+      <c r="J7" s="244"/>
     </row>
     <row r="8" spans="1:10" ht="336" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="229"/>
-      <c r="B8" s="230"/>
-      <c r="C8" s="230"/>
-      <c r="D8" s="230"/>
-      <c r="E8" s="230"/>
-      <c r="F8" s="230"/>
-      <c r="G8" s="230"/>
-      <c r="H8" s="231"/>
-      <c r="I8" s="224" t="s">
+      <c r="A8" s="250"/>
+      <c r="B8" s="251"/>
+      <c r="C8" s="251"/>
+      <c r="D8" s="251"/>
+      <c r="E8" s="251"/>
+      <c r="F8" s="251"/>
+      <c r="G8" s="251"/>
+      <c r="H8" s="252"/>
+      <c r="I8" s="245" t="s">
         <v>171</v>
       </c>
-      <c r="J8" s="225"/>
+      <c r="J8" s="246"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
@@ -5650,339 +5651,359 @@
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="192"/>
-      <c r="F15" s="192"/>
-      <c r="G15" s="192"/>
-      <c r="H15" s="192"/>
-      <c r="I15" s="192"/>
-      <c r="J15" s="192"/>
+      <c r="E15" s="220"/>
+      <c r="F15" s="220"/>
+      <c r="G15" s="220"/>
+      <c r="H15" s="220"/>
+      <c r="I15" s="220"/>
+      <c r="J15" s="220"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="192"/>
-      <c r="F16" s="192"/>
-      <c r="G16" s="192"/>
-      <c r="H16" s="192"/>
-      <c r="I16" s="192"/>
-      <c r="J16" s="192"/>
+      <c r="E16" s="220"/>
+      <c r="F16" s="220"/>
+      <c r="G16" s="220"/>
+      <c r="H16" s="220"/>
+      <c r="I16" s="220"/>
+      <c r="J16" s="220"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="192"/>
-      <c r="F17" s="192"/>
-      <c r="G17" s="192"/>
-      <c r="H17" s="192"/>
-      <c r="I17" s="192"/>
-      <c r="J17" s="192"/>
+      <c r="E17" s="220"/>
+      <c r="F17" s="220"/>
+      <c r="G17" s="220"/>
+      <c r="H17" s="220"/>
+      <c r="I17" s="220"/>
+      <c r="J17" s="220"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="192"/>
-      <c r="F18" s="192"/>
-      <c r="G18" s="192"/>
-      <c r="H18" s="192"/>
-      <c r="I18" s="192"/>
-      <c r="J18" s="192"/>
+      <c r="E18" s="220"/>
+      <c r="F18" s="220"/>
+      <c r="G18" s="220"/>
+      <c r="H18" s="220"/>
+      <c r="I18" s="220"/>
+      <c r="J18" s="220"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="192"/>
-      <c r="F19" s="192"/>
-      <c r="G19" s="192"/>
-      <c r="H19" s="192"/>
-      <c r="I19" s="192"/>
-      <c r="J19" s="192"/>
+      <c r="E19" s="220"/>
+      <c r="F19" s="220"/>
+      <c r="G19" s="220"/>
+      <c r="H19" s="220"/>
+      <c r="I19" s="220"/>
+      <c r="J19" s="220"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="192"/>
-      <c r="F20" s="192"/>
-      <c r="G20" s="192"/>
-      <c r="H20" s="192"/>
-      <c r="I20" s="192"/>
-      <c r="J20" s="192"/>
+      <c r="E20" s="220"/>
+      <c r="F20" s="220"/>
+      <c r="G20" s="220"/>
+      <c r="H20" s="220"/>
+      <c r="I20" s="220"/>
+      <c r="J20" s="220"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="192"/>
-      <c r="F21" s="192"/>
-      <c r="G21" s="192"/>
-      <c r="H21" s="192"/>
-      <c r="I21" s="192"/>
-      <c r="J21" s="192"/>
+      <c r="E21" s="220"/>
+      <c r="F21" s="220"/>
+      <c r="G21" s="220"/>
+      <c r="H21" s="220"/>
+      <c r="I21" s="220"/>
+      <c r="J21" s="220"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="192"/>
-      <c r="F22" s="192"/>
-      <c r="G22" s="192"/>
-      <c r="H22" s="192"/>
-      <c r="I22" s="192"/>
-      <c r="J22" s="192"/>
+      <c r="E22" s="220"/>
+      <c r="F22" s="220"/>
+      <c r="G22" s="220"/>
+      <c r="H22" s="220"/>
+      <c r="I22" s="220"/>
+      <c r="J22" s="220"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="192"/>
-      <c r="F23" s="192"/>
-      <c r="G23" s="192"/>
-      <c r="H23" s="192"/>
-      <c r="I23" s="192"/>
-      <c r="J23" s="192"/>
+      <c r="E23" s="220"/>
+      <c r="F23" s="220"/>
+      <c r="G23" s="220"/>
+      <c r="H23" s="220"/>
+      <c r="I23" s="220"/>
+      <c r="J23" s="220"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="192"/>
-      <c r="F24" s="192"/>
-      <c r="G24" s="192"/>
-      <c r="H24" s="192"/>
-      <c r="I24" s="192"/>
-      <c r="J24" s="192"/>
+      <c r="E24" s="220"/>
+      <c r="F24" s="220"/>
+      <c r="G24" s="220"/>
+      <c r="H24" s="220"/>
+      <c r="I24" s="220"/>
+      <c r="J24" s="220"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="192"/>
-      <c r="F25" s="192"/>
-      <c r="G25" s="192"/>
-      <c r="H25" s="192"/>
-      <c r="I25" s="192"/>
-      <c r="J25" s="192"/>
+      <c r="E25" s="220"/>
+      <c r="F25" s="220"/>
+      <c r="G25" s="220"/>
+      <c r="H25" s="220"/>
+      <c r="I25" s="220"/>
+      <c r="J25" s="220"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="192"/>
-      <c r="F26" s="192"/>
-      <c r="G26" s="192"/>
-      <c r="H26" s="192"/>
-      <c r="I26" s="192"/>
-      <c r="J26" s="192"/>
+      <c r="E26" s="220"/>
+      <c r="F26" s="220"/>
+      <c r="G26" s="220"/>
+      <c r="H26" s="220"/>
+      <c r="I26" s="220"/>
+      <c r="J26" s="220"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="192"/>
-      <c r="F27" s="192"/>
-      <c r="G27" s="192"/>
-      <c r="H27" s="192"/>
-      <c r="I27" s="192"/>
-      <c r="J27" s="192"/>
+      <c r="E27" s="220"/>
+      <c r="F27" s="220"/>
+      <c r="G27" s="220"/>
+      <c r="H27" s="220"/>
+      <c r="I27" s="220"/>
+      <c r="J27" s="220"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="192"/>
-      <c r="F28" s="192"/>
-      <c r="G28" s="192"/>
-      <c r="H28" s="192"/>
-      <c r="I28" s="192"/>
-      <c r="J28" s="192"/>
+      <c r="E28" s="220"/>
+      <c r="F28" s="220"/>
+      <c r="G28" s="220"/>
+      <c r="H28" s="220"/>
+      <c r="I28" s="220"/>
+      <c r="J28" s="220"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="192"/>
-      <c r="F29" s="192"/>
-      <c r="G29" s="192"/>
-      <c r="H29" s="192"/>
-      <c r="I29" s="192"/>
-      <c r="J29" s="192"/>
+      <c r="E29" s="220"/>
+      <c r="F29" s="220"/>
+      <c r="G29" s="220"/>
+      <c r="H29" s="220"/>
+      <c r="I29" s="220"/>
+      <c r="J29" s="220"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="192"/>
-      <c r="F30" s="192"/>
-      <c r="G30" s="192"/>
-      <c r="H30" s="192"/>
-      <c r="I30" s="192"/>
-      <c r="J30" s="192"/>
+      <c r="E30" s="220"/>
+      <c r="F30" s="220"/>
+      <c r="G30" s="220"/>
+      <c r="H30" s="220"/>
+      <c r="I30" s="220"/>
+      <c r="J30" s="220"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="192"/>
-      <c r="F31" s="192"/>
-      <c r="G31" s="192"/>
-      <c r="H31" s="192"/>
-      <c r="I31" s="192"/>
-      <c r="J31" s="192"/>
+      <c r="E31" s="220"/>
+      <c r="F31" s="220"/>
+      <c r="G31" s="220"/>
+      <c r="H31" s="220"/>
+      <c r="I31" s="220"/>
+      <c r="J31" s="220"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="192"/>
-      <c r="F32" s="192"/>
-      <c r="G32" s="192"/>
-      <c r="H32" s="192"/>
-      <c r="I32" s="192"/>
-      <c r="J32" s="192"/>
+      <c r="E32" s="220"/>
+      <c r="F32" s="220"/>
+      <c r="G32" s="220"/>
+      <c r="H32" s="220"/>
+      <c r="I32" s="220"/>
+      <c r="J32" s="220"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="192"/>
-      <c r="F33" s="192"/>
-      <c r="G33" s="192"/>
-      <c r="H33" s="192"/>
-      <c r="I33" s="192"/>
-      <c r="J33" s="192"/>
+      <c r="E33" s="220"/>
+      <c r="F33" s="220"/>
+      <c r="G33" s="220"/>
+      <c r="H33" s="220"/>
+      <c r="I33" s="220"/>
+      <c r="J33" s="220"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="192"/>
-      <c r="F34" s="192"/>
-      <c r="G34" s="192"/>
-      <c r="H34" s="192"/>
-      <c r="I34" s="192"/>
-      <c r="J34" s="192"/>
+      <c r="E34" s="220"/>
+      <c r="F34" s="220"/>
+      <c r="G34" s="220"/>
+      <c r="H34" s="220"/>
+      <c r="I34" s="220"/>
+      <c r="J34" s="220"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="192"/>
-      <c r="F35" s="192"/>
-      <c r="G35" s="192"/>
-      <c r="H35" s="192"/>
-      <c r="I35" s="192"/>
-      <c r="J35" s="192"/>
+      <c r="E35" s="220"/>
+      <c r="F35" s="220"/>
+      <c r="G35" s="220"/>
+      <c r="H35" s="220"/>
+      <c r="I35" s="220"/>
+      <c r="J35" s="220"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="192"/>
-      <c r="F36" s="192"/>
-      <c r="G36" s="192"/>
-      <c r="H36" s="192"/>
-      <c r="I36" s="192"/>
-      <c r="J36" s="192"/>
+      <c r="E36" s="220"/>
+      <c r="F36" s="220"/>
+      <c r="G36" s="220"/>
+      <c r="H36" s="220"/>
+      <c r="I36" s="220"/>
+      <c r="J36" s="220"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="192"/>
-      <c r="F37" s="192"/>
-      <c r="G37" s="192"/>
-      <c r="H37" s="192"/>
-      <c r="I37" s="192"/>
-      <c r="J37" s="192"/>
+      <c r="E37" s="220"/>
+      <c r="F37" s="220"/>
+      <c r="G37" s="220"/>
+      <c r="H37" s="220"/>
+      <c r="I37" s="220"/>
+      <c r="J37" s="220"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="192"/>
-      <c r="F38" s="192"/>
-      <c r="G38" s="192"/>
-      <c r="H38" s="192"/>
-      <c r="I38" s="192"/>
-      <c r="J38" s="192"/>
+      <c r="E38" s="220"/>
+      <c r="F38" s="220"/>
+      <c r="G38" s="220"/>
+      <c r="H38" s="220"/>
+      <c r="I38" s="220"/>
+      <c r="J38" s="220"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="192"/>
-      <c r="F39" s="192"/>
-      <c r="G39" s="192"/>
-      <c r="H39" s="192"/>
-      <c r="I39" s="192"/>
-      <c r="J39" s="192"/>
+      <c r="E39" s="220"/>
+      <c r="F39" s="220"/>
+      <c r="G39" s="220"/>
+      <c r="H39" s="220"/>
+      <c r="I39" s="220"/>
+      <c r="J39" s="220"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="192"/>
-      <c r="F40" s="192"/>
-      <c r="G40" s="192"/>
-      <c r="H40" s="192"/>
-      <c r="I40" s="192"/>
-      <c r="J40" s="192"/>
+      <c r="E40" s="220"/>
+      <c r="F40" s="220"/>
+      <c r="G40" s="220"/>
+      <c r="H40" s="220"/>
+      <c r="I40" s="220"/>
+      <c r="J40" s="220"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="192"/>
-      <c r="F41" s="192"/>
-      <c r="G41" s="192"/>
-      <c r="H41" s="192"/>
-      <c r="I41" s="192"/>
-      <c r="J41" s="192"/>
+      <c r="E41" s="220"/>
+      <c r="F41" s="220"/>
+      <c r="G41" s="220"/>
+      <c r="H41" s="220"/>
+      <c r="I41" s="220"/>
+      <c r="J41" s="220"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="192"/>
-      <c r="F42" s="192"/>
-      <c r="G42" s="192"/>
-      <c r="H42" s="192"/>
-      <c r="I42" s="192"/>
-      <c r="J42" s="192"/>
+      <c r="E42" s="220"/>
+      <c r="F42" s="220"/>
+      <c r="G42" s="220"/>
+      <c r="H42" s="220"/>
+      <c r="I42" s="220"/>
+      <c r="J42" s="220"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="A5:H8"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
     <mergeCell ref="E39:J39"/>
     <mergeCell ref="E40:J40"/>
     <mergeCell ref="E41:J41"/>
@@ -5999,26 +6020,6 @@
     <mergeCell ref="E37:J37"/>
     <mergeCell ref="E38:J38"/>
     <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="A5:H8"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E20:J20"/>
-    <mergeCell ref="E21:J21"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E25:J25"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2">
@@ -6036,8 +6037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N226"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="G1" activePane="topRight" state="frozen"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -6060,10 +6061,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="214" t="s">
+      <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="238"/>
+      <c r="B1" s="253"/>
       <c r="C1" s="128" t="s">
         <v>1</v>
       </c>
@@ -6088,18 +6089,18 @@
       <c r="I1" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="239" t="str">
+      <c r="J1" s="254" t="str">
         <f>'Update History'!J1</f>
         <v>Thị Phượng</v>
       </c>
-      <c r="K1" s="240"/>
+      <c r="K1" s="255"/>
       <c r="L1" s="17"/>
       <c r="M1" s="17"/>
       <c r="N1" s="17"/>
     </row>
     <row r="2" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="214"/>
-      <c r="B2" s="238"/>
+      <c r="A2" s="210"/>
+      <c r="B2" s="253"/>
       <c r="C2" s="128" t="s">
         <v>7</v>
       </c>
@@ -6124,11 +6125,11 @@
       <c r="I2" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="241">
+      <c r="J2" s="256">
         <f>'Update History'!J2</f>
         <v>42381</v>
       </c>
-      <c r="K2" s="242"/>
+      <c r="K2" s="257"/>
       <c r="L2" s="17"/>
       <c r="M2" s="17"/>
       <c r="N2" s="17"/>
@@ -7828,8 +7829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:J6"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7847,10 +7848,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="214" t="s">
+      <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="214"/>
+      <c r="B1" s="210"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -7881,8 +7882,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="214"/>
-      <c r="B2" s="214"/>
+      <c r="A2" s="210"/>
+      <c r="B2" s="210"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -7946,55 +7947,55 @@
       <c r="G4" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="246" t="s">
+      <c r="H4" s="261" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="246"/>
-      <c r="J4" s="246"/>
+      <c r="I4" s="261"/>
+      <c r="J4" s="261"/>
     </row>
     <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
       <c r="B5" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="C5" s="198" t="s">
         <v>250</v>
       </c>
-      <c r="C5" s="277" t="s">
+      <c r="D5" s="199"/>
+      <c r="E5" s="195"/>
+      <c r="F5" s="194" t="s">
         <v>251</v>
       </c>
-      <c r="D5" s="278"/>
-      <c r="E5" s="271"/>
-      <c r="F5" s="270" t="s">
+      <c r="G5" s="194" t="s">
         <v>252</v>
       </c>
-      <c r="G5" s="270" t="s">
+      <c r="H5" s="262" t="s">
+        <v>254</v>
+      </c>
+      <c r="I5" s="263"/>
+      <c r="J5" s="264"/>
+    </row>
+    <row r="6" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="200"/>
+      <c r="B6" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="C6" s="201" t="s">
+        <v>250</v>
+      </c>
+      <c r="D6" s="202"/>
+      <c r="E6" s="203"/>
+      <c r="F6" s="204" t="s">
+        <v>251</v>
+      </c>
+      <c r="G6" s="204" t="s">
+        <v>252</v>
+      </c>
+      <c r="H6" s="262" t="s">
         <v>253</v>
       </c>
-      <c r="H5" s="272" t="s">
-        <v>255</v>
-      </c>
-      <c r="I5" s="273"/>
-      <c r="J5" s="274"/>
-    </row>
-    <row r="6" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="279"/>
-      <c r="B6" s="21" t="s">
-        <v>250</v>
-      </c>
-      <c r="C6" s="280" t="s">
-        <v>251</v>
-      </c>
-      <c r="D6" s="281"/>
-      <c r="E6" s="282"/>
-      <c r="F6" s="283" t="s">
-        <v>252</v>
-      </c>
-      <c r="G6" s="283" t="s">
-        <v>253</v>
-      </c>
-      <c r="H6" s="272" t="s">
-        <v>254</v>
-      </c>
-      <c r="I6" s="273"/>
-      <c r="J6" s="274"/>
+      <c r="I6" s="263"/>
+      <c r="J6" s="264"/>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="56"/>
@@ -8004,9 +8005,9 @@
       <c r="E7" s="51"/>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
-      <c r="H7" s="243"/>
-      <c r="I7" s="244"/>
-      <c r="J7" s="245"/>
+      <c r="H7" s="258"/>
+      <c r="I7" s="259"/>
+      <c r="J7" s="260"/>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
@@ -8016,9 +8017,9 @@
       <c r="E8" s="50"/>
       <c r="F8" s="50"/>
       <c r="G8" s="50"/>
-      <c r="H8" s="243"/>
-      <c r="I8" s="244"/>
-      <c r="J8" s="245"/>
+      <c r="H8" s="258"/>
+      <c r="I8" s="259"/>
+      <c r="J8" s="260"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
@@ -8028,9 +8029,9 @@
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
-      <c r="H9" s="243"/>
-      <c r="I9" s="244"/>
-      <c r="J9" s="245"/>
+      <c r="H9" s="258"/>
+      <c r="I9" s="259"/>
+      <c r="J9" s="260"/>
     </row>
     <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="56"/>
@@ -8040,9 +8041,9 @@
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
-      <c r="H10" s="243"/>
-      <c r="I10" s="244"/>
-      <c r="J10" s="245"/>
+      <c r="H10" s="258"/>
+      <c r="I10" s="259"/>
+      <c r="J10" s="260"/>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="56"/>
@@ -8052,9 +8053,9 @@
       <c r="E11" s="51"/>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
-      <c r="H11" s="243"/>
-      <c r="I11" s="244"/>
-      <c r="J11" s="245"/>
+      <c r="H11" s="258"/>
+      <c r="I11" s="259"/>
+      <c r="J11" s="260"/>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="56"/>
@@ -8064,9 +8065,9 @@
       <c r="E12" s="51"/>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
-      <c r="H12" s="243"/>
-      <c r="I12" s="244"/>
-      <c r="J12" s="245"/>
+      <c r="H12" s="258"/>
+      <c r="I12" s="259"/>
+      <c r="J12" s="260"/>
     </row>
     <row r="13" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="56"/>
@@ -8076,9 +8077,9 @@
       <c r="E13" s="55"/>
       <c r="F13" s="55"/>
       <c r="G13" s="55"/>
-      <c r="H13" s="243"/>
-      <c r="I13" s="244"/>
-      <c r="J13" s="245"/>
+      <c r="H13" s="258"/>
+      <c r="I13" s="259"/>
+      <c r="J13" s="260"/>
     </row>
     <row r="14" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="56"/>
@@ -8088,348 +8089,372 @@
       <c r="E14" s="55"/>
       <c r="F14" s="55"/>
       <c r="G14" s="55"/>
-      <c r="H14" s="243"/>
-      <c r="I14" s="244"/>
-      <c r="J14" s="245"/>
+      <c r="H14" s="258"/>
+      <c r="I14" s="259"/>
+      <c r="J14" s="260"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="192"/>
-      <c r="F15" s="192"/>
-      <c r="G15" s="192"/>
-      <c r="H15" s="192"/>
-      <c r="I15" s="192"/>
-      <c r="J15" s="192"/>
+      <c r="E15" s="220"/>
+      <c r="F15" s="220"/>
+      <c r="G15" s="220"/>
+      <c r="H15" s="220"/>
+      <c r="I15" s="220"/>
+      <c r="J15" s="220"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="192"/>
-      <c r="F16" s="192"/>
-      <c r="G16" s="192"/>
-      <c r="H16" s="192"/>
-      <c r="I16" s="192"/>
-      <c r="J16" s="192"/>
+      <c r="E16" s="220"/>
+      <c r="F16" s="220"/>
+      <c r="G16" s="220"/>
+      <c r="H16" s="220"/>
+      <c r="I16" s="220"/>
+      <c r="J16" s="220"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="192"/>
-      <c r="F17" s="192"/>
-      <c r="G17" s="192"/>
-      <c r="H17" s="192"/>
-      <c r="I17" s="192"/>
-      <c r="J17" s="192"/>
+      <c r="E17" s="220"/>
+      <c r="F17" s="220"/>
+      <c r="G17" s="220"/>
+      <c r="H17" s="220"/>
+      <c r="I17" s="220"/>
+      <c r="J17" s="220"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="192"/>
-      <c r="F18" s="192"/>
-      <c r="G18" s="192"/>
-      <c r="H18" s="192"/>
-      <c r="I18" s="192"/>
-      <c r="J18" s="192"/>
+      <c r="E18" s="220"/>
+      <c r="F18" s="220"/>
+      <c r="G18" s="220"/>
+      <c r="H18" s="220"/>
+      <c r="I18" s="220"/>
+      <c r="J18" s="220"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="192"/>
-      <c r="F19" s="192"/>
-      <c r="G19" s="192"/>
-      <c r="H19" s="192"/>
-      <c r="I19" s="192"/>
-      <c r="J19" s="192"/>
+      <c r="E19" s="220"/>
+      <c r="F19" s="220"/>
+      <c r="G19" s="220"/>
+      <c r="H19" s="220"/>
+      <c r="I19" s="220"/>
+      <c r="J19" s="220"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="192"/>
-      <c r="F20" s="192"/>
-      <c r="G20" s="192"/>
-      <c r="H20" s="192"/>
-      <c r="I20" s="192"/>
-      <c r="J20" s="192"/>
+      <c r="E20" s="220"/>
+      <c r="F20" s="220"/>
+      <c r="G20" s="220"/>
+      <c r="H20" s="220"/>
+      <c r="I20" s="220"/>
+      <c r="J20" s="220"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="192"/>
-      <c r="F21" s="192"/>
-      <c r="G21" s="192"/>
-      <c r="H21" s="192"/>
-      <c r="I21" s="192"/>
-      <c r="J21" s="192"/>
+      <c r="E21" s="220"/>
+      <c r="F21" s="220"/>
+      <c r="G21" s="220"/>
+      <c r="H21" s="220"/>
+      <c r="I21" s="220"/>
+      <c r="J21" s="220"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="192"/>
-      <c r="F22" s="192"/>
-      <c r="G22" s="192"/>
-      <c r="H22" s="192"/>
-      <c r="I22" s="192"/>
-      <c r="J22" s="192"/>
+      <c r="E22" s="220"/>
+      <c r="F22" s="220"/>
+      <c r="G22" s="220"/>
+      <c r="H22" s="220"/>
+      <c r="I22" s="220"/>
+      <c r="J22" s="220"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="192"/>
-      <c r="F23" s="192"/>
-      <c r="G23" s="192"/>
-      <c r="H23" s="192"/>
-      <c r="I23" s="192"/>
-      <c r="J23" s="192"/>
+      <c r="E23" s="220"/>
+      <c r="F23" s="220"/>
+      <c r="G23" s="220"/>
+      <c r="H23" s="220"/>
+      <c r="I23" s="220"/>
+      <c r="J23" s="220"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="192"/>
-      <c r="F24" s="192"/>
-      <c r="G24" s="192"/>
-      <c r="H24" s="192"/>
-      <c r="I24" s="192"/>
-      <c r="J24" s="192"/>
+      <c r="E24" s="220"/>
+      <c r="F24" s="220"/>
+      <c r="G24" s="220"/>
+      <c r="H24" s="220"/>
+      <c r="I24" s="220"/>
+      <c r="J24" s="220"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="192"/>
-      <c r="F25" s="192"/>
-      <c r="G25" s="192"/>
-      <c r="H25" s="192"/>
-      <c r="I25" s="192"/>
-      <c r="J25" s="192"/>
+      <c r="E25" s="220"/>
+      <c r="F25" s="220"/>
+      <c r="G25" s="220"/>
+      <c r="H25" s="220"/>
+      <c r="I25" s="220"/>
+      <c r="J25" s="220"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="192"/>
-      <c r="F26" s="192"/>
-      <c r="G26" s="192"/>
-      <c r="H26" s="192"/>
-      <c r="I26" s="192"/>
-      <c r="J26" s="192"/>
+      <c r="E26" s="220"/>
+      <c r="F26" s="220"/>
+      <c r="G26" s="220"/>
+      <c r="H26" s="220"/>
+      <c r="I26" s="220"/>
+      <c r="J26" s="220"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="192"/>
-      <c r="F27" s="192"/>
-      <c r="G27" s="192"/>
-      <c r="H27" s="192"/>
-      <c r="I27" s="192"/>
-      <c r="J27" s="192"/>
+      <c r="E27" s="220"/>
+      <c r="F27" s="220"/>
+      <c r="G27" s="220"/>
+      <c r="H27" s="220"/>
+      <c r="I27" s="220"/>
+      <c r="J27" s="220"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="192"/>
-      <c r="F28" s="192"/>
-      <c r="G28" s="192"/>
-      <c r="H28" s="192"/>
-      <c r="I28" s="192"/>
-      <c r="J28" s="192"/>
+      <c r="E28" s="220"/>
+      <c r="F28" s="220"/>
+      <c r="G28" s="220"/>
+      <c r="H28" s="220"/>
+      <c r="I28" s="220"/>
+      <c r="J28" s="220"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="192"/>
-      <c r="F29" s="192"/>
-      <c r="G29" s="192"/>
-      <c r="H29" s="192"/>
-      <c r="I29" s="192"/>
-      <c r="J29" s="192"/>
+      <c r="E29" s="220"/>
+      <c r="F29" s="220"/>
+      <c r="G29" s="220"/>
+      <c r="H29" s="220"/>
+      <c r="I29" s="220"/>
+      <c r="J29" s="220"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="192"/>
-      <c r="F30" s="192"/>
-      <c r="G30" s="192"/>
-      <c r="H30" s="192"/>
-      <c r="I30" s="192"/>
-      <c r="J30" s="192"/>
+      <c r="E30" s="220"/>
+      <c r="F30" s="220"/>
+      <c r="G30" s="220"/>
+      <c r="H30" s="220"/>
+      <c r="I30" s="220"/>
+      <c r="J30" s="220"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="192"/>
-      <c r="F31" s="192"/>
-      <c r="G31" s="192"/>
-      <c r="H31" s="192"/>
-      <c r="I31" s="192"/>
-      <c r="J31" s="192"/>
+      <c r="E31" s="220"/>
+      <c r="F31" s="220"/>
+      <c r="G31" s="220"/>
+      <c r="H31" s="220"/>
+      <c r="I31" s="220"/>
+      <c r="J31" s="220"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="192"/>
-      <c r="F32" s="192"/>
-      <c r="G32" s="192"/>
-      <c r="H32" s="192"/>
-      <c r="I32" s="192"/>
-      <c r="J32" s="192"/>
+      <c r="E32" s="220"/>
+      <c r="F32" s="220"/>
+      <c r="G32" s="220"/>
+      <c r="H32" s="220"/>
+      <c r="I32" s="220"/>
+      <c r="J32" s="220"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="192"/>
-      <c r="F33" s="192"/>
-      <c r="G33" s="192"/>
-      <c r="H33" s="192"/>
-      <c r="I33" s="192"/>
-      <c r="J33" s="192"/>
+      <c r="E33" s="220"/>
+      <c r="F33" s="220"/>
+      <c r="G33" s="220"/>
+      <c r="H33" s="220"/>
+      <c r="I33" s="220"/>
+      <c r="J33" s="220"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="192"/>
-      <c r="F34" s="192"/>
-      <c r="G34" s="192"/>
-      <c r="H34" s="192"/>
-      <c r="I34" s="192"/>
-      <c r="J34" s="192"/>
+      <c r="E34" s="220"/>
+      <c r="F34" s="220"/>
+      <c r="G34" s="220"/>
+      <c r="H34" s="220"/>
+      <c r="I34" s="220"/>
+      <c r="J34" s="220"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="192"/>
-      <c r="F35" s="192"/>
-      <c r="G35" s="192"/>
-      <c r="H35" s="192"/>
-      <c r="I35" s="192"/>
-      <c r="J35" s="192"/>
+      <c r="E35" s="220"/>
+      <c r="F35" s="220"/>
+      <c r="G35" s="220"/>
+      <c r="H35" s="220"/>
+      <c r="I35" s="220"/>
+      <c r="J35" s="220"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="192"/>
-      <c r="F36" s="192"/>
-      <c r="G36" s="192"/>
-      <c r="H36" s="192"/>
-      <c r="I36" s="192"/>
-      <c r="J36" s="192"/>
+      <c r="E36" s="220"/>
+      <c r="F36" s="220"/>
+      <c r="G36" s="220"/>
+      <c r="H36" s="220"/>
+      <c r="I36" s="220"/>
+      <c r="J36" s="220"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="192"/>
-      <c r="F37" s="192"/>
-      <c r="G37" s="192"/>
-      <c r="H37" s="192"/>
-      <c r="I37" s="192"/>
-      <c r="J37" s="192"/>
+      <c r="E37" s="220"/>
+      <c r="F37" s="220"/>
+      <c r="G37" s="220"/>
+      <c r="H37" s="220"/>
+      <c r="I37" s="220"/>
+      <c r="J37" s="220"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="192"/>
-      <c r="F38" s="192"/>
-      <c r="G38" s="192"/>
-      <c r="H38" s="192"/>
-      <c r="I38" s="192"/>
-      <c r="J38" s="192"/>
+      <c r="E38" s="220"/>
+      <c r="F38" s="220"/>
+      <c r="G38" s="220"/>
+      <c r="H38" s="220"/>
+      <c r="I38" s="220"/>
+      <c r="J38" s="220"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="192"/>
-      <c r="F39" s="192"/>
-      <c r="G39" s="192"/>
-      <c r="H39" s="192"/>
-      <c r="I39" s="192"/>
-      <c r="J39" s="192"/>
+      <c r="E39" s="220"/>
+      <c r="F39" s="220"/>
+      <c r="G39" s="220"/>
+      <c r="H39" s="220"/>
+      <c r="I39" s="220"/>
+      <c r="J39" s="220"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="192"/>
-      <c r="F40" s="192"/>
-      <c r="G40" s="192"/>
-      <c r="H40" s="192"/>
-      <c r="I40" s="192"/>
-      <c r="J40" s="192"/>
+      <c r="E40" s="220"/>
+      <c r="F40" s="220"/>
+      <c r="G40" s="220"/>
+      <c r="H40" s="220"/>
+      <c r="I40" s="220"/>
+      <c r="J40" s="220"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="192"/>
-      <c r="F41" s="192"/>
-      <c r="G41" s="192"/>
-      <c r="H41" s="192"/>
-      <c r="I41" s="192"/>
-      <c r="J41" s="192"/>
+      <c r="E41" s="220"/>
+      <c r="F41" s="220"/>
+      <c r="G41" s="220"/>
+      <c r="H41" s="220"/>
+      <c r="I41" s="220"/>
+      <c r="J41" s="220"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="192"/>
-      <c r="F42" s="192"/>
-      <c r="G42" s="192"/>
-      <c r="H42" s="192"/>
-      <c r="I42" s="192"/>
-      <c r="J42" s="192"/>
+      <c r="E42" s="220"/>
+      <c r="F42" s="220"/>
+      <c r="G42" s="220"/>
+      <c r="H42" s="220"/>
+      <c r="I42" s="220"/>
+      <c r="J42" s="220"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="E39:J39"/>
     <mergeCell ref="E40:J40"/>
@@ -8446,30 +8471,6 @@
     <mergeCell ref="E20:J20"/>
     <mergeCell ref="E21:J21"/>
     <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H8:J8"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2">
@@ -8505,10 +8506,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="214" t="s">
+      <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="214"/>
+      <c r="B1" s="210"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -8539,8 +8540,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="214"/>
-      <c r="B2" s="214"/>
+      <c r="A2" s="210"/>
+      <c r="B2" s="210"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -8571,16 +8572,16 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="251"/>
-      <c r="B3" s="252"/>
-      <c r="C3" s="252"/>
-      <c r="D3" s="252"/>
-      <c r="E3" s="252"/>
-      <c r="F3" s="252"/>
-      <c r="G3" s="252"/>
-      <c r="H3" s="252"/>
-      <c r="I3" s="252"/>
-      <c r="J3" s="253"/>
+      <c r="A3" s="269"/>
+      <c r="B3" s="270"/>
+      <c r="C3" s="270"/>
+      <c r="D3" s="270"/>
+      <c r="E3" s="270"/>
+      <c r="F3" s="270"/>
+      <c r="G3" s="270"/>
+      <c r="H3" s="270"/>
+      <c r="I3" s="270"/>
+      <c r="J3" s="271"/>
     </row>
     <row r="4" spans="1:10" s="45" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="66" t="s">
@@ -8595,16 +8596,16 @@
       <c r="D4" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="247" t="s">
+      <c r="E4" s="265" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="247"/>
-      <c r="G4" s="248" t="s">
+      <c r="F4" s="265"/>
+      <c r="G4" s="266" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="249"/>
-      <c r="I4" s="249"/>
-      <c r="J4" s="250"/>
+      <c r="H4" s="267"/>
+      <c r="I4" s="267"/>
+      <c r="J4" s="268"/>
     </row>
     <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
@@ -8731,339 +8732,359 @@
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="192"/>
-      <c r="F15" s="192"/>
-      <c r="G15" s="192"/>
-      <c r="H15" s="192"/>
-      <c r="I15" s="192"/>
-      <c r="J15" s="192"/>
+      <c r="E15" s="220"/>
+      <c r="F15" s="220"/>
+      <c r="G15" s="220"/>
+      <c r="H15" s="220"/>
+      <c r="I15" s="220"/>
+      <c r="J15" s="220"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="192"/>
-      <c r="F16" s="192"/>
-      <c r="G16" s="192"/>
-      <c r="H16" s="192"/>
-      <c r="I16" s="192"/>
-      <c r="J16" s="192"/>
+      <c r="E16" s="220"/>
+      <c r="F16" s="220"/>
+      <c r="G16" s="220"/>
+      <c r="H16" s="220"/>
+      <c r="I16" s="220"/>
+      <c r="J16" s="220"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="192"/>
-      <c r="F17" s="192"/>
-      <c r="G17" s="192"/>
-      <c r="H17" s="192"/>
-      <c r="I17" s="192"/>
-      <c r="J17" s="192"/>
+      <c r="E17" s="220"/>
+      <c r="F17" s="220"/>
+      <c r="G17" s="220"/>
+      <c r="H17" s="220"/>
+      <c r="I17" s="220"/>
+      <c r="J17" s="220"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="192"/>
-      <c r="F18" s="192"/>
-      <c r="G18" s="192"/>
-      <c r="H18" s="192"/>
-      <c r="I18" s="192"/>
-      <c r="J18" s="192"/>
+      <c r="E18" s="220"/>
+      <c r="F18" s="220"/>
+      <c r="G18" s="220"/>
+      <c r="H18" s="220"/>
+      <c r="I18" s="220"/>
+      <c r="J18" s="220"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="192"/>
-      <c r="F19" s="192"/>
-      <c r="G19" s="192"/>
-      <c r="H19" s="192"/>
-      <c r="I19" s="192"/>
-      <c r="J19" s="192"/>
+      <c r="E19" s="220"/>
+      <c r="F19" s="220"/>
+      <c r="G19" s="220"/>
+      <c r="H19" s="220"/>
+      <c r="I19" s="220"/>
+      <c r="J19" s="220"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="192"/>
-      <c r="F20" s="192"/>
-      <c r="G20" s="192"/>
-      <c r="H20" s="192"/>
-      <c r="I20" s="192"/>
-      <c r="J20" s="192"/>
+      <c r="E20" s="220"/>
+      <c r="F20" s="220"/>
+      <c r="G20" s="220"/>
+      <c r="H20" s="220"/>
+      <c r="I20" s="220"/>
+      <c r="J20" s="220"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="192"/>
-      <c r="F21" s="192"/>
-      <c r="G21" s="192"/>
-      <c r="H21" s="192"/>
-      <c r="I21" s="192"/>
-      <c r="J21" s="192"/>
+      <c r="E21" s="220"/>
+      <c r="F21" s="220"/>
+      <c r="G21" s="220"/>
+      <c r="H21" s="220"/>
+      <c r="I21" s="220"/>
+      <c r="J21" s="220"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="192"/>
-      <c r="F22" s="192"/>
-      <c r="G22" s="192"/>
-      <c r="H22" s="192"/>
-      <c r="I22" s="192"/>
-      <c r="J22" s="192"/>
+      <c r="E22" s="220"/>
+      <c r="F22" s="220"/>
+      <c r="G22" s="220"/>
+      <c r="H22" s="220"/>
+      <c r="I22" s="220"/>
+      <c r="J22" s="220"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="192"/>
-      <c r="F23" s="192"/>
-      <c r="G23" s="192"/>
-      <c r="H23" s="192"/>
-      <c r="I23" s="192"/>
-      <c r="J23" s="192"/>
+      <c r="E23" s="220"/>
+      <c r="F23" s="220"/>
+      <c r="G23" s="220"/>
+      <c r="H23" s="220"/>
+      <c r="I23" s="220"/>
+      <c r="J23" s="220"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="192"/>
-      <c r="F24" s="192"/>
-      <c r="G24" s="192"/>
-      <c r="H24" s="192"/>
-      <c r="I24" s="192"/>
-      <c r="J24" s="192"/>
+      <c r="E24" s="220"/>
+      <c r="F24" s="220"/>
+      <c r="G24" s="220"/>
+      <c r="H24" s="220"/>
+      <c r="I24" s="220"/>
+      <c r="J24" s="220"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="192"/>
-      <c r="F25" s="192"/>
-      <c r="G25" s="192"/>
-      <c r="H25" s="192"/>
-      <c r="I25" s="192"/>
-      <c r="J25" s="192"/>
+      <c r="E25" s="220"/>
+      <c r="F25" s="220"/>
+      <c r="G25" s="220"/>
+      <c r="H25" s="220"/>
+      <c r="I25" s="220"/>
+      <c r="J25" s="220"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="192"/>
-      <c r="F26" s="192"/>
-      <c r="G26" s="192"/>
-      <c r="H26" s="192"/>
-      <c r="I26" s="192"/>
-      <c r="J26" s="192"/>
+      <c r="E26" s="220"/>
+      <c r="F26" s="220"/>
+      <c r="G26" s="220"/>
+      <c r="H26" s="220"/>
+      <c r="I26" s="220"/>
+      <c r="J26" s="220"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="192"/>
-      <c r="F27" s="192"/>
-      <c r="G27" s="192"/>
-      <c r="H27" s="192"/>
-      <c r="I27" s="192"/>
-      <c r="J27" s="192"/>
+      <c r="E27" s="220"/>
+      <c r="F27" s="220"/>
+      <c r="G27" s="220"/>
+      <c r="H27" s="220"/>
+      <c r="I27" s="220"/>
+      <c r="J27" s="220"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="192"/>
-      <c r="F28" s="192"/>
-      <c r="G28" s="192"/>
-      <c r="H28" s="192"/>
-      <c r="I28" s="192"/>
-      <c r="J28" s="192"/>
+      <c r="E28" s="220"/>
+      <c r="F28" s="220"/>
+      <c r="G28" s="220"/>
+      <c r="H28" s="220"/>
+      <c r="I28" s="220"/>
+      <c r="J28" s="220"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="192"/>
-      <c r="F29" s="192"/>
-      <c r="G29" s="192"/>
-      <c r="H29" s="192"/>
-      <c r="I29" s="192"/>
-      <c r="J29" s="192"/>
+      <c r="E29" s="220"/>
+      <c r="F29" s="220"/>
+      <c r="G29" s="220"/>
+      <c r="H29" s="220"/>
+      <c r="I29" s="220"/>
+      <c r="J29" s="220"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="192"/>
-      <c r="F30" s="192"/>
-      <c r="G30" s="192"/>
-      <c r="H30" s="192"/>
-      <c r="I30" s="192"/>
-      <c r="J30" s="192"/>
+      <c r="E30" s="220"/>
+      <c r="F30" s="220"/>
+      <c r="G30" s="220"/>
+      <c r="H30" s="220"/>
+      <c r="I30" s="220"/>
+      <c r="J30" s="220"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="192"/>
-      <c r="F31" s="192"/>
-      <c r="G31" s="192"/>
-      <c r="H31" s="192"/>
-      <c r="I31" s="192"/>
-      <c r="J31" s="192"/>
+      <c r="E31" s="220"/>
+      <c r="F31" s="220"/>
+      <c r="G31" s="220"/>
+      <c r="H31" s="220"/>
+      <c r="I31" s="220"/>
+      <c r="J31" s="220"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="192"/>
-      <c r="F32" s="192"/>
-      <c r="G32" s="192"/>
-      <c r="H32" s="192"/>
-      <c r="I32" s="192"/>
-      <c r="J32" s="192"/>
+      <c r="E32" s="220"/>
+      <c r="F32" s="220"/>
+      <c r="G32" s="220"/>
+      <c r="H32" s="220"/>
+      <c r="I32" s="220"/>
+      <c r="J32" s="220"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="192"/>
-      <c r="F33" s="192"/>
-      <c r="G33" s="192"/>
-      <c r="H33" s="192"/>
-      <c r="I33" s="192"/>
-      <c r="J33" s="192"/>
+      <c r="E33" s="220"/>
+      <c r="F33" s="220"/>
+      <c r="G33" s="220"/>
+      <c r="H33" s="220"/>
+      <c r="I33" s="220"/>
+      <c r="J33" s="220"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="192"/>
-      <c r="F34" s="192"/>
-      <c r="G34" s="192"/>
-      <c r="H34" s="192"/>
-      <c r="I34" s="192"/>
-      <c r="J34" s="192"/>
+      <c r="E34" s="220"/>
+      <c r="F34" s="220"/>
+      <c r="G34" s="220"/>
+      <c r="H34" s="220"/>
+      <c r="I34" s="220"/>
+      <c r="J34" s="220"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="192"/>
-      <c r="F35" s="192"/>
-      <c r="G35" s="192"/>
-      <c r="H35" s="192"/>
-      <c r="I35" s="192"/>
-      <c r="J35" s="192"/>
+      <c r="E35" s="220"/>
+      <c r="F35" s="220"/>
+      <c r="G35" s="220"/>
+      <c r="H35" s="220"/>
+      <c r="I35" s="220"/>
+      <c r="J35" s="220"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="192"/>
-      <c r="F36" s="192"/>
-      <c r="G36" s="192"/>
-      <c r="H36" s="192"/>
-      <c r="I36" s="192"/>
-      <c r="J36" s="192"/>
+      <c r="E36" s="220"/>
+      <c r="F36" s="220"/>
+      <c r="G36" s="220"/>
+      <c r="H36" s="220"/>
+      <c r="I36" s="220"/>
+      <c r="J36" s="220"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="192"/>
-      <c r="F37" s="192"/>
-      <c r="G37" s="192"/>
-      <c r="H37" s="192"/>
-      <c r="I37" s="192"/>
-      <c r="J37" s="192"/>
+      <c r="E37" s="220"/>
+      <c r="F37" s="220"/>
+      <c r="G37" s="220"/>
+      <c r="H37" s="220"/>
+      <c r="I37" s="220"/>
+      <c r="J37" s="220"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="192"/>
-      <c r="F38" s="192"/>
-      <c r="G38" s="192"/>
-      <c r="H38" s="192"/>
-      <c r="I38" s="192"/>
-      <c r="J38" s="192"/>
+      <c r="E38" s="220"/>
+      <c r="F38" s="220"/>
+      <c r="G38" s="220"/>
+      <c r="H38" s="220"/>
+      <c r="I38" s="220"/>
+      <c r="J38" s="220"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="192"/>
-      <c r="F39" s="192"/>
-      <c r="G39" s="192"/>
-      <c r="H39" s="192"/>
-      <c r="I39" s="192"/>
-      <c r="J39" s="192"/>
+      <c r="E39" s="220"/>
+      <c r="F39" s="220"/>
+      <c r="G39" s="220"/>
+      <c r="H39" s="220"/>
+      <c r="I39" s="220"/>
+      <c r="J39" s="220"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="192"/>
-      <c r="F40" s="192"/>
-      <c r="G40" s="192"/>
-      <c r="H40" s="192"/>
-      <c r="I40" s="192"/>
-      <c r="J40" s="192"/>
+      <c r="E40" s="220"/>
+      <c r="F40" s="220"/>
+      <c r="G40" s="220"/>
+      <c r="H40" s="220"/>
+      <c r="I40" s="220"/>
+      <c r="J40" s="220"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="192"/>
-      <c r="F41" s="192"/>
-      <c r="G41" s="192"/>
-      <c r="H41" s="192"/>
-      <c r="I41" s="192"/>
-      <c r="J41" s="192"/>
+      <c r="E41" s="220"/>
+      <c r="F41" s="220"/>
+      <c r="G41" s="220"/>
+      <c r="H41" s="220"/>
+      <c r="I41" s="220"/>
+      <c r="J41" s="220"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="192"/>
-      <c r="F42" s="192"/>
-      <c r="G42" s="192"/>
-      <c r="H42" s="192"/>
-      <c r="I42" s="192"/>
-      <c r="J42" s="192"/>
+      <c r="E42" s="220"/>
+      <c r="F42" s="220"/>
+      <c r="G42" s="220"/>
+      <c r="H42" s="220"/>
+      <c r="I42" s="220"/>
+      <c r="J42" s="220"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E40:J40"/>
     <mergeCell ref="E30:J30"/>
     <mergeCell ref="E19:J19"/>
     <mergeCell ref="E20:J20"/>
@@ -9076,26 +9097,6 @@
     <mergeCell ref="E28:J28"/>
     <mergeCell ref="E29:J29"/>
     <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2">
@@ -9112,8 +9113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView view="pageBreakPreview" topLeftCell="I7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9139,10 +9140,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="214" t="s">
+      <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="214"/>
+      <c r="B1" s="210"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -9180,8 +9181,8 @@
       <c r="Q1" s="17"/>
     </row>
     <row r="2" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="214"/>
-      <c r="B2" s="214"/>
+      <c r="A2" s="210"/>
+      <c r="B2" s="210"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -9219,16 +9220,16 @@
       <c r="Q2" s="17"/>
     </row>
     <row r="3" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="251"/>
-      <c r="B3" s="252"/>
-      <c r="C3" s="252"/>
-      <c r="D3" s="252"/>
-      <c r="E3" s="252"/>
-      <c r="F3" s="252"/>
-      <c r="G3" s="252"/>
-      <c r="H3" s="252"/>
-      <c r="I3" s="252"/>
-      <c r="J3" s="253"/>
+      <c r="A3" s="269"/>
+      <c r="B3" s="270"/>
+      <c r="C3" s="270"/>
+      <c r="D3" s="270"/>
+      <c r="E3" s="270"/>
+      <c r="F3" s="270"/>
+      <c r="G3" s="270"/>
+      <c r="H3" s="270"/>
+      <c r="I3" s="270"/>
+      <c r="J3" s="271"/>
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
@@ -9262,12 +9263,12 @@
       <c r="H4" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="248" t="s">
+      <c r="I4" s="266" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="249"/>
-      <c r="K4" s="249"/>
-      <c r="L4" s="250"/>
+      <c r="J4" s="267"/>
+      <c r="K4" s="267"/>
+      <c r="L4" s="268"/>
       <c r="M4" s="66" t="s">
         <v>44</v>
       </c>
@@ -9301,12 +9302,12 @@
       <c r="H5" s="166" t="s">
         <v>231</v>
       </c>
-      <c r="I5" s="257" t="s">
+      <c r="I5" s="278" t="s">
         <v>232</v>
       </c>
-      <c r="J5" s="258"/>
-      <c r="K5" s="258"/>
-      <c r="L5" s="259"/>
+      <c r="J5" s="279"/>
+      <c r="K5" s="279"/>
+      <c r="L5" s="280"/>
       <c r="M5" s="151"/>
       <c r="N5" s="151"/>
       <c r="O5" s="151"/>
@@ -9330,12 +9331,12 @@
       <c r="H6" s="166" t="s">
         <v>175</v>
       </c>
-      <c r="I6" s="260" t="s">
+      <c r="I6" s="272" t="s">
         <v>228</v>
       </c>
-      <c r="J6" s="261"/>
-      <c r="K6" s="261"/>
-      <c r="L6" s="262"/>
+      <c r="J6" s="273"/>
+      <c r="K6" s="273"/>
+      <c r="L6" s="274"/>
       <c r="M6" s="151"/>
       <c r="N6" s="151"/>
       <c r="O6" s="151"/>
@@ -9357,55 +9358,55 @@
       <c r="H7" s="189" t="s">
         <v>238</v>
       </c>
-      <c r="I7" s="254" t="s">
+      <c r="I7" s="275" t="s">
         <v>237</v>
       </c>
-      <c r="J7" s="255"/>
-      <c r="K7" s="255"/>
-      <c r="L7" s="256"/>
+      <c r="J7" s="276"/>
+      <c r="K7" s="276"/>
+      <c r="L7" s="277"/>
       <c r="M7" s="190"/>
       <c r="N7" s="190"/>
       <c r="O7" s="190"/>
       <c r="P7" s="190"/>
       <c r="Q7" s="190"/>
     </row>
-    <row r="8" spans="1:17" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="269"/>
+    <row r="8" spans="1:17" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="193"/>
       <c r="B8" s="21"/>
       <c r="C8" s="22"/>
       <c r="D8" s="23"/>
-      <c r="E8" s="270" t="s">
+      <c r="E8" s="194" t="s">
         <v>243</v>
       </c>
-      <c r="F8" s="268" t="s">
+      <c r="F8" s="192" t="s">
         <v>172</v>
       </c>
-      <c r="G8" s="268" t="s">
+      <c r="G8" s="192" t="s">
         <v>236</v>
       </c>
-      <c r="H8" s="271" t="s">
+      <c r="H8" s="195" t="s">
         <v>242</v>
       </c>
-      <c r="I8" s="272" t="s">
+      <c r="I8" s="262" t="s">
         <v>244</v>
       </c>
-      <c r="J8" s="273"/>
-      <c r="K8" s="273"/>
-      <c r="L8" s="274"/>
-      <c r="M8" s="275" t="s">
+      <c r="J8" s="263"/>
+      <c r="K8" s="263"/>
+      <c r="L8" s="264"/>
+      <c r="M8" s="196" t="s">
         <v>245</v>
       </c>
-      <c r="N8" s="271" t="s">
+      <c r="N8" s="195" t="s">
         <v>246</v>
       </c>
-      <c r="O8" s="276" t="s">
-        <v>249</v>
-      </c>
-      <c r="P8" s="276" t="s">
+      <c r="O8" s="197" t="s">
         <v>248</v>
       </c>
-      <c r="Q8" s="270" t="s">
+      <c r="P8" s="197" t="s">
         <v>247</v>
+      </c>
+      <c r="Q8" s="194" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9417,10 +9418,10 @@
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
       <c r="H9" s="51"/>
-      <c r="I9" s="243"/>
-      <c r="J9" s="244"/>
-      <c r="K9" s="244"/>
-      <c r="L9" s="245"/>
+      <c r="I9" s="258"/>
+      <c r="J9" s="259"/>
+      <c r="K9" s="259"/>
+      <c r="L9" s="260"/>
       <c r="M9" s="60"/>
       <c r="N9" s="60"/>
       <c r="O9" s="60"/>
@@ -9436,10 +9437,10 @@
       <c r="F10" s="55"/>
       <c r="G10" s="55"/>
       <c r="H10" s="55"/>
-      <c r="I10" s="243"/>
-      <c r="J10" s="244"/>
-      <c r="K10" s="244"/>
-      <c r="L10" s="245"/>
+      <c r="I10" s="258"/>
+      <c r="J10" s="259"/>
+      <c r="K10" s="259"/>
+      <c r="L10" s="260"/>
       <c r="M10" s="60"/>
       <c r="N10" s="60"/>
       <c r="O10" s="60"/>
@@ -9455,10 +9456,10 @@
       <c r="F11" s="55"/>
       <c r="G11" s="55"/>
       <c r="H11" s="55"/>
-      <c r="I11" s="243"/>
-      <c r="J11" s="244"/>
-      <c r="K11" s="244"/>
-      <c r="L11" s="245"/>
+      <c r="I11" s="258"/>
+      <c r="J11" s="259"/>
+      <c r="K11" s="259"/>
+      <c r="L11" s="260"/>
       <c r="M11" s="60"/>
       <c r="N11" s="60"/>
       <c r="O11" s="60"/>
@@ -9470,339 +9471,361 @@
       <c r="B12" s="35"/>
       <c r="C12" s="36"/>
       <c r="D12" s="34"/>
-      <c r="E12" s="192"/>
-      <c r="F12" s="192"/>
-      <c r="G12" s="192"/>
-      <c r="H12" s="192"/>
-      <c r="I12" s="192"/>
-      <c r="J12" s="192"/>
+      <c r="E12" s="220"/>
+      <c r="F12" s="220"/>
+      <c r="G12" s="220"/>
+      <c r="H12" s="220"/>
+      <c r="I12" s="220"/>
+      <c r="J12" s="220"/>
     </row>
     <row r="13" spans="1:17" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="35"/>
       <c r="C13" s="36"/>
       <c r="D13" s="34"/>
-      <c r="E13" s="192"/>
-      <c r="F13" s="192"/>
-      <c r="G13" s="192"/>
-      <c r="H13" s="192"/>
-      <c r="I13" s="192"/>
-      <c r="J13" s="192"/>
+      <c r="E13" s="220"/>
+      <c r="F13" s="220"/>
+      <c r="G13" s="220"/>
+      <c r="H13" s="220"/>
+      <c r="I13" s="220"/>
+      <c r="J13" s="220"/>
     </row>
     <row r="14" spans="1:17" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="35"/>
       <c r="C14" s="36"/>
       <c r="D14" s="34"/>
-      <c r="E14" s="192"/>
-      <c r="F14" s="192"/>
-      <c r="G14" s="192"/>
-      <c r="H14" s="192"/>
-      <c r="I14" s="192"/>
-      <c r="J14" s="192"/>
+      <c r="E14" s="220"/>
+      <c r="F14" s="220"/>
+      <c r="G14" s="220"/>
+      <c r="H14" s="220"/>
+      <c r="I14" s="220"/>
+      <c r="J14" s="220"/>
     </row>
     <row r="15" spans="1:17" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="192"/>
-      <c r="F15" s="192"/>
-      <c r="G15" s="192"/>
-      <c r="H15" s="192"/>
-      <c r="I15" s="192"/>
-      <c r="J15" s="192"/>
+      <c r="E15" s="220"/>
+      <c r="F15" s="220"/>
+      <c r="G15" s="220"/>
+      <c r="H15" s="220"/>
+      <c r="I15" s="220"/>
+      <c r="J15" s="220"/>
     </row>
     <row r="16" spans="1:17" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="192"/>
-      <c r="F16" s="192"/>
-      <c r="G16" s="192"/>
-      <c r="H16" s="192"/>
-      <c r="I16" s="192"/>
-      <c r="J16" s="192"/>
+      <c r="E16" s="220"/>
+      <c r="F16" s="220"/>
+      <c r="G16" s="220"/>
+      <c r="H16" s="220"/>
+      <c r="I16" s="220"/>
+      <c r="J16" s="220"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="192"/>
-      <c r="F17" s="192"/>
-      <c r="G17" s="192"/>
-      <c r="H17" s="192"/>
-      <c r="I17" s="192"/>
-      <c r="J17" s="192"/>
+      <c r="E17" s="220"/>
+      <c r="F17" s="220"/>
+      <c r="G17" s="220"/>
+      <c r="H17" s="220"/>
+      <c r="I17" s="220"/>
+      <c r="J17" s="220"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="192"/>
-      <c r="F18" s="192"/>
-      <c r="G18" s="192"/>
-      <c r="H18" s="192"/>
-      <c r="I18" s="192"/>
-      <c r="J18" s="192"/>
+      <c r="E18" s="220"/>
+      <c r="F18" s="220"/>
+      <c r="G18" s="220"/>
+      <c r="H18" s="220"/>
+      <c r="I18" s="220"/>
+      <c r="J18" s="220"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="192"/>
-      <c r="F19" s="192"/>
-      <c r="G19" s="192"/>
-      <c r="H19" s="192"/>
-      <c r="I19" s="192"/>
-      <c r="J19" s="192"/>
+      <c r="E19" s="220"/>
+      <c r="F19" s="220"/>
+      <c r="G19" s="220"/>
+      <c r="H19" s="220"/>
+      <c r="I19" s="220"/>
+      <c r="J19" s="220"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="192"/>
-      <c r="F20" s="192"/>
-      <c r="G20" s="192"/>
-      <c r="H20" s="192"/>
-      <c r="I20" s="192"/>
-      <c r="J20" s="192"/>
+      <c r="E20" s="220"/>
+      <c r="F20" s="220"/>
+      <c r="G20" s="220"/>
+      <c r="H20" s="220"/>
+      <c r="I20" s="220"/>
+      <c r="J20" s="220"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="192"/>
-      <c r="F21" s="192"/>
-      <c r="G21" s="192"/>
-      <c r="H21" s="192"/>
-      <c r="I21" s="192"/>
-      <c r="J21" s="192"/>
+      <c r="E21" s="220"/>
+      <c r="F21" s="220"/>
+      <c r="G21" s="220"/>
+      <c r="H21" s="220"/>
+      <c r="I21" s="220"/>
+      <c r="J21" s="220"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="34"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="192"/>
-      <c r="F22" s="192"/>
-      <c r="G22" s="192"/>
-      <c r="H22" s="192"/>
-      <c r="I22" s="192"/>
-      <c r="J22" s="192"/>
+      <c r="E22" s="220"/>
+      <c r="F22" s="220"/>
+      <c r="G22" s="220"/>
+      <c r="H22" s="220"/>
+      <c r="I22" s="220"/>
+      <c r="J22" s="220"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="192"/>
-      <c r="F23" s="192"/>
-      <c r="G23" s="192"/>
-      <c r="H23" s="192"/>
-      <c r="I23" s="192"/>
-      <c r="J23" s="192"/>
+      <c r="E23" s="220"/>
+      <c r="F23" s="220"/>
+      <c r="G23" s="220"/>
+      <c r="H23" s="220"/>
+      <c r="I23" s="220"/>
+      <c r="J23" s="220"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="192"/>
-      <c r="F24" s="192"/>
-      <c r="G24" s="192"/>
-      <c r="H24" s="192"/>
-      <c r="I24" s="192"/>
-      <c r="J24" s="192"/>
+      <c r="E24" s="220"/>
+      <c r="F24" s="220"/>
+      <c r="G24" s="220"/>
+      <c r="H24" s="220"/>
+      <c r="I24" s="220"/>
+      <c r="J24" s="220"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="192"/>
-      <c r="F25" s="192"/>
-      <c r="G25" s="192"/>
-      <c r="H25" s="192"/>
-      <c r="I25" s="192"/>
-      <c r="J25" s="192"/>
+      <c r="E25" s="220"/>
+      <c r="F25" s="220"/>
+      <c r="G25" s="220"/>
+      <c r="H25" s="220"/>
+      <c r="I25" s="220"/>
+      <c r="J25" s="220"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="192"/>
-      <c r="F26" s="192"/>
-      <c r="G26" s="192"/>
-      <c r="H26" s="192"/>
-      <c r="I26" s="192"/>
-      <c r="J26" s="192"/>
+      <c r="E26" s="220"/>
+      <c r="F26" s="220"/>
+      <c r="G26" s="220"/>
+      <c r="H26" s="220"/>
+      <c r="I26" s="220"/>
+      <c r="J26" s="220"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="192"/>
-      <c r="F27" s="192"/>
-      <c r="G27" s="192"/>
-      <c r="H27" s="192"/>
-      <c r="I27" s="192"/>
-      <c r="J27" s="192"/>
+      <c r="E27" s="220"/>
+      <c r="F27" s="220"/>
+      <c r="G27" s="220"/>
+      <c r="H27" s="220"/>
+      <c r="I27" s="220"/>
+      <c r="J27" s="220"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="192"/>
-      <c r="F28" s="192"/>
-      <c r="G28" s="192"/>
-      <c r="H28" s="192"/>
-      <c r="I28" s="192"/>
-      <c r="J28" s="192"/>
+      <c r="E28" s="220"/>
+      <c r="F28" s="220"/>
+      <c r="G28" s="220"/>
+      <c r="H28" s="220"/>
+      <c r="I28" s="220"/>
+      <c r="J28" s="220"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="192"/>
-      <c r="F29" s="192"/>
-      <c r="G29" s="192"/>
-      <c r="H29" s="192"/>
-      <c r="I29" s="192"/>
-      <c r="J29" s="192"/>
+      <c r="E29" s="220"/>
+      <c r="F29" s="220"/>
+      <c r="G29" s="220"/>
+      <c r="H29" s="220"/>
+      <c r="I29" s="220"/>
+      <c r="J29" s="220"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="192"/>
-      <c r="F30" s="192"/>
-      <c r="G30" s="192"/>
-      <c r="H30" s="192"/>
-      <c r="I30" s="192"/>
-      <c r="J30" s="192"/>
+      <c r="E30" s="220"/>
+      <c r="F30" s="220"/>
+      <c r="G30" s="220"/>
+      <c r="H30" s="220"/>
+      <c r="I30" s="220"/>
+      <c r="J30" s="220"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="192"/>
-      <c r="F31" s="192"/>
-      <c r="G31" s="192"/>
-      <c r="H31" s="192"/>
-      <c r="I31" s="192"/>
-      <c r="J31" s="192"/>
+      <c r="E31" s="220"/>
+      <c r="F31" s="220"/>
+      <c r="G31" s="220"/>
+      <c r="H31" s="220"/>
+      <c r="I31" s="220"/>
+      <c r="J31" s="220"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="34"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="192"/>
-      <c r="F32" s="192"/>
-      <c r="G32" s="192"/>
-      <c r="H32" s="192"/>
-      <c r="I32" s="192"/>
-      <c r="J32" s="192"/>
+      <c r="E32" s="220"/>
+      <c r="F32" s="220"/>
+      <c r="G32" s="220"/>
+      <c r="H32" s="220"/>
+      <c r="I32" s="220"/>
+      <c r="J32" s="220"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="192"/>
-      <c r="F33" s="192"/>
-      <c r="G33" s="192"/>
-      <c r="H33" s="192"/>
-      <c r="I33" s="192"/>
-      <c r="J33" s="192"/>
+      <c r="E33" s="220"/>
+      <c r="F33" s="220"/>
+      <c r="G33" s="220"/>
+      <c r="H33" s="220"/>
+      <c r="I33" s="220"/>
+      <c r="J33" s="220"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="192"/>
-      <c r="F34" s="192"/>
-      <c r="G34" s="192"/>
-      <c r="H34" s="192"/>
-      <c r="I34" s="192"/>
-      <c r="J34" s="192"/>
+      <c r="E34" s="220"/>
+      <c r="F34" s="220"/>
+      <c r="G34" s="220"/>
+      <c r="H34" s="220"/>
+      <c r="I34" s="220"/>
+      <c r="J34" s="220"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="192"/>
-      <c r="F35" s="192"/>
-      <c r="G35" s="192"/>
-      <c r="H35" s="192"/>
-      <c r="I35" s="192"/>
-      <c r="J35" s="192"/>
+      <c r="E35" s="220"/>
+      <c r="F35" s="220"/>
+      <c r="G35" s="220"/>
+      <c r="H35" s="220"/>
+      <c r="I35" s="220"/>
+      <c r="J35" s="220"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="192"/>
-      <c r="F36" s="192"/>
-      <c r="G36" s="192"/>
-      <c r="H36" s="192"/>
-      <c r="I36" s="192"/>
-      <c r="J36" s="192"/>
+      <c r="E36" s="220"/>
+      <c r="F36" s="220"/>
+      <c r="G36" s="220"/>
+      <c r="H36" s="220"/>
+      <c r="I36" s="220"/>
+      <c r="J36" s="220"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="192"/>
-      <c r="F37" s="192"/>
-      <c r="G37" s="192"/>
-      <c r="H37" s="192"/>
-      <c r="I37" s="192"/>
-      <c r="J37" s="192"/>
+      <c r="E37" s="220"/>
+      <c r="F37" s="220"/>
+      <c r="G37" s="220"/>
+      <c r="H37" s="220"/>
+      <c r="I37" s="220"/>
+      <c r="J37" s="220"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="192"/>
-      <c r="F38" s="192"/>
-      <c r="G38" s="192"/>
-      <c r="H38" s="192"/>
-      <c r="I38" s="192"/>
-      <c r="J38" s="192"/>
+      <c r="E38" s="220"/>
+      <c r="F38" s="220"/>
+      <c r="G38" s="220"/>
+      <c r="H38" s="220"/>
+      <c r="I38" s="220"/>
+      <c r="J38" s="220"/>
     </row>
     <row r="39" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="192"/>
-      <c r="F39" s="192"/>
-      <c r="G39" s="192"/>
-      <c r="H39" s="192"/>
-      <c r="I39" s="192"/>
-      <c r="J39" s="192"/>
+      <c r="E39" s="220"/>
+      <c r="F39" s="220"/>
+      <c r="G39" s="220"/>
+      <c r="H39" s="220"/>
+      <c r="I39" s="220"/>
+      <c r="J39" s="220"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E14:J14"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E23:J23"/>
     <mergeCell ref="E39:J39"/>
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="I6:L6"/>
@@ -9819,28 +9842,6 @@
     <mergeCell ref="E31:J31"/>
     <mergeCell ref="E25:J25"/>
     <mergeCell ref="E38:J38"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E20:J20"/>
-    <mergeCell ref="E21:J21"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E14:J14"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="E12:J12"/>
-    <mergeCell ref="E13:J13"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
-    <mergeCell ref="I5:L5"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2">
@@ -9863,7 +9864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A18" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A18" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <selection activeCell="C24" sqref="C24:K24"/>
     </sheetView>
   </sheetViews>
@@ -9883,11 +9884,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="214" t="s">
+      <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="214"/>
-      <c r="C1" s="214"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
       <c r="D1" s="46" t="s">
         <v>1</v>
       </c>
@@ -9918,9 +9919,9 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="214"/>
-      <c r="B2" s="214"/>
-      <c r="C2" s="214"/>
+      <c r="A2" s="210"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
       <c r="D2" s="46" t="s">
         <v>7</v>
       </c>
@@ -10261,19 +10262,19 @@
       <c r="K23" s="182"/>
     </row>
     <row r="24" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="286"/>
-      <c r="B24" s="287"/>
-      <c r="C24" s="288" t="s">
-        <v>256</v>
-      </c>
-      <c r="D24" s="284"/>
-      <c r="E24" s="284"/>
-      <c r="F24" s="284"/>
-      <c r="G24" s="284"/>
-      <c r="H24" s="284"/>
-      <c r="I24" s="284"/>
-      <c r="J24" s="284"/>
-      <c r="K24" s="285"/>
+      <c r="A24" s="205"/>
+      <c r="B24" s="206"/>
+      <c r="C24" s="282" t="s">
+        <v>255</v>
+      </c>
+      <c r="D24" s="283"/>
+      <c r="E24" s="283"/>
+      <c r="F24" s="283"/>
+      <c r="G24" s="283"/>
+      <c r="H24" s="283"/>
+      <c r="I24" s="283"/>
+      <c r="J24" s="283"/>
+      <c r="K24" s="284"/>
       <c r="L24" s="17"/>
     </row>
     <row r="25" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -10358,12 +10359,12 @@
       <c r="C30" s="39"/>
       <c r="D30" s="42"/>
       <c r="E30" s="38"/>
-      <c r="F30" s="263"/>
-      <c r="G30" s="263"/>
-      <c r="H30" s="263"/>
-      <c r="I30" s="263"/>
-      <c r="J30" s="263"/>
-      <c r="K30" s="263"/>
+      <c r="F30" s="281"/>
+      <c r="G30" s="281"/>
+      <c r="H30" s="281"/>
+      <c r="I30" s="281"/>
+      <c r="J30" s="281"/>
+      <c r="K30" s="281"/>
       <c r="L30" s="17"/>
     </row>
     <row r="31" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -10372,12 +10373,12 @@
       <c r="C31" s="39"/>
       <c r="D31" s="42"/>
       <c r="E31" s="38"/>
-      <c r="F31" s="263"/>
-      <c r="G31" s="263"/>
-      <c r="H31" s="263"/>
-      <c r="I31" s="263"/>
-      <c r="J31" s="263"/>
-      <c r="K31" s="263"/>
+      <c r="F31" s="281"/>
+      <c r="G31" s="281"/>
+      <c r="H31" s="281"/>
+      <c r="I31" s="281"/>
+      <c r="J31" s="281"/>
+      <c r="K31" s="281"/>
       <c r="L31" s="17"/>
     </row>
     <row r="32" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -10386,12 +10387,12 @@
       <c r="C32" s="39"/>
       <c r="D32" s="42"/>
       <c r="E32" s="38"/>
-      <c r="F32" s="263"/>
-      <c r="G32" s="263"/>
-      <c r="H32" s="263"/>
-      <c r="I32" s="263"/>
-      <c r="J32" s="263"/>
-      <c r="K32" s="263"/>
+      <c r="F32" s="281"/>
+      <c r="G32" s="281"/>
+      <c r="H32" s="281"/>
+      <c r="I32" s="281"/>
+      <c r="J32" s="281"/>
+      <c r="K32" s="281"/>
       <c r="L32" s="17"/>
     </row>
     <row r="33" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10400,12 +10401,12 @@
       <c r="C33" s="39"/>
       <c r="D33" s="42"/>
       <c r="E33" s="38"/>
-      <c r="F33" s="263"/>
-      <c r="G33" s="263"/>
-      <c r="H33" s="263"/>
-      <c r="I33" s="263"/>
-      <c r="J33" s="263"/>
-      <c r="K33" s="263"/>
+      <c r="F33" s="281"/>
+      <c r="G33" s="281"/>
+      <c r="H33" s="281"/>
+      <c r="I33" s="281"/>
+      <c r="J33" s="281"/>
+      <c r="K33" s="281"/>
       <c r="L33" s="17"/>
     </row>
     <row r="34" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -10634,11 +10635,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="214" t="s">
+      <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="214"/>
-      <c r="C1" s="214"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
       <c r="D1" s="46" t="s">
         <v>1</v>
       </c>
@@ -10661,9 +10662,9 @@
       <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="214"/>
-      <c r="B2" s="214"/>
-      <c r="C2" s="214"/>
+      <c r="A2" s="210"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
       <c r="D2" s="46" t="s">
         <v>7</v>
       </c>
@@ -11033,12 +11034,12 @@
       <c r="C28" s="39"/>
       <c r="D28" s="42"/>
       <c r="E28" s="38"/>
-      <c r="F28" s="263"/>
-      <c r="G28" s="263"/>
-      <c r="H28" s="263"/>
-      <c r="I28" s="263"/>
-      <c r="J28" s="263"/>
-      <c r="K28" s="263"/>
+      <c r="F28" s="281"/>
+      <c r="G28" s="281"/>
+      <c r="H28" s="281"/>
+      <c r="I28" s="281"/>
+      <c r="J28" s="281"/>
+      <c r="K28" s="281"/>
       <c r="L28" s="17"/>
     </row>
     <row r="29" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -11047,12 +11048,12 @@
       <c r="C29" s="39"/>
       <c r="D29" s="42"/>
       <c r="E29" s="38"/>
-      <c r="F29" s="263"/>
-      <c r="G29" s="263"/>
-      <c r="H29" s="263"/>
-      <c r="I29" s="263"/>
-      <c r="J29" s="263"/>
-      <c r="K29" s="263"/>
+      <c r="F29" s="281"/>
+      <c r="G29" s="281"/>
+      <c r="H29" s="281"/>
+      <c r="I29" s="281"/>
+      <c r="J29" s="281"/>
+      <c r="K29" s="281"/>
       <c r="L29" s="17"/>
     </row>
     <row r="30" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -11061,12 +11062,12 @@
       <c r="C30" s="39"/>
       <c r="D30" s="42"/>
       <c r="E30" s="38"/>
-      <c r="F30" s="263"/>
-      <c r="G30" s="263"/>
-      <c r="H30" s="263"/>
-      <c r="I30" s="263"/>
-      <c r="J30" s="263"/>
-      <c r="K30" s="263"/>
+      <c r="F30" s="281"/>
+      <c r="G30" s="281"/>
+      <c r="H30" s="281"/>
+      <c r="I30" s="281"/>
+      <c r="J30" s="281"/>
+      <c r="K30" s="281"/>
       <c r="L30" s="17"/>
     </row>
     <row r="31" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11075,12 +11076,12 @@
       <c r="C31" s="39"/>
       <c r="D31" s="42"/>
       <c r="E31" s="38"/>
-      <c r="F31" s="263"/>
-      <c r="G31" s="263"/>
-      <c r="H31" s="263"/>
-      <c r="I31" s="263"/>
-      <c r="J31" s="263"/>
-      <c r="K31" s="263"/>
+      <c r="F31" s="281"/>
+      <c r="G31" s="281"/>
+      <c r="H31" s="281"/>
+      <c r="I31" s="281"/>
+      <c r="J31" s="281"/>
+      <c r="K31" s="281"/>
       <c r="L31" s="17"/>
     </row>
     <row r="32" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -11300,14 +11301,14 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="78"/>
-      <c r="E2" s="264" t="s">
+      <c r="E2" s="285" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="264"/>
-      <c r="G2" s="264"/>
-      <c r="H2" s="264"/>
-      <c r="I2" s="264"/>
-      <c r="J2" s="264"/>
+      <c r="F2" s="285"/>
+      <c r="G2" s="285"/>
+      <c r="H2" s="285"/>
+      <c r="I2" s="285"/>
+      <c r="J2" s="285"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="79"/>
@@ -11728,11 +11729,11 @@
       <c r="B28" s="78"/>
       <c r="C28" s="78"/>
       <c r="D28" s="78"/>
-      <c r="E28" s="265" t="s">
+      <c r="E28" s="286" t="s">
         <v>107</v>
       </c>
-      <c r="F28" s="266"/>
-      <c r="G28" s="267"/>
+      <c r="F28" s="287"/>
+      <c r="G28" s="288"/>
       <c r="H28" s="78"/>
       <c r="I28" s="78"/>
       <c r="J28" s="78"/>

</xml_diff>

<commit_message>
Thực hiện bổ sung theo yêu cầu của khách hàng
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/WF0008 Danh muc phieu nhap xuat vcnb.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/WF0008 Danh muc phieu nhap xuat vcnb.xlsx
@@ -1928,7 +1928,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="260">
   <si>
     <t>Detail Design</t>
   </si>
@@ -2927,11 +2927,6 @@
     <t>WFML000185</t>
   </si>
   <si>
-    <t>Click LickEdit Thực thi @SQL0004 để kiểm tra điều kiện IsWeb,
-- Nếu =1 cảnh báo message WFML000185 nếu là Phiếu VCNB, và WFML000186 nếu là Phiếu nhập or Phiếu xuất
-- Nếu =0 thực thi @SQL002 load form Detail</t>
-  </si>
-  <si>
     <t>CustomizeIndex = 51 (Hoàng Trần): kiểm tra điều kiện phiếu nhập xuất VCNB
 - Thêm câu @SQL004 trong sheet Data Input
 - Thêm WFML000185 và WFML000186 trong sheet Input Check
@@ -2939,6 +2934,25 @@
   </si>
   <si>
     <t>Thực hiện câu @SQL004 để kiểm tra điệu kiện để load màn hình Cập nhật khi thực hiện Click LinkEdit cho Cus Hoàng Trần</t>
+  </si>
+  <si>
+    <t>Click LickEdit Thực thi @SQL0004 để kiểm tra điều kiện IsWeb,
+- Nếu =1 cảnh báo message WFML000185 nếu là Phiếu VCNB, và WFML000186 nếu là Phiếu nhập or Phiếu xuất
+ + Click Ok Thực thi @SQL002 Load Form 
+    * Nếu là Phiếu nhập Load form WF0011 và chỉ Enabled các trường Description , RefNo01, RefNo02, ActualQuantity, Ana01ID, Ana02ID, Ana03ID, Ana04ID, Ana05ID, Ana06ID, Ana07ID, Ana08ID, Ana09ID, Ana10ID, PeriodID, ProductID để sửa còn lại thì disabled
+    *  Nếu là Phiếu xuất load form WF0012 và chỉ Enabled các trường RefNo01, RefNo02, Description,  RDAddress, ContactPerson, ActualQuantity, Ana01ID, Ana02ID, Ana03ID, Ana04ID, Ana05ID, Ana06ID, Ana07ID, Ana08ID, Ana09ID, Ana10ID, PeriodID, ProductID để sửa còn lại thì disabled
+    * Nếu là Phiếu VCNB load form WF0013 và disabled tất cả các trường
+ + Click No trở về From WF0008
+- Nếu =0 thực thi @SQL002 load form 
+ + Nếu là Phiếu nhập Load form WF0011
+ + Nếu là Phiếu xuất load form WF0012
+ + Nếu là Phiếu VCNB load form WF0013</t>
+  </si>
+  <si>
+    <t>CustomizeIndex = 51</t>
+  </si>
+  <si>
+    <t>AT2006</t>
   </si>
 </sst>
 </file>
@@ -3952,11 +3966,62 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3997,62 +4062,29 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4072,30 +4104,6 @@
     <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4153,6 +4161,24 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4162,24 +4188,6 @@
     <xf numFmtId="0" fontId="7" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4203,6 +4211,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4561,10 +4575,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="210" t="s">
+      <c r="A1" s="227" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="210"/>
+      <c r="B1" s="227"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -4591,8 +4605,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="210"/>
-      <c r="B2" s="210"/>
+      <c r="A2" s="227"/>
+      <c r="B2" s="227"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -4643,14 +4657,14 @@
       <c r="D4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="211" t="s">
+      <c r="E4" s="228" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="211"/>
-      <c r="G4" s="211"/>
-      <c r="H4" s="211"/>
-      <c r="I4" s="211"/>
-      <c r="J4" s="211"/>
+      <c r="F4" s="228"/>
+      <c r="G4" s="228"/>
+      <c r="H4" s="228"/>
+      <c r="I4" s="228"/>
+      <c r="J4" s="228"/>
     </row>
     <row r="5" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
@@ -4667,14 +4681,14 @@
         <f>H1</f>
         <v>Thanh Sơn</v>
       </c>
-      <c r="E5" s="212" t="s">
+      <c r="E5" s="229" t="s">
         <v>176</v>
       </c>
-      <c r="F5" s="213"/>
-      <c r="G5" s="213"/>
-      <c r="H5" s="213"/>
-      <c r="I5" s="213"/>
-      <c r="J5" s="213"/>
+      <c r="F5" s="230"/>
+      <c r="G5" s="230"/>
+      <c r="H5" s="230"/>
+      <c r="I5" s="230"/>
+      <c r="J5" s="230"/>
     </row>
     <row r="6" spans="1:10" s="111" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
@@ -4689,14 +4703,14 @@
       <c r="D6" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="214" t="s">
+      <c r="E6" s="231" t="s">
         <v>179</v>
       </c>
-      <c r="F6" s="215"/>
-      <c r="G6" s="215"/>
-      <c r="H6" s="215"/>
-      <c r="I6" s="215"/>
-      <c r="J6" s="216"/>
+      <c r="F6" s="232"/>
+      <c r="G6" s="232"/>
+      <c r="H6" s="232"/>
+      <c r="I6" s="232"/>
+      <c r="J6" s="233"/>
     </row>
     <row r="7" spans="1:10" s="111" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="112">
@@ -4711,14 +4725,14 @@
       <c r="D7" s="115" t="s">
         <v>239</v>
       </c>
-      <c r="E7" s="217" t="s">
+      <c r="E7" s="234" t="s">
         <v>240</v>
       </c>
-      <c r="F7" s="218"/>
-      <c r="G7" s="218"/>
-      <c r="H7" s="218"/>
-      <c r="I7" s="218"/>
-      <c r="J7" s="219"/>
+      <c r="F7" s="235"/>
+      <c r="G7" s="235"/>
+      <c r="H7" s="235"/>
+      <c r="I7" s="235"/>
+      <c r="J7" s="236"/>
     </row>
     <row r="8" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -4733,14 +4747,14 @@
       <c r="D8" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="E8" s="207" t="s">
-        <v>256</v>
-      </c>
-      <c r="F8" s="208"/>
-      <c r="G8" s="208"/>
-      <c r="H8" s="208"/>
-      <c r="I8" s="208"/>
-      <c r="J8" s="209"/>
+      <c r="E8" s="224" t="s">
+        <v>255</v>
+      </c>
+      <c r="F8" s="225"/>
+      <c r="G8" s="225"/>
+      <c r="H8" s="225"/>
+      <c r="I8" s="225"/>
+      <c r="J8" s="226"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -4751,12 +4765,12 @@
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="26"/>
-      <c r="E9" s="221"/>
-      <c r="F9" s="222"/>
-      <c r="G9" s="222"/>
-      <c r="H9" s="222"/>
-      <c r="I9" s="222"/>
-      <c r="J9" s="223"/>
+      <c r="E9" s="206"/>
+      <c r="F9" s="207"/>
+      <c r="G9" s="207"/>
+      <c r="H9" s="207"/>
+      <c r="I9" s="207"/>
+      <c r="J9" s="208"/>
     </row>
     <row r="10" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -4767,12 +4781,12 @@
       </c>
       <c r="C10" s="117"/>
       <c r="D10" s="118"/>
-      <c r="E10" s="224"/>
-      <c r="F10" s="225"/>
-      <c r="G10" s="225"/>
-      <c r="H10" s="225"/>
-      <c r="I10" s="225"/>
-      <c r="J10" s="226"/>
+      <c r="E10" s="209"/>
+      <c r="F10" s="210"/>
+      <c r="G10" s="210"/>
+      <c r="H10" s="210"/>
+      <c r="I10" s="210"/>
+      <c r="J10" s="211"/>
     </row>
     <row r="11" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -4783,12 +4797,12 @@
       </c>
       <c r="C11" s="120"/>
       <c r="D11" s="121"/>
-      <c r="E11" s="227"/>
-      <c r="F11" s="228"/>
-      <c r="G11" s="228"/>
-      <c r="H11" s="228"/>
-      <c r="I11" s="228"/>
-      <c r="J11" s="229"/>
+      <c r="E11" s="212"/>
+      <c r="F11" s="213"/>
+      <c r="G11" s="213"/>
+      <c r="H11" s="213"/>
+      <c r="I11" s="213"/>
+      <c r="J11" s="214"/>
     </row>
     <row r="12" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -4799,12 +4813,12 @@
       </c>
       <c r="C12" s="123"/>
       <c r="D12" s="124"/>
-      <c r="E12" s="230"/>
-      <c r="F12" s="231"/>
-      <c r="G12" s="231"/>
-      <c r="H12" s="231"/>
-      <c r="I12" s="231"/>
-      <c r="J12" s="232"/>
+      <c r="E12" s="215"/>
+      <c r="F12" s="216"/>
+      <c r="G12" s="216"/>
+      <c r="H12" s="216"/>
+      <c r="I12" s="216"/>
+      <c r="J12" s="217"/>
     </row>
     <row r="13" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -4815,12 +4829,12 @@
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="29"/>
-      <c r="E13" s="233"/>
-      <c r="F13" s="234"/>
-      <c r="G13" s="234"/>
-      <c r="H13" s="234"/>
-      <c r="I13" s="234"/>
-      <c r="J13" s="235"/>
+      <c r="E13" s="218"/>
+      <c r="F13" s="219"/>
+      <c r="G13" s="219"/>
+      <c r="H13" s="219"/>
+      <c r="I13" s="219"/>
+      <c r="J13" s="220"/>
     </row>
     <row r="14" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
@@ -4831,361 +4845,369 @@
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="33"/>
-      <c r="E14" s="236"/>
-      <c r="F14" s="237"/>
-      <c r="G14" s="237"/>
-      <c r="H14" s="237"/>
-      <c r="I14" s="237"/>
-      <c r="J14" s="238"/>
+      <c r="E14" s="221"/>
+      <c r="F14" s="222"/>
+      <c r="G14" s="222"/>
+      <c r="H14" s="222"/>
+      <c r="I14" s="222"/>
+      <c r="J14" s="223"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="220"/>
-      <c r="F15" s="220"/>
-      <c r="G15" s="220"/>
-      <c r="H15" s="220"/>
-      <c r="I15" s="220"/>
-      <c r="J15" s="220"/>
+      <c r="E15" s="205"/>
+      <c r="F15" s="205"/>
+      <c r="G15" s="205"/>
+      <c r="H15" s="205"/>
+      <c r="I15" s="205"/>
+      <c r="J15" s="205"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="220"/>
-      <c r="F16" s="220"/>
-      <c r="G16" s="220"/>
-      <c r="H16" s="220"/>
-      <c r="I16" s="220"/>
-      <c r="J16" s="220"/>
+      <c r="E16" s="205"/>
+      <c r="F16" s="205"/>
+      <c r="G16" s="205"/>
+      <c r="H16" s="205"/>
+      <c r="I16" s="205"/>
+      <c r="J16" s="205"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="220"/>
-      <c r="F17" s="220"/>
-      <c r="G17" s="220"/>
-      <c r="H17" s="220"/>
-      <c r="I17" s="220"/>
-      <c r="J17" s="220"/>
+      <c r="E17" s="205"/>
+      <c r="F17" s="205"/>
+      <c r="G17" s="205"/>
+      <c r="H17" s="205"/>
+      <c r="I17" s="205"/>
+      <c r="J17" s="205"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="220"/>
-      <c r="F18" s="220"/>
-      <c r="G18" s="220"/>
-      <c r="H18" s="220"/>
-      <c r="I18" s="220"/>
-      <c r="J18" s="220"/>
+      <c r="E18" s="205"/>
+      <c r="F18" s="205"/>
+      <c r="G18" s="205"/>
+      <c r="H18" s="205"/>
+      <c r="I18" s="205"/>
+      <c r="J18" s="205"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="220"/>
-      <c r="F19" s="220"/>
-      <c r="G19" s="220"/>
-      <c r="H19" s="220"/>
-      <c r="I19" s="220"/>
-      <c r="J19" s="220"/>
+      <c r="E19" s="205"/>
+      <c r="F19" s="205"/>
+      <c r="G19" s="205"/>
+      <c r="H19" s="205"/>
+      <c r="I19" s="205"/>
+      <c r="J19" s="205"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="220"/>
-      <c r="F20" s="220"/>
-      <c r="G20" s="220"/>
-      <c r="H20" s="220"/>
-      <c r="I20" s="220"/>
-      <c r="J20" s="220"/>
+      <c r="E20" s="205"/>
+      <c r="F20" s="205"/>
+      <c r="G20" s="205"/>
+      <c r="H20" s="205"/>
+      <c r="I20" s="205"/>
+      <c r="J20" s="205"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="220"/>
-      <c r="F21" s="220"/>
-      <c r="G21" s="220"/>
-      <c r="H21" s="220"/>
-      <c r="I21" s="220"/>
-      <c r="J21" s="220"/>
+      <c r="E21" s="205"/>
+      <c r="F21" s="205"/>
+      <c r="G21" s="205"/>
+      <c r="H21" s="205"/>
+      <c r="I21" s="205"/>
+      <c r="J21" s="205"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="220"/>
-      <c r="F22" s="220"/>
-      <c r="G22" s="220"/>
-      <c r="H22" s="220"/>
-      <c r="I22" s="220"/>
-      <c r="J22" s="220"/>
+      <c r="E22" s="205"/>
+      <c r="F22" s="205"/>
+      <c r="G22" s="205"/>
+      <c r="H22" s="205"/>
+      <c r="I22" s="205"/>
+      <c r="J22" s="205"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="220"/>
-      <c r="F23" s="220"/>
-      <c r="G23" s="220"/>
-      <c r="H23" s="220"/>
-      <c r="I23" s="220"/>
-      <c r="J23" s="220"/>
+      <c r="E23" s="205"/>
+      <c r="F23" s="205"/>
+      <c r="G23" s="205"/>
+      <c r="H23" s="205"/>
+      <c r="I23" s="205"/>
+      <c r="J23" s="205"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="220"/>
-      <c r="F24" s="220"/>
-      <c r="G24" s="220"/>
-      <c r="H24" s="220"/>
-      <c r="I24" s="220"/>
-      <c r="J24" s="220"/>
+      <c r="E24" s="205"/>
+      <c r="F24" s="205"/>
+      <c r="G24" s="205"/>
+      <c r="H24" s="205"/>
+      <c r="I24" s="205"/>
+      <c r="J24" s="205"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="220"/>
-      <c r="F25" s="220"/>
-      <c r="G25" s="220"/>
-      <c r="H25" s="220"/>
-      <c r="I25" s="220"/>
-      <c r="J25" s="220"/>
+      <c r="E25" s="205"/>
+      <c r="F25" s="205"/>
+      <c r="G25" s="205"/>
+      <c r="H25" s="205"/>
+      <c r="I25" s="205"/>
+      <c r="J25" s="205"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="220"/>
-      <c r="F26" s="220"/>
-      <c r="G26" s="220"/>
-      <c r="H26" s="220"/>
-      <c r="I26" s="220"/>
-      <c r="J26" s="220"/>
+      <c r="E26" s="205"/>
+      <c r="F26" s="205"/>
+      <c r="G26" s="205"/>
+      <c r="H26" s="205"/>
+      <c r="I26" s="205"/>
+      <c r="J26" s="205"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="220"/>
-      <c r="F27" s="220"/>
-      <c r="G27" s="220"/>
-      <c r="H27" s="220"/>
-      <c r="I27" s="220"/>
-      <c r="J27" s="220"/>
+      <c r="E27" s="205"/>
+      <c r="F27" s="205"/>
+      <c r="G27" s="205"/>
+      <c r="H27" s="205"/>
+      <c r="I27" s="205"/>
+      <c r="J27" s="205"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="220"/>
-      <c r="F28" s="220"/>
-      <c r="G28" s="220"/>
-      <c r="H28" s="220"/>
-      <c r="I28" s="220"/>
-      <c r="J28" s="220"/>
+      <c r="E28" s="205"/>
+      <c r="F28" s="205"/>
+      <c r="G28" s="205"/>
+      <c r="H28" s="205"/>
+      <c r="I28" s="205"/>
+      <c r="J28" s="205"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="220"/>
-      <c r="F29" s="220"/>
-      <c r="G29" s="220"/>
-      <c r="H29" s="220"/>
-      <c r="I29" s="220"/>
-      <c r="J29" s="220"/>
+      <c r="E29" s="205"/>
+      <c r="F29" s="205"/>
+      <c r="G29" s="205"/>
+      <c r="H29" s="205"/>
+      <c r="I29" s="205"/>
+      <c r="J29" s="205"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="220"/>
-      <c r="F30" s="220"/>
-      <c r="G30" s="220"/>
-      <c r="H30" s="220"/>
-      <c r="I30" s="220"/>
-      <c r="J30" s="220"/>
+      <c r="E30" s="205"/>
+      <c r="F30" s="205"/>
+      <c r="G30" s="205"/>
+      <c r="H30" s="205"/>
+      <c r="I30" s="205"/>
+      <c r="J30" s="205"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="220"/>
-      <c r="F31" s="220"/>
-      <c r="G31" s="220"/>
-      <c r="H31" s="220"/>
-      <c r="I31" s="220"/>
-      <c r="J31" s="220"/>
+      <c r="E31" s="205"/>
+      <c r="F31" s="205"/>
+      <c r="G31" s="205"/>
+      <c r="H31" s="205"/>
+      <c r="I31" s="205"/>
+      <c r="J31" s="205"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="220"/>
-      <c r="F32" s="220"/>
-      <c r="G32" s="220"/>
-      <c r="H32" s="220"/>
-      <c r="I32" s="220"/>
-      <c r="J32" s="220"/>
+      <c r="E32" s="205"/>
+      <c r="F32" s="205"/>
+      <c r="G32" s="205"/>
+      <c r="H32" s="205"/>
+      <c r="I32" s="205"/>
+      <c r="J32" s="205"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="220"/>
-      <c r="F33" s="220"/>
-      <c r="G33" s="220"/>
-      <c r="H33" s="220"/>
-      <c r="I33" s="220"/>
-      <c r="J33" s="220"/>
+      <c r="E33" s="205"/>
+      <c r="F33" s="205"/>
+      <c r="G33" s="205"/>
+      <c r="H33" s="205"/>
+      <c r="I33" s="205"/>
+      <c r="J33" s="205"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="220"/>
-      <c r="F34" s="220"/>
-      <c r="G34" s="220"/>
-      <c r="H34" s="220"/>
-      <c r="I34" s="220"/>
-      <c r="J34" s="220"/>
+      <c r="E34" s="205"/>
+      <c r="F34" s="205"/>
+      <c r="G34" s="205"/>
+      <c r="H34" s="205"/>
+      <c r="I34" s="205"/>
+      <c r="J34" s="205"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="220"/>
-      <c r="F35" s="220"/>
-      <c r="G35" s="220"/>
-      <c r="H35" s="220"/>
-      <c r="I35" s="220"/>
-      <c r="J35" s="220"/>
+      <c r="E35" s="205"/>
+      <c r="F35" s="205"/>
+      <c r="G35" s="205"/>
+      <c r="H35" s="205"/>
+      <c r="I35" s="205"/>
+      <c r="J35" s="205"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="220"/>
-      <c r="F36" s="220"/>
-      <c r="G36" s="220"/>
-      <c r="H36" s="220"/>
-      <c r="I36" s="220"/>
-      <c r="J36" s="220"/>
+      <c r="E36" s="205"/>
+      <c r="F36" s="205"/>
+      <c r="G36" s="205"/>
+      <c r="H36" s="205"/>
+      <c r="I36" s="205"/>
+      <c r="J36" s="205"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="220"/>
-      <c r="F37" s="220"/>
-      <c r="G37" s="220"/>
-      <c r="H37" s="220"/>
-      <c r="I37" s="220"/>
-      <c r="J37" s="220"/>
+      <c r="E37" s="205"/>
+      <c r="F37" s="205"/>
+      <c r="G37" s="205"/>
+      <c r="H37" s="205"/>
+      <c r="I37" s="205"/>
+      <c r="J37" s="205"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="220"/>
-      <c r="F38" s="220"/>
-      <c r="G38" s="220"/>
-      <c r="H38" s="220"/>
-      <c r="I38" s="220"/>
-      <c r="J38" s="220"/>
+      <c r="E38" s="205"/>
+      <c r="F38" s="205"/>
+      <c r="G38" s="205"/>
+      <c r="H38" s="205"/>
+      <c r="I38" s="205"/>
+      <c r="J38" s="205"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="220"/>
-      <c r="F39" s="220"/>
-      <c r="G39" s="220"/>
-      <c r="H39" s="220"/>
-      <c r="I39" s="220"/>
-      <c r="J39" s="220"/>
+      <c r="E39" s="205"/>
+      <c r="F39" s="205"/>
+      <c r="G39" s="205"/>
+      <c r="H39" s="205"/>
+      <c r="I39" s="205"/>
+      <c r="J39" s="205"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="220"/>
-      <c r="F40" s="220"/>
-      <c r="G40" s="220"/>
-      <c r="H40" s="220"/>
-      <c r="I40" s="220"/>
-      <c r="J40" s="220"/>
+      <c r="E40" s="205"/>
+      <c r="F40" s="205"/>
+      <c r="G40" s="205"/>
+      <c r="H40" s="205"/>
+      <c r="I40" s="205"/>
+      <c r="J40" s="205"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="220"/>
-      <c r="F41" s="220"/>
-      <c r="G41" s="220"/>
-      <c r="H41" s="220"/>
-      <c r="I41" s="220"/>
-      <c r="J41" s="220"/>
+      <c r="E41" s="205"/>
+      <c r="F41" s="205"/>
+      <c r="G41" s="205"/>
+      <c r="H41" s="205"/>
+      <c r="I41" s="205"/>
+      <c r="J41" s="205"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="220"/>
-      <c r="F42" s="220"/>
-      <c r="G42" s="220"/>
-      <c r="H42" s="220"/>
-      <c r="I42" s="220"/>
-      <c r="J42" s="220"/>
+      <c r="E42" s="205"/>
+      <c r="F42" s="205"/>
+      <c r="G42" s="205"/>
+      <c r="H42" s="205"/>
+      <c r="I42" s="205"/>
+      <c r="J42" s="205"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="E14:J14"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E19:J19"/>
     <mergeCell ref="E32:J32"/>
     <mergeCell ref="E21:J21"/>
     <mergeCell ref="E22:J22"/>
@@ -5198,24 +5220,16 @@
     <mergeCell ref="E29:J29"/>
     <mergeCell ref="E30:J30"/>
     <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E20:J20"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="E12:J12"/>
-    <mergeCell ref="E13:J13"/>
-    <mergeCell ref="E14:J14"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E38:J38"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
@@ -5425,10 +5439,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="210" t="s">
+      <c r="A1" s="227" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="210"/>
+      <c r="B1" s="227"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -5459,8 +5473,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="210"/>
-      <c r="B2" s="210"/>
+      <c r="A2" s="227"/>
+      <c r="B2" s="227"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -5503,76 +5517,76 @@
       <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="210" t="s">
+      <c r="A4" s="227" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="210"/>
-      <c r="C4" s="210"/>
-      <c r="D4" s="210"/>
-      <c r="E4" s="210"/>
-      <c r="F4" s="210"/>
-      <c r="G4" s="210"/>
-      <c r="H4" s="210"/>
-      <c r="I4" s="210" t="s">
+      <c r="B4" s="227"/>
+      <c r="C4" s="227"/>
+      <c r="D4" s="227"/>
+      <c r="E4" s="227"/>
+      <c r="F4" s="227"/>
+      <c r="G4" s="227"/>
+      <c r="H4" s="227"/>
+      <c r="I4" s="227" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="210"/>
+      <c r="J4" s="227"/>
     </row>
     <row r="5" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="247"/>
-      <c r="B5" s="248"/>
-      <c r="C5" s="248"/>
-      <c r="D5" s="248"/>
-      <c r="E5" s="248"/>
-      <c r="F5" s="248"/>
-      <c r="G5" s="248"/>
-      <c r="H5" s="249"/>
-      <c r="I5" s="239" t="s">
+      <c r="A5" s="239"/>
+      <c r="B5" s="240"/>
+      <c r="C5" s="240"/>
+      <c r="D5" s="240"/>
+      <c r="E5" s="240"/>
+      <c r="F5" s="240"/>
+      <c r="G5" s="240"/>
+      <c r="H5" s="241"/>
+      <c r="I5" s="245" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="240"/>
+      <c r="J5" s="246"/>
     </row>
     <row r="6" spans="1:10" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="250"/>
-      <c r="B6" s="251"/>
-      <c r="C6" s="251"/>
-      <c r="D6" s="251"/>
-      <c r="E6" s="251"/>
-      <c r="F6" s="251"/>
-      <c r="G6" s="251"/>
-      <c r="H6" s="252"/>
-      <c r="I6" s="241" t="s">
+      <c r="A6" s="242"/>
+      <c r="B6" s="243"/>
+      <c r="C6" s="243"/>
+      <c r="D6" s="243"/>
+      <c r="E6" s="243"/>
+      <c r="F6" s="243"/>
+      <c r="G6" s="243"/>
+      <c r="H6" s="244"/>
+      <c r="I6" s="247" t="s">
         <v>177</v>
       </c>
-      <c r="J6" s="242"/>
+      <c r="J6" s="248"/>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="250"/>
-      <c r="B7" s="251"/>
-      <c r="C7" s="251"/>
-      <c r="D7" s="251"/>
-      <c r="E7" s="251"/>
-      <c r="F7" s="251"/>
-      <c r="G7" s="251"/>
-      <c r="H7" s="252"/>
-      <c r="I7" s="243" t="s">
+      <c r="A7" s="242"/>
+      <c r="B7" s="243"/>
+      <c r="C7" s="243"/>
+      <c r="D7" s="243"/>
+      <c r="E7" s="243"/>
+      <c r="F7" s="243"/>
+      <c r="G7" s="243"/>
+      <c r="H7" s="244"/>
+      <c r="I7" s="249" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="244"/>
+      <c r="J7" s="250"/>
     </row>
     <row r="8" spans="1:10" ht="336" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="250"/>
-      <c r="B8" s="251"/>
-      <c r="C8" s="251"/>
-      <c r="D8" s="251"/>
-      <c r="E8" s="251"/>
-      <c r="F8" s="251"/>
-      <c r="G8" s="251"/>
-      <c r="H8" s="252"/>
-      <c r="I8" s="245" t="s">
+      <c r="A8" s="242"/>
+      <c r="B8" s="243"/>
+      <c r="C8" s="243"/>
+      <c r="D8" s="243"/>
+      <c r="E8" s="243"/>
+      <c r="F8" s="243"/>
+      <c r="G8" s="243"/>
+      <c r="H8" s="244"/>
+      <c r="I8" s="237" t="s">
         <v>171</v>
       </c>
-      <c r="J8" s="246"/>
+      <c r="J8" s="238"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
@@ -5651,359 +5665,339 @@
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="220"/>
-      <c r="F15" s="220"/>
-      <c r="G15" s="220"/>
-      <c r="H15" s="220"/>
-      <c r="I15" s="220"/>
-      <c r="J15" s="220"/>
+      <c r="E15" s="205"/>
+      <c r="F15" s="205"/>
+      <c r="G15" s="205"/>
+      <c r="H15" s="205"/>
+      <c r="I15" s="205"/>
+      <c r="J15" s="205"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="220"/>
-      <c r="F16" s="220"/>
-      <c r="G16" s="220"/>
-      <c r="H16" s="220"/>
-      <c r="I16" s="220"/>
-      <c r="J16" s="220"/>
+      <c r="E16" s="205"/>
+      <c r="F16" s="205"/>
+      <c r="G16" s="205"/>
+      <c r="H16" s="205"/>
+      <c r="I16" s="205"/>
+      <c r="J16" s="205"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="220"/>
-      <c r="F17" s="220"/>
-      <c r="G17" s="220"/>
-      <c r="H17" s="220"/>
-      <c r="I17" s="220"/>
-      <c r="J17" s="220"/>
+      <c r="E17" s="205"/>
+      <c r="F17" s="205"/>
+      <c r="G17" s="205"/>
+      <c r="H17" s="205"/>
+      <c r="I17" s="205"/>
+      <c r="J17" s="205"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="220"/>
-      <c r="F18" s="220"/>
-      <c r="G18" s="220"/>
-      <c r="H18" s="220"/>
-      <c r="I18" s="220"/>
-      <c r="J18" s="220"/>
+      <c r="E18" s="205"/>
+      <c r="F18" s="205"/>
+      <c r="G18" s="205"/>
+      <c r="H18" s="205"/>
+      <c r="I18" s="205"/>
+      <c r="J18" s="205"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="220"/>
-      <c r="F19" s="220"/>
-      <c r="G19" s="220"/>
-      <c r="H19" s="220"/>
-      <c r="I19" s="220"/>
-      <c r="J19" s="220"/>
+      <c r="E19" s="205"/>
+      <c r="F19" s="205"/>
+      <c r="G19" s="205"/>
+      <c r="H19" s="205"/>
+      <c r="I19" s="205"/>
+      <c r="J19" s="205"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="220"/>
-      <c r="F20" s="220"/>
-      <c r="G20" s="220"/>
-      <c r="H20" s="220"/>
-      <c r="I20" s="220"/>
-      <c r="J20" s="220"/>
+      <c r="E20" s="205"/>
+      <c r="F20" s="205"/>
+      <c r="G20" s="205"/>
+      <c r="H20" s="205"/>
+      <c r="I20" s="205"/>
+      <c r="J20" s="205"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="220"/>
-      <c r="F21" s="220"/>
-      <c r="G21" s="220"/>
-      <c r="H21" s="220"/>
-      <c r="I21" s="220"/>
-      <c r="J21" s="220"/>
+      <c r="E21" s="205"/>
+      <c r="F21" s="205"/>
+      <c r="G21" s="205"/>
+      <c r="H21" s="205"/>
+      <c r="I21" s="205"/>
+      <c r="J21" s="205"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="220"/>
-      <c r="F22" s="220"/>
-      <c r="G22" s="220"/>
-      <c r="H22" s="220"/>
-      <c r="I22" s="220"/>
-      <c r="J22" s="220"/>
+      <c r="E22" s="205"/>
+      <c r="F22" s="205"/>
+      <c r="G22" s="205"/>
+      <c r="H22" s="205"/>
+      <c r="I22" s="205"/>
+      <c r="J22" s="205"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="220"/>
-      <c r="F23" s="220"/>
-      <c r="G23" s="220"/>
-      <c r="H23" s="220"/>
-      <c r="I23" s="220"/>
-      <c r="J23" s="220"/>
+      <c r="E23" s="205"/>
+      <c r="F23" s="205"/>
+      <c r="G23" s="205"/>
+      <c r="H23" s="205"/>
+      <c r="I23" s="205"/>
+      <c r="J23" s="205"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="220"/>
-      <c r="F24" s="220"/>
-      <c r="G24" s="220"/>
-      <c r="H24" s="220"/>
-      <c r="I24" s="220"/>
-      <c r="J24" s="220"/>
+      <c r="E24" s="205"/>
+      <c r="F24" s="205"/>
+      <c r="G24" s="205"/>
+      <c r="H24" s="205"/>
+      <c r="I24" s="205"/>
+      <c r="J24" s="205"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="220"/>
-      <c r="F25" s="220"/>
-      <c r="G25" s="220"/>
-      <c r="H25" s="220"/>
-      <c r="I25" s="220"/>
-      <c r="J25" s="220"/>
+      <c r="E25" s="205"/>
+      <c r="F25" s="205"/>
+      <c r="G25" s="205"/>
+      <c r="H25" s="205"/>
+      <c r="I25" s="205"/>
+      <c r="J25" s="205"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="220"/>
-      <c r="F26" s="220"/>
-      <c r="G26" s="220"/>
-      <c r="H26" s="220"/>
-      <c r="I26" s="220"/>
-      <c r="J26" s="220"/>
+      <c r="E26" s="205"/>
+      <c r="F26" s="205"/>
+      <c r="G26" s="205"/>
+      <c r="H26" s="205"/>
+      <c r="I26" s="205"/>
+      <c r="J26" s="205"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="220"/>
-      <c r="F27" s="220"/>
-      <c r="G27" s="220"/>
-      <c r="H27" s="220"/>
-      <c r="I27" s="220"/>
-      <c r="J27" s="220"/>
+      <c r="E27" s="205"/>
+      <c r="F27" s="205"/>
+      <c r="G27" s="205"/>
+      <c r="H27" s="205"/>
+      <c r="I27" s="205"/>
+      <c r="J27" s="205"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="220"/>
-      <c r="F28" s="220"/>
-      <c r="G28" s="220"/>
-      <c r="H28" s="220"/>
-      <c r="I28" s="220"/>
-      <c r="J28" s="220"/>
+      <c r="E28" s="205"/>
+      <c r="F28" s="205"/>
+      <c r="G28" s="205"/>
+      <c r="H28" s="205"/>
+      <c r="I28" s="205"/>
+      <c r="J28" s="205"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="220"/>
-      <c r="F29" s="220"/>
-      <c r="G29" s="220"/>
-      <c r="H29" s="220"/>
-      <c r="I29" s="220"/>
-      <c r="J29" s="220"/>
+      <c r="E29" s="205"/>
+      <c r="F29" s="205"/>
+      <c r="G29" s="205"/>
+      <c r="H29" s="205"/>
+      <c r="I29" s="205"/>
+      <c r="J29" s="205"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="220"/>
-      <c r="F30" s="220"/>
-      <c r="G30" s="220"/>
-      <c r="H30" s="220"/>
-      <c r="I30" s="220"/>
-      <c r="J30" s="220"/>
+      <c r="E30" s="205"/>
+      <c r="F30" s="205"/>
+      <c r="G30" s="205"/>
+      <c r="H30" s="205"/>
+      <c r="I30" s="205"/>
+      <c r="J30" s="205"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="220"/>
-      <c r="F31" s="220"/>
-      <c r="G31" s="220"/>
-      <c r="H31" s="220"/>
-      <c r="I31" s="220"/>
-      <c r="J31" s="220"/>
+      <c r="E31" s="205"/>
+      <c r="F31" s="205"/>
+      <c r="G31" s="205"/>
+      <c r="H31" s="205"/>
+      <c r="I31" s="205"/>
+      <c r="J31" s="205"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="220"/>
-      <c r="F32" s="220"/>
-      <c r="G32" s="220"/>
-      <c r="H32" s="220"/>
-      <c r="I32" s="220"/>
-      <c r="J32" s="220"/>
+      <c r="E32" s="205"/>
+      <c r="F32" s="205"/>
+      <c r="G32" s="205"/>
+      <c r="H32" s="205"/>
+      <c r="I32" s="205"/>
+      <c r="J32" s="205"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="220"/>
-      <c r="F33" s="220"/>
-      <c r="G33" s="220"/>
-      <c r="H33" s="220"/>
-      <c r="I33" s="220"/>
-      <c r="J33" s="220"/>
+      <c r="E33" s="205"/>
+      <c r="F33" s="205"/>
+      <c r="G33" s="205"/>
+      <c r="H33" s="205"/>
+      <c r="I33" s="205"/>
+      <c r="J33" s="205"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="220"/>
-      <c r="F34" s="220"/>
-      <c r="G34" s="220"/>
-      <c r="H34" s="220"/>
-      <c r="I34" s="220"/>
-      <c r="J34" s="220"/>
+      <c r="E34" s="205"/>
+      <c r="F34" s="205"/>
+      <c r="G34" s="205"/>
+      <c r="H34" s="205"/>
+      <c r="I34" s="205"/>
+      <c r="J34" s="205"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="220"/>
-      <c r="F35" s="220"/>
-      <c r="G35" s="220"/>
-      <c r="H35" s="220"/>
-      <c r="I35" s="220"/>
-      <c r="J35" s="220"/>
+      <c r="E35" s="205"/>
+      <c r="F35" s="205"/>
+      <c r="G35" s="205"/>
+      <c r="H35" s="205"/>
+      <c r="I35" s="205"/>
+      <c r="J35" s="205"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="220"/>
-      <c r="F36" s="220"/>
-      <c r="G36" s="220"/>
-      <c r="H36" s="220"/>
-      <c r="I36" s="220"/>
-      <c r="J36" s="220"/>
+      <c r="E36" s="205"/>
+      <c r="F36" s="205"/>
+      <c r="G36" s="205"/>
+      <c r="H36" s="205"/>
+      <c r="I36" s="205"/>
+      <c r="J36" s="205"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="220"/>
-      <c r="F37" s="220"/>
-      <c r="G37" s="220"/>
-      <c r="H37" s="220"/>
-      <c r="I37" s="220"/>
-      <c r="J37" s="220"/>
+      <c r="E37" s="205"/>
+      <c r="F37" s="205"/>
+      <c r="G37" s="205"/>
+      <c r="H37" s="205"/>
+      <c r="I37" s="205"/>
+      <c r="J37" s="205"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="220"/>
-      <c r="F38" s="220"/>
-      <c r="G38" s="220"/>
-      <c r="H38" s="220"/>
-      <c r="I38" s="220"/>
-      <c r="J38" s="220"/>
+      <c r="E38" s="205"/>
+      <c r="F38" s="205"/>
+      <c r="G38" s="205"/>
+      <c r="H38" s="205"/>
+      <c r="I38" s="205"/>
+      <c r="J38" s="205"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="220"/>
-      <c r="F39" s="220"/>
-      <c r="G39" s="220"/>
-      <c r="H39" s="220"/>
-      <c r="I39" s="220"/>
-      <c r="J39" s="220"/>
+      <c r="E39" s="205"/>
+      <c r="F39" s="205"/>
+      <c r="G39" s="205"/>
+      <c r="H39" s="205"/>
+      <c r="I39" s="205"/>
+      <c r="J39" s="205"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="220"/>
-      <c r="F40" s="220"/>
-      <c r="G40" s="220"/>
-      <c r="H40" s="220"/>
-      <c r="I40" s="220"/>
-      <c r="J40" s="220"/>
+      <c r="E40" s="205"/>
+      <c r="F40" s="205"/>
+      <c r="G40" s="205"/>
+      <c r="H40" s="205"/>
+      <c r="I40" s="205"/>
+      <c r="J40" s="205"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="220"/>
-      <c r="F41" s="220"/>
-      <c r="G41" s="220"/>
-      <c r="H41" s="220"/>
-      <c r="I41" s="220"/>
-      <c r="J41" s="220"/>
+      <c r="E41" s="205"/>
+      <c r="F41" s="205"/>
+      <c r="G41" s="205"/>
+      <c r="H41" s="205"/>
+      <c r="I41" s="205"/>
+      <c r="J41" s="205"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="220"/>
-      <c r="F42" s="220"/>
-      <c r="G42" s="220"/>
-      <c r="H42" s="220"/>
-      <c r="I42" s="220"/>
-      <c r="J42" s="220"/>
+      <c r="E42" s="205"/>
+      <c r="F42" s="205"/>
+      <c r="G42" s="205"/>
+      <c r="H42" s="205"/>
+      <c r="I42" s="205"/>
+      <c r="J42" s="205"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="A5:H8"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E20:J20"/>
-    <mergeCell ref="E21:J21"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
     <mergeCell ref="E39:J39"/>
     <mergeCell ref="E40:J40"/>
     <mergeCell ref="E41:J41"/>
@@ -6020,6 +6014,26 @@
     <mergeCell ref="E37:J37"/>
     <mergeCell ref="E38:J38"/>
     <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="A5:H8"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E25:J25"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2">
@@ -6061,10 +6075,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="210" t="s">
+      <c r="A1" s="227" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="253"/>
+      <c r="B1" s="251"/>
       <c r="C1" s="128" t="s">
         <v>1</v>
       </c>
@@ -6089,18 +6103,18 @@
       <c r="I1" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="254" t="str">
+      <c r="J1" s="252" t="str">
         <f>'Update History'!J1</f>
         <v>Thị Phượng</v>
       </c>
-      <c r="K1" s="255"/>
+      <c r="K1" s="253"/>
       <c r="L1" s="17"/>
       <c r="M1" s="17"/>
       <c r="N1" s="17"/>
     </row>
     <row r="2" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="210"/>
-      <c r="B2" s="253"/>
+      <c r="A2" s="227"/>
+      <c r="B2" s="251"/>
       <c r="C2" s="128" t="s">
         <v>7</v>
       </c>
@@ -6125,11 +6139,11 @@
       <c r="I2" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="256">
+      <c r="J2" s="254">
         <f>'Update History'!J2</f>
         <v>42381</v>
       </c>
-      <c r="K2" s="257"/>
+      <c r="K2" s="255"/>
       <c r="L2" s="17"/>
       <c r="M2" s="17"/>
       <c r="N2" s="17"/>
@@ -7848,10 +7862,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="210" t="s">
+      <c r="A1" s="227" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="210"/>
+      <c r="B1" s="227"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -7882,8 +7896,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="210"/>
-      <c r="B2" s="210"/>
+      <c r="A2" s="227"/>
+      <c r="B2" s="227"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -7947,11 +7961,11 @@
       <c r="G4" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="261" t="s">
+      <c r="H4" s="259" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="261"/>
-      <c r="J4" s="261"/>
+      <c r="I4" s="259"/>
+      <c r="J4" s="259"/>
     </row>
     <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
@@ -7969,11 +7983,11 @@
       <c r="G5" s="194" t="s">
         <v>252</v>
       </c>
-      <c r="H5" s="262" t="s">
+      <c r="H5" s="260" t="s">
         <v>254</v>
       </c>
-      <c r="I5" s="263"/>
-      <c r="J5" s="264"/>
+      <c r="I5" s="261"/>
+      <c r="J5" s="262"/>
     </row>
     <row r="6" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="200"/>
@@ -7991,11 +8005,11 @@
       <c r="G6" s="204" t="s">
         <v>252</v>
       </c>
-      <c r="H6" s="262" t="s">
+      <c r="H6" s="260" t="s">
         <v>253</v>
       </c>
-      <c r="I6" s="263"/>
-      <c r="J6" s="264"/>
+      <c r="I6" s="261"/>
+      <c r="J6" s="262"/>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="56"/>
@@ -8005,9 +8019,9 @@
       <c r="E7" s="51"/>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
-      <c r="H7" s="258"/>
-      <c r="I7" s="259"/>
-      <c r="J7" s="260"/>
+      <c r="H7" s="256"/>
+      <c r="I7" s="257"/>
+      <c r="J7" s="258"/>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
@@ -8017,9 +8031,9 @@
       <c r="E8" s="50"/>
       <c r="F8" s="50"/>
       <c r="G8" s="50"/>
-      <c r="H8" s="258"/>
-      <c r="I8" s="259"/>
-      <c r="J8" s="260"/>
+      <c r="H8" s="256"/>
+      <c r="I8" s="257"/>
+      <c r="J8" s="258"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
@@ -8029,9 +8043,9 @@
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
-      <c r="H9" s="258"/>
-      <c r="I9" s="259"/>
-      <c r="J9" s="260"/>
+      <c r="H9" s="256"/>
+      <c r="I9" s="257"/>
+      <c r="J9" s="258"/>
     </row>
     <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="56"/>
@@ -8041,9 +8055,9 @@
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
-      <c r="H10" s="258"/>
-      <c r="I10" s="259"/>
-      <c r="J10" s="260"/>
+      <c r="H10" s="256"/>
+      <c r="I10" s="257"/>
+      <c r="J10" s="258"/>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="56"/>
@@ -8053,9 +8067,9 @@
       <c r="E11" s="51"/>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
-      <c r="H11" s="258"/>
-      <c r="I11" s="259"/>
-      <c r="J11" s="260"/>
+      <c r="H11" s="256"/>
+      <c r="I11" s="257"/>
+      <c r="J11" s="258"/>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="56"/>
@@ -8065,9 +8079,9 @@
       <c r="E12" s="51"/>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
-      <c r="H12" s="258"/>
-      <c r="I12" s="259"/>
-      <c r="J12" s="260"/>
+      <c r="H12" s="256"/>
+      <c r="I12" s="257"/>
+      <c r="J12" s="258"/>
     </row>
     <row r="13" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="56"/>
@@ -8077,9 +8091,9 @@
       <c r="E13" s="55"/>
       <c r="F13" s="55"/>
       <c r="G13" s="55"/>
-      <c r="H13" s="258"/>
-      <c r="I13" s="259"/>
-      <c r="J13" s="260"/>
+      <c r="H13" s="256"/>
+      <c r="I13" s="257"/>
+      <c r="J13" s="258"/>
     </row>
     <row r="14" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="56"/>
@@ -8089,372 +8103,348 @@
       <c r="E14" s="55"/>
       <c r="F14" s="55"/>
       <c r="G14" s="55"/>
-      <c r="H14" s="258"/>
-      <c r="I14" s="259"/>
-      <c r="J14" s="260"/>
+      <c r="H14" s="256"/>
+      <c r="I14" s="257"/>
+      <c r="J14" s="258"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="220"/>
-      <c r="F15" s="220"/>
-      <c r="G15" s="220"/>
-      <c r="H15" s="220"/>
-      <c r="I15" s="220"/>
-      <c r="J15" s="220"/>
+      <c r="E15" s="205"/>
+      <c r="F15" s="205"/>
+      <c r="G15" s="205"/>
+      <c r="H15" s="205"/>
+      <c r="I15" s="205"/>
+      <c r="J15" s="205"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="220"/>
-      <c r="F16" s="220"/>
-      <c r="G16" s="220"/>
-      <c r="H16" s="220"/>
-      <c r="I16" s="220"/>
-      <c r="J16" s="220"/>
+      <c r="E16" s="205"/>
+      <c r="F16" s="205"/>
+      <c r="G16" s="205"/>
+      <c r="H16" s="205"/>
+      <c r="I16" s="205"/>
+      <c r="J16" s="205"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="220"/>
-      <c r="F17" s="220"/>
-      <c r="G17" s="220"/>
-      <c r="H17" s="220"/>
-      <c r="I17" s="220"/>
-      <c r="J17" s="220"/>
+      <c r="E17" s="205"/>
+      <c r="F17" s="205"/>
+      <c r="G17" s="205"/>
+      <c r="H17" s="205"/>
+      <c r="I17" s="205"/>
+      <c r="J17" s="205"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="220"/>
-      <c r="F18" s="220"/>
-      <c r="G18" s="220"/>
-      <c r="H18" s="220"/>
-      <c r="I18" s="220"/>
-      <c r="J18" s="220"/>
+      <c r="E18" s="205"/>
+      <c r="F18" s="205"/>
+      <c r="G18" s="205"/>
+      <c r="H18" s="205"/>
+      <c r="I18" s="205"/>
+      <c r="J18" s="205"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="220"/>
-      <c r="F19" s="220"/>
-      <c r="G19" s="220"/>
-      <c r="H19" s="220"/>
-      <c r="I19" s="220"/>
-      <c r="J19" s="220"/>
+      <c r="E19" s="205"/>
+      <c r="F19" s="205"/>
+      <c r="G19" s="205"/>
+      <c r="H19" s="205"/>
+      <c r="I19" s="205"/>
+      <c r="J19" s="205"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="220"/>
-      <c r="F20" s="220"/>
-      <c r="G20" s="220"/>
-      <c r="H20" s="220"/>
-      <c r="I20" s="220"/>
-      <c r="J20" s="220"/>
+      <c r="E20" s="205"/>
+      <c r="F20" s="205"/>
+      <c r="G20" s="205"/>
+      <c r="H20" s="205"/>
+      <c r="I20" s="205"/>
+      <c r="J20" s="205"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="220"/>
-      <c r="F21" s="220"/>
-      <c r="G21" s="220"/>
-      <c r="H21" s="220"/>
-      <c r="I21" s="220"/>
-      <c r="J21" s="220"/>
+      <c r="E21" s="205"/>
+      <c r="F21" s="205"/>
+      <c r="G21" s="205"/>
+      <c r="H21" s="205"/>
+      <c r="I21" s="205"/>
+      <c r="J21" s="205"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="220"/>
-      <c r="F22" s="220"/>
-      <c r="G22" s="220"/>
-      <c r="H22" s="220"/>
-      <c r="I22" s="220"/>
-      <c r="J22" s="220"/>
+      <c r="E22" s="205"/>
+      <c r="F22" s="205"/>
+      <c r="G22" s="205"/>
+      <c r="H22" s="205"/>
+      <c r="I22" s="205"/>
+      <c r="J22" s="205"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="220"/>
-      <c r="F23" s="220"/>
-      <c r="G23" s="220"/>
-      <c r="H23" s="220"/>
-      <c r="I23" s="220"/>
-      <c r="J23" s="220"/>
+      <c r="E23" s="205"/>
+      <c r="F23" s="205"/>
+      <c r="G23" s="205"/>
+      <c r="H23" s="205"/>
+      <c r="I23" s="205"/>
+      <c r="J23" s="205"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="220"/>
-      <c r="F24" s="220"/>
-      <c r="G24" s="220"/>
-      <c r="H24" s="220"/>
-      <c r="I24" s="220"/>
-      <c r="J24" s="220"/>
+      <c r="E24" s="205"/>
+      <c r="F24" s="205"/>
+      <c r="G24" s="205"/>
+      <c r="H24" s="205"/>
+      <c r="I24" s="205"/>
+      <c r="J24" s="205"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="220"/>
-      <c r="F25" s="220"/>
-      <c r="G25" s="220"/>
-      <c r="H25" s="220"/>
-      <c r="I25" s="220"/>
-      <c r="J25" s="220"/>
+      <c r="E25" s="205"/>
+      <c r="F25" s="205"/>
+      <c r="G25" s="205"/>
+      <c r="H25" s="205"/>
+      <c r="I25" s="205"/>
+      <c r="J25" s="205"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="220"/>
-      <c r="F26" s="220"/>
-      <c r="G26" s="220"/>
-      <c r="H26" s="220"/>
-      <c r="I26" s="220"/>
-      <c r="J26" s="220"/>
+      <c r="E26" s="205"/>
+      <c r="F26" s="205"/>
+      <c r="G26" s="205"/>
+      <c r="H26" s="205"/>
+      <c r="I26" s="205"/>
+      <c r="J26" s="205"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="220"/>
-      <c r="F27" s="220"/>
-      <c r="G27" s="220"/>
-      <c r="H27" s="220"/>
-      <c r="I27" s="220"/>
-      <c r="J27" s="220"/>
+      <c r="E27" s="205"/>
+      <c r="F27" s="205"/>
+      <c r="G27" s="205"/>
+      <c r="H27" s="205"/>
+      <c r="I27" s="205"/>
+      <c r="J27" s="205"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="220"/>
-      <c r="F28" s="220"/>
-      <c r="G28" s="220"/>
-      <c r="H28" s="220"/>
-      <c r="I28" s="220"/>
-      <c r="J28" s="220"/>
+      <c r="E28" s="205"/>
+      <c r="F28" s="205"/>
+      <c r="G28" s="205"/>
+      <c r="H28" s="205"/>
+      <c r="I28" s="205"/>
+      <c r="J28" s="205"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="220"/>
-      <c r="F29" s="220"/>
-      <c r="G29" s="220"/>
-      <c r="H29" s="220"/>
-      <c r="I29" s="220"/>
-      <c r="J29" s="220"/>
+      <c r="E29" s="205"/>
+      <c r="F29" s="205"/>
+      <c r="G29" s="205"/>
+      <c r="H29" s="205"/>
+      <c r="I29" s="205"/>
+      <c r="J29" s="205"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="220"/>
-      <c r="F30" s="220"/>
-      <c r="G30" s="220"/>
-      <c r="H30" s="220"/>
-      <c r="I30" s="220"/>
-      <c r="J30" s="220"/>
+      <c r="E30" s="205"/>
+      <c r="F30" s="205"/>
+      <c r="G30" s="205"/>
+      <c r="H30" s="205"/>
+      <c r="I30" s="205"/>
+      <c r="J30" s="205"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="220"/>
-      <c r="F31" s="220"/>
-      <c r="G31" s="220"/>
-      <c r="H31" s="220"/>
-      <c r="I31" s="220"/>
-      <c r="J31" s="220"/>
+      <c r="E31" s="205"/>
+      <c r="F31" s="205"/>
+      <c r="G31" s="205"/>
+      <c r="H31" s="205"/>
+      <c r="I31" s="205"/>
+      <c r="J31" s="205"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="220"/>
-      <c r="F32" s="220"/>
-      <c r="G32" s="220"/>
-      <c r="H32" s="220"/>
-      <c r="I32" s="220"/>
-      <c r="J32" s="220"/>
+      <c r="E32" s="205"/>
+      <c r="F32" s="205"/>
+      <c r="G32" s="205"/>
+      <c r="H32" s="205"/>
+      <c r="I32" s="205"/>
+      <c r="J32" s="205"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="220"/>
-      <c r="F33" s="220"/>
-      <c r="G33" s="220"/>
-      <c r="H33" s="220"/>
-      <c r="I33" s="220"/>
-      <c r="J33" s="220"/>
+      <c r="E33" s="205"/>
+      <c r="F33" s="205"/>
+      <c r="G33" s="205"/>
+      <c r="H33" s="205"/>
+      <c r="I33" s="205"/>
+      <c r="J33" s="205"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="220"/>
-      <c r="F34" s="220"/>
-      <c r="G34" s="220"/>
-      <c r="H34" s="220"/>
-      <c r="I34" s="220"/>
-      <c r="J34" s="220"/>
+      <c r="E34" s="205"/>
+      <c r="F34" s="205"/>
+      <c r="G34" s="205"/>
+      <c r="H34" s="205"/>
+      <c r="I34" s="205"/>
+      <c r="J34" s="205"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="220"/>
-      <c r="F35" s="220"/>
-      <c r="G35" s="220"/>
-      <c r="H35" s="220"/>
-      <c r="I35" s="220"/>
-      <c r="J35" s="220"/>
+      <c r="E35" s="205"/>
+      <c r="F35" s="205"/>
+      <c r="G35" s="205"/>
+      <c r="H35" s="205"/>
+      <c r="I35" s="205"/>
+      <c r="J35" s="205"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="220"/>
-      <c r="F36" s="220"/>
-      <c r="G36" s="220"/>
-      <c r="H36" s="220"/>
-      <c r="I36" s="220"/>
-      <c r="J36" s="220"/>
+      <c r="E36" s="205"/>
+      <c r="F36" s="205"/>
+      <c r="G36" s="205"/>
+      <c r="H36" s="205"/>
+      <c r="I36" s="205"/>
+      <c r="J36" s="205"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="220"/>
-      <c r="F37" s="220"/>
-      <c r="G37" s="220"/>
-      <c r="H37" s="220"/>
-      <c r="I37" s="220"/>
-      <c r="J37" s="220"/>
+      <c r="E37" s="205"/>
+      <c r="F37" s="205"/>
+      <c r="G37" s="205"/>
+      <c r="H37" s="205"/>
+      <c r="I37" s="205"/>
+      <c r="J37" s="205"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="220"/>
-      <c r="F38" s="220"/>
-      <c r="G38" s="220"/>
-      <c r="H38" s="220"/>
-      <c r="I38" s="220"/>
-      <c r="J38" s="220"/>
+      <c r="E38" s="205"/>
+      <c r="F38" s="205"/>
+      <c r="G38" s="205"/>
+      <c r="H38" s="205"/>
+      <c r="I38" s="205"/>
+      <c r="J38" s="205"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="220"/>
-      <c r="F39" s="220"/>
-      <c r="G39" s="220"/>
-      <c r="H39" s="220"/>
-      <c r="I39" s="220"/>
-      <c r="J39" s="220"/>
+      <c r="E39" s="205"/>
+      <c r="F39" s="205"/>
+      <c r="G39" s="205"/>
+      <c r="H39" s="205"/>
+      <c r="I39" s="205"/>
+      <c r="J39" s="205"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="220"/>
-      <c r="F40" s="220"/>
-      <c r="G40" s="220"/>
-      <c r="H40" s="220"/>
-      <c r="I40" s="220"/>
-      <c r="J40" s="220"/>
+      <c r="E40" s="205"/>
+      <c r="F40" s="205"/>
+      <c r="G40" s="205"/>
+      <c r="H40" s="205"/>
+      <c r="I40" s="205"/>
+      <c r="J40" s="205"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="220"/>
-      <c r="F41" s="220"/>
-      <c r="G41" s="220"/>
-      <c r="H41" s="220"/>
-      <c r="I41" s="220"/>
-      <c r="J41" s="220"/>
+      <c r="E41" s="205"/>
+      <c r="F41" s="205"/>
+      <c r="G41" s="205"/>
+      <c r="H41" s="205"/>
+      <c r="I41" s="205"/>
+      <c r="J41" s="205"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="220"/>
-      <c r="F42" s="220"/>
-      <c r="G42" s="220"/>
-      <c r="H42" s="220"/>
-      <c r="I42" s="220"/>
-      <c r="J42" s="220"/>
+      <c r="E42" s="205"/>
+      <c r="F42" s="205"/>
+      <c r="G42" s="205"/>
+      <c r="H42" s="205"/>
+      <c r="I42" s="205"/>
+      <c r="J42" s="205"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="E39:J39"/>
     <mergeCell ref="E40:J40"/>
@@ -8471,6 +8461,30 @@
     <mergeCell ref="E20:J20"/>
     <mergeCell ref="E21:J21"/>
     <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H8:J8"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2">
@@ -8506,10 +8520,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="210" t="s">
+      <c r="A1" s="227" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="210"/>
+      <c r="B1" s="227"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -8540,8 +8554,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="210"/>
-      <c r="B2" s="210"/>
+      <c r="A2" s="227"/>
+      <c r="B2" s="227"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -8572,16 +8586,16 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="269"/>
-      <c r="B3" s="270"/>
-      <c r="C3" s="270"/>
-      <c r="D3" s="270"/>
-      <c r="E3" s="270"/>
-      <c r="F3" s="270"/>
-      <c r="G3" s="270"/>
-      <c r="H3" s="270"/>
-      <c r="I3" s="270"/>
-      <c r="J3" s="271"/>
+      <c r="A3" s="267"/>
+      <c r="B3" s="268"/>
+      <c r="C3" s="268"/>
+      <c r="D3" s="268"/>
+      <c r="E3" s="268"/>
+      <c r="F3" s="268"/>
+      <c r="G3" s="268"/>
+      <c r="H3" s="268"/>
+      <c r="I3" s="268"/>
+      <c r="J3" s="269"/>
     </row>
     <row r="4" spans="1:10" s="45" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="66" t="s">
@@ -8596,16 +8610,16 @@
       <c r="D4" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="265" t="s">
+      <c r="E4" s="263" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="265"/>
-      <c r="G4" s="266" t="s">
+      <c r="F4" s="263"/>
+      <c r="G4" s="264" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="267"/>
-      <c r="I4" s="267"/>
-      <c r="J4" s="268"/>
+      <c r="H4" s="265"/>
+      <c r="I4" s="265"/>
+      <c r="J4" s="266"/>
     </row>
     <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
@@ -8732,347 +8746,351 @@
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="220"/>
-      <c r="F15" s="220"/>
-      <c r="G15" s="220"/>
-      <c r="H15" s="220"/>
-      <c r="I15" s="220"/>
-      <c r="J15" s="220"/>
+      <c r="E15" s="205"/>
+      <c r="F15" s="205"/>
+      <c r="G15" s="205"/>
+      <c r="H15" s="205"/>
+      <c r="I15" s="205"/>
+      <c r="J15" s="205"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="220"/>
-      <c r="F16" s="220"/>
-      <c r="G16" s="220"/>
-      <c r="H16" s="220"/>
-      <c r="I16" s="220"/>
-      <c r="J16" s="220"/>
+      <c r="E16" s="205"/>
+      <c r="F16" s="205"/>
+      <c r="G16" s="205"/>
+      <c r="H16" s="205"/>
+      <c r="I16" s="205"/>
+      <c r="J16" s="205"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="220"/>
-      <c r="F17" s="220"/>
-      <c r="G17" s="220"/>
-      <c r="H17" s="220"/>
-      <c r="I17" s="220"/>
-      <c r="J17" s="220"/>
+      <c r="E17" s="205"/>
+      <c r="F17" s="205"/>
+      <c r="G17" s="205"/>
+      <c r="H17" s="205"/>
+      <c r="I17" s="205"/>
+      <c r="J17" s="205"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="220"/>
-      <c r="F18" s="220"/>
-      <c r="G18" s="220"/>
-      <c r="H18" s="220"/>
-      <c r="I18" s="220"/>
-      <c r="J18" s="220"/>
+      <c r="E18" s="205"/>
+      <c r="F18" s="205"/>
+      <c r="G18" s="205"/>
+      <c r="H18" s="205"/>
+      <c r="I18" s="205"/>
+      <c r="J18" s="205"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="220"/>
-      <c r="F19" s="220"/>
-      <c r="G19" s="220"/>
-      <c r="H19" s="220"/>
-      <c r="I19" s="220"/>
-      <c r="J19" s="220"/>
+      <c r="E19" s="205"/>
+      <c r="F19" s="205"/>
+      <c r="G19" s="205"/>
+      <c r="H19" s="205"/>
+      <c r="I19" s="205"/>
+      <c r="J19" s="205"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="220"/>
-      <c r="F20" s="220"/>
-      <c r="G20" s="220"/>
-      <c r="H20" s="220"/>
-      <c r="I20" s="220"/>
-      <c r="J20" s="220"/>
+      <c r="E20" s="205"/>
+      <c r="F20" s="205"/>
+      <c r="G20" s="205"/>
+      <c r="H20" s="205"/>
+      <c r="I20" s="205"/>
+      <c r="J20" s="205"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="220"/>
-      <c r="F21" s="220"/>
-      <c r="G21" s="220"/>
-      <c r="H21" s="220"/>
-      <c r="I21" s="220"/>
-      <c r="J21" s="220"/>
+      <c r="E21" s="205"/>
+      <c r="F21" s="205"/>
+      <c r="G21" s="205"/>
+      <c r="H21" s="205"/>
+      <c r="I21" s="205"/>
+      <c r="J21" s="205"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="220"/>
-      <c r="F22" s="220"/>
-      <c r="G22" s="220"/>
-      <c r="H22" s="220"/>
-      <c r="I22" s="220"/>
-      <c r="J22" s="220"/>
+      <c r="E22" s="205"/>
+      <c r="F22" s="205"/>
+      <c r="G22" s="205"/>
+      <c r="H22" s="205"/>
+      <c r="I22" s="205"/>
+      <c r="J22" s="205"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="220"/>
-      <c r="F23" s="220"/>
-      <c r="G23" s="220"/>
-      <c r="H23" s="220"/>
-      <c r="I23" s="220"/>
-      <c r="J23" s="220"/>
+      <c r="E23" s="205"/>
+      <c r="F23" s="205"/>
+      <c r="G23" s="205"/>
+      <c r="H23" s="205"/>
+      <c r="I23" s="205"/>
+      <c r="J23" s="205"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="220"/>
-      <c r="F24" s="220"/>
-      <c r="G24" s="220"/>
-      <c r="H24" s="220"/>
-      <c r="I24" s="220"/>
-      <c r="J24" s="220"/>
+      <c r="E24" s="205"/>
+      <c r="F24" s="205"/>
+      <c r="G24" s="205"/>
+      <c r="H24" s="205"/>
+      <c r="I24" s="205"/>
+      <c r="J24" s="205"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="220"/>
-      <c r="F25" s="220"/>
-      <c r="G25" s="220"/>
-      <c r="H25" s="220"/>
-      <c r="I25" s="220"/>
-      <c r="J25" s="220"/>
+      <c r="E25" s="205"/>
+      <c r="F25" s="205"/>
+      <c r="G25" s="205"/>
+      <c r="H25" s="205"/>
+      <c r="I25" s="205"/>
+      <c r="J25" s="205"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="220"/>
-      <c r="F26" s="220"/>
-      <c r="G26" s="220"/>
-      <c r="H26" s="220"/>
-      <c r="I26" s="220"/>
-      <c r="J26" s="220"/>
+      <c r="E26" s="205"/>
+      <c r="F26" s="205"/>
+      <c r="G26" s="205"/>
+      <c r="H26" s="205"/>
+      <c r="I26" s="205"/>
+      <c r="J26" s="205"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="220"/>
-      <c r="F27" s="220"/>
-      <c r="G27" s="220"/>
-      <c r="H27" s="220"/>
-      <c r="I27" s="220"/>
-      <c r="J27" s="220"/>
+      <c r="E27" s="205"/>
+      <c r="F27" s="205"/>
+      <c r="G27" s="205"/>
+      <c r="H27" s="205"/>
+      <c r="I27" s="205"/>
+      <c r="J27" s="205"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="220"/>
-      <c r="F28" s="220"/>
-      <c r="G28" s="220"/>
-      <c r="H28" s="220"/>
-      <c r="I28" s="220"/>
-      <c r="J28" s="220"/>
+      <c r="E28" s="205"/>
+      <c r="F28" s="205"/>
+      <c r="G28" s="205"/>
+      <c r="H28" s="205"/>
+      <c r="I28" s="205"/>
+      <c r="J28" s="205"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="220"/>
-      <c r="F29" s="220"/>
-      <c r="G29" s="220"/>
-      <c r="H29" s="220"/>
-      <c r="I29" s="220"/>
-      <c r="J29" s="220"/>
+      <c r="E29" s="205"/>
+      <c r="F29" s="205"/>
+      <c r="G29" s="205"/>
+      <c r="H29" s="205"/>
+      <c r="I29" s="205"/>
+      <c r="J29" s="205"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="220"/>
-      <c r="F30" s="220"/>
-      <c r="G30" s="220"/>
-      <c r="H30" s="220"/>
-      <c r="I30" s="220"/>
-      <c r="J30" s="220"/>
+      <c r="E30" s="205"/>
+      <c r="F30" s="205"/>
+      <c r="G30" s="205"/>
+      <c r="H30" s="205"/>
+      <c r="I30" s="205"/>
+      <c r="J30" s="205"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="220"/>
-      <c r="F31" s="220"/>
-      <c r="G31" s="220"/>
-      <c r="H31" s="220"/>
-      <c r="I31" s="220"/>
-      <c r="J31" s="220"/>
+      <c r="E31" s="205"/>
+      <c r="F31" s="205"/>
+      <c r="G31" s="205"/>
+      <c r="H31" s="205"/>
+      <c r="I31" s="205"/>
+      <c r="J31" s="205"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="220"/>
-      <c r="F32" s="220"/>
-      <c r="G32" s="220"/>
-      <c r="H32" s="220"/>
-      <c r="I32" s="220"/>
-      <c r="J32" s="220"/>
+      <c r="E32" s="205"/>
+      <c r="F32" s="205"/>
+      <c r="G32" s="205"/>
+      <c r="H32" s="205"/>
+      <c r="I32" s="205"/>
+      <c r="J32" s="205"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="220"/>
-      <c r="F33" s="220"/>
-      <c r="G33" s="220"/>
-      <c r="H33" s="220"/>
-      <c r="I33" s="220"/>
-      <c r="J33" s="220"/>
+      <c r="E33" s="205"/>
+      <c r="F33" s="205"/>
+      <c r="G33" s="205"/>
+      <c r="H33" s="205"/>
+      <c r="I33" s="205"/>
+      <c r="J33" s="205"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="220"/>
-      <c r="F34" s="220"/>
-      <c r="G34" s="220"/>
-      <c r="H34" s="220"/>
-      <c r="I34" s="220"/>
-      <c r="J34" s="220"/>
+      <c r="E34" s="205"/>
+      <c r="F34" s="205"/>
+      <c r="G34" s="205"/>
+      <c r="H34" s="205"/>
+      <c r="I34" s="205"/>
+      <c r="J34" s="205"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="220"/>
-      <c r="F35" s="220"/>
-      <c r="G35" s="220"/>
-      <c r="H35" s="220"/>
-      <c r="I35" s="220"/>
-      <c r="J35" s="220"/>
+      <c r="E35" s="205"/>
+      <c r="F35" s="205"/>
+      <c r="G35" s="205"/>
+      <c r="H35" s="205"/>
+      <c r="I35" s="205"/>
+      <c r="J35" s="205"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="220"/>
-      <c r="F36" s="220"/>
-      <c r="G36" s="220"/>
-      <c r="H36" s="220"/>
-      <c r="I36" s="220"/>
-      <c r="J36" s="220"/>
+      <c r="E36" s="205"/>
+      <c r="F36" s="205"/>
+      <c r="G36" s="205"/>
+      <c r="H36" s="205"/>
+      <c r="I36" s="205"/>
+      <c r="J36" s="205"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="220"/>
-      <c r="F37" s="220"/>
-      <c r="G37" s="220"/>
-      <c r="H37" s="220"/>
-      <c r="I37" s="220"/>
-      <c r="J37" s="220"/>
+      <c r="E37" s="205"/>
+      <c r="F37" s="205"/>
+      <c r="G37" s="205"/>
+      <c r="H37" s="205"/>
+      <c r="I37" s="205"/>
+      <c r="J37" s="205"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="220"/>
-      <c r="F38" s="220"/>
-      <c r="G38" s="220"/>
-      <c r="H38" s="220"/>
-      <c r="I38" s="220"/>
-      <c r="J38" s="220"/>
+      <c r="E38" s="205"/>
+      <c r="F38" s="205"/>
+      <c r="G38" s="205"/>
+      <c r="H38" s="205"/>
+      <c r="I38" s="205"/>
+      <c r="J38" s="205"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="220"/>
-      <c r="F39" s="220"/>
-      <c r="G39" s="220"/>
-      <c r="H39" s="220"/>
-      <c r="I39" s="220"/>
-      <c r="J39" s="220"/>
+      <c r="E39" s="205"/>
+      <c r="F39" s="205"/>
+      <c r="G39" s="205"/>
+      <c r="H39" s="205"/>
+      <c r="I39" s="205"/>
+      <c r="J39" s="205"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="220"/>
-      <c r="F40" s="220"/>
-      <c r="G40" s="220"/>
-      <c r="H40" s="220"/>
-      <c r="I40" s="220"/>
-      <c r="J40" s="220"/>
+      <c r="E40" s="205"/>
+      <c r="F40" s="205"/>
+      <c r="G40" s="205"/>
+      <c r="H40" s="205"/>
+      <c r="I40" s="205"/>
+      <c r="J40" s="205"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="220"/>
-      <c r="F41" s="220"/>
-      <c r="G41" s="220"/>
-      <c r="H41" s="220"/>
-      <c r="I41" s="220"/>
-      <c r="J41" s="220"/>
+      <c r="E41" s="205"/>
+      <c r="F41" s="205"/>
+      <c r="G41" s="205"/>
+      <c r="H41" s="205"/>
+      <c r="I41" s="205"/>
+      <c r="J41" s="205"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="220"/>
-      <c r="F42" s="220"/>
-      <c r="G42" s="220"/>
-      <c r="H42" s="220"/>
-      <c r="I42" s="220"/>
-      <c r="J42" s="220"/>
+      <c r="E42" s="205"/>
+      <c r="F42" s="205"/>
+      <c r="G42" s="205"/>
+      <c r="H42" s="205"/>
+      <c r="I42" s="205"/>
+      <c r="J42" s="205"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E24:J24"/>
     <mergeCell ref="E41:J41"/>
     <mergeCell ref="E42:J42"/>
     <mergeCell ref="E31:J31"/>
@@ -9085,18 +9103,14 @@
     <mergeCell ref="E38:J38"/>
     <mergeCell ref="E39:J39"/>
     <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E20:J20"/>
-    <mergeCell ref="E21:J21"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2">
@@ -9113,8 +9127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="I7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9140,10 +9154,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="210" t="s">
+      <c r="A1" s="227" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="210"/>
+      <c r="B1" s="227"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -9181,8 +9195,8 @@
       <c r="Q1" s="17"/>
     </row>
     <row r="2" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="210"/>
-      <c r="B2" s="210"/>
+      <c r="A2" s="227"/>
+      <c r="B2" s="227"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -9220,16 +9234,16 @@
       <c r="Q2" s="17"/>
     </row>
     <row r="3" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="269"/>
-      <c r="B3" s="270"/>
-      <c r="C3" s="270"/>
-      <c r="D3" s="270"/>
-      <c r="E3" s="270"/>
-      <c r="F3" s="270"/>
-      <c r="G3" s="270"/>
-      <c r="H3" s="270"/>
-      <c r="I3" s="270"/>
-      <c r="J3" s="271"/>
+      <c r="A3" s="267"/>
+      <c r="B3" s="268"/>
+      <c r="C3" s="268"/>
+      <c r="D3" s="268"/>
+      <c r="E3" s="268"/>
+      <c r="F3" s="268"/>
+      <c r="G3" s="268"/>
+      <c r="H3" s="268"/>
+      <c r="I3" s="268"/>
+      <c r="J3" s="269"/>
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
@@ -9263,12 +9277,12 @@
       <c r="H4" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="266" t="s">
+      <c r="I4" s="264" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="267"/>
-      <c r="K4" s="267"/>
-      <c r="L4" s="268"/>
+      <c r="J4" s="265"/>
+      <c r="K4" s="265"/>
+      <c r="L4" s="266"/>
       <c r="M4" s="66" t="s">
         <v>44</v>
       </c>
@@ -9302,12 +9316,12 @@
       <c r="H5" s="166" t="s">
         <v>231</v>
       </c>
-      <c r="I5" s="278" t="s">
+      <c r="I5" s="273" t="s">
         <v>232</v>
       </c>
-      <c r="J5" s="279"/>
-      <c r="K5" s="279"/>
-      <c r="L5" s="280"/>
+      <c r="J5" s="274"/>
+      <c r="K5" s="274"/>
+      <c r="L5" s="275"/>
       <c r="M5" s="151"/>
       <c r="N5" s="151"/>
       <c r="O5" s="151"/>
@@ -9331,12 +9345,12 @@
       <c r="H6" s="166" t="s">
         <v>175</v>
       </c>
-      <c r="I6" s="272" t="s">
+      <c r="I6" s="276" t="s">
         <v>228</v>
       </c>
-      <c r="J6" s="273"/>
-      <c r="K6" s="273"/>
-      <c r="L6" s="274"/>
+      <c r="J6" s="277"/>
+      <c r="K6" s="277"/>
+      <c r="L6" s="278"/>
       <c r="M6" s="151"/>
       <c r="N6" s="151"/>
       <c r="O6" s="151"/>
@@ -9358,12 +9372,12 @@
       <c r="H7" s="189" t="s">
         <v>238</v>
       </c>
-      <c r="I7" s="275" t="s">
+      <c r="I7" s="270" t="s">
         <v>237</v>
       </c>
-      <c r="J7" s="276"/>
-      <c r="K7" s="276"/>
-      <c r="L7" s="277"/>
+      <c r="J7" s="271"/>
+      <c r="K7" s="271"/>
+      <c r="L7" s="272"/>
       <c r="M7" s="190"/>
       <c r="N7" s="190"/>
       <c r="O7" s="190"/>
@@ -9372,7 +9386,9 @@
     </row>
     <row r="8" spans="1:17" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="193"/>
-      <c r="B8" s="21"/>
+      <c r="B8" s="21" t="s">
+        <v>259</v>
+      </c>
       <c r="C8" s="22"/>
       <c r="D8" s="23"/>
       <c r="E8" s="194" t="s">
@@ -9387,12 +9403,12 @@
       <c r="H8" s="195" t="s">
         <v>242</v>
       </c>
-      <c r="I8" s="262" t="s">
+      <c r="I8" s="260" t="s">
         <v>244</v>
       </c>
-      <c r="J8" s="263"/>
-      <c r="K8" s="263"/>
-      <c r="L8" s="264"/>
+      <c r="J8" s="261"/>
+      <c r="K8" s="261"/>
+      <c r="L8" s="262"/>
       <c r="M8" s="196" t="s">
         <v>245</v>
       </c>
@@ -9406,7 +9422,7 @@
         <v>247</v>
       </c>
       <c r="Q8" s="194" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9418,10 +9434,10 @@
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
       <c r="H9" s="51"/>
-      <c r="I9" s="258"/>
-      <c r="J9" s="259"/>
-      <c r="K9" s="259"/>
-      <c r="L9" s="260"/>
+      <c r="I9" s="256"/>
+      <c r="J9" s="257"/>
+      <c r="K9" s="257"/>
+      <c r="L9" s="258"/>
       <c r="M9" s="60"/>
       <c r="N9" s="60"/>
       <c r="O9" s="60"/>
@@ -9437,10 +9453,10 @@
       <c r="F10" s="55"/>
       <c r="G10" s="55"/>
       <c r="H10" s="55"/>
-      <c r="I10" s="258"/>
-      <c r="J10" s="259"/>
-      <c r="K10" s="259"/>
-      <c r="L10" s="260"/>
+      <c r="I10" s="256"/>
+      <c r="J10" s="257"/>
+      <c r="K10" s="257"/>
+      <c r="L10" s="258"/>
       <c r="M10" s="60"/>
       <c r="N10" s="60"/>
       <c r="O10" s="60"/>
@@ -9456,10 +9472,10 @@
       <c r="F11" s="55"/>
       <c r="G11" s="55"/>
       <c r="H11" s="55"/>
-      <c r="I11" s="258"/>
-      <c r="J11" s="259"/>
-      <c r="K11" s="259"/>
-      <c r="L11" s="260"/>
+      <c r="I11" s="256"/>
+      <c r="J11" s="257"/>
+      <c r="K11" s="257"/>
+      <c r="L11" s="258"/>
       <c r="M11" s="60"/>
       <c r="N11" s="60"/>
       <c r="O11" s="60"/>
@@ -9471,361 +9487,339 @@
       <c r="B12" s="35"/>
       <c r="C12" s="36"/>
       <c r="D12" s="34"/>
-      <c r="E12" s="220"/>
-      <c r="F12" s="220"/>
-      <c r="G12" s="220"/>
-      <c r="H12" s="220"/>
-      <c r="I12" s="220"/>
-      <c r="J12" s="220"/>
+      <c r="E12" s="205"/>
+      <c r="F12" s="205"/>
+      <c r="G12" s="205"/>
+      <c r="H12" s="205"/>
+      <c r="I12" s="205"/>
+      <c r="J12" s="205"/>
     </row>
     <row r="13" spans="1:17" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="35"/>
       <c r="C13" s="36"/>
       <c r="D13" s="34"/>
-      <c r="E13" s="220"/>
-      <c r="F13" s="220"/>
-      <c r="G13" s="220"/>
-      <c r="H13" s="220"/>
-      <c r="I13" s="220"/>
-      <c r="J13" s="220"/>
+      <c r="E13" s="205"/>
+      <c r="F13" s="205"/>
+      <c r="G13" s="205"/>
+      <c r="H13" s="205"/>
+      <c r="I13" s="205"/>
+      <c r="J13" s="205"/>
     </row>
     <row r="14" spans="1:17" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="35"/>
       <c r="C14" s="36"/>
       <c r="D14" s="34"/>
-      <c r="E14" s="220"/>
-      <c r="F14" s="220"/>
-      <c r="G14" s="220"/>
-      <c r="H14" s="220"/>
-      <c r="I14" s="220"/>
-      <c r="J14" s="220"/>
+      <c r="E14" s="205"/>
+      <c r="F14" s="205"/>
+      <c r="G14" s="205"/>
+      <c r="H14" s="205"/>
+      <c r="I14" s="205"/>
+      <c r="J14" s="205"/>
     </row>
     <row r="15" spans="1:17" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="220"/>
-      <c r="F15" s="220"/>
-      <c r="G15" s="220"/>
-      <c r="H15" s="220"/>
-      <c r="I15" s="220"/>
-      <c r="J15" s="220"/>
+      <c r="E15" s="205"/>
+      <c r="F15" s="205"/>
+      <c r="G15" s="205"/>
+      <c r="H15" s="205"/>
+      <c r="I15" s="205"/>
+      <c r="J15" s="205"/>
     </row>
     <row r="16" spans="1:17" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="220"/>
-      <c r="F16" s="220"/>
-      <c r="G16" s="220"/>
-      <c r="H16" s="220"/>
-      <c r="I16" s="220"/>
-      <c r="J16" s="220"/>
+      <c r="E16" s="205"/>
+      <c r="F16" s="205"/>
+      <c r="G16" s="205"/>
+      <c r="H16" s="205"/>
+      <c r="I16" s="205"/>
+      <c r="J16" s="205"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="220"/>
-      <c r="F17" s="220"/>
-      <c r="G17" s="220"/>
-      <c r="H17" s="220"/>
-      <c r="I17" s="220"/>
-      <c r="J17" s="220"/>
+      <c r="E17" s="205"/>
+      <c r="F17" s="205"/>
+      <c r="G17" s="205"/>
+      <c r="H17" s="205"/>
+      <c r="I17" s="205"/>
+      <c r="J17" s="205"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="220"/>
-      <c r="F18" s="220"/>
-      <c r="G18" s="220"/>
-      <c r="H18" s="220"/>
-      <c r="I18" s="220"/>
-      <c r="J18" s="220"/>
+      <c r="E18" s="205"/>
+      <c r="F18" s="205"/>
+      <c r="G18" s="205"/>
+      <c r="H18" s="205"/>
+      <c r="I18" s="205"/>
+      <c r="J18" s="205"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="220"/>
-      <c r="F19" s="220"/>
-      <c r="G19" s="220"/>
-      <c r="H19" s="220"/>
-      <c r="I19" s="220"/>
-      <c r="J19" s="220"/>
+      <c r="E19" s="205"/>
+      <c r="F19" s="205"/>
+      <c r="G19" s="205"/>
+      <c r="H19" s="205"/>
+      <c r="I19" s="205"/>
+      <c r="J19" s="205"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="220"/>
-      <c r="F20" s="220"/>
-      <c r="G20" s="220"/>
-      <c r="H20" s="220"/>
-      <c r="I20" s="220"/>
-      <c r="J20" s="220"/>
+      <c r="E20" s="205"/>
+      <c r="F20" s="205"/>
+      <c r="G20" s="205"/>
+      <c r="H20" s="205"/>
+      <c r="I20" s="205"/>
+      <c r="J20" s="205"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="220"/>
-      <c r="F21" s="220"/>
-      <c r="G21" s="220"/>
-      <c r="H21" s="220"/>
-      <c r="I21" s="220"/>
-      <c r="J21" s="220"/>
+      <c r="E21" s="205"/>
+      <c r="F21" s="205"/>
+      <c r="G21" s="205"/>
+      <c r="H21" s="205"/>
+      <c r="I21" s="205"/>
+      <c r="J21" s="205"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="34"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="220"/>
-      <c r="F22" s="220"/>
-      <c r="G22" s="220"/>
-      <c r="H22" s="220"/>
-      <c r="I22" s="220"/>
-      <c r="J22" s="220"/>
+      <c r="E22" s="205"/>
+      <c r="F22" s="205"/>
+      <c r="G22" s="205"/>
+      <c r="H22" s="205"/>
+      <c r="I22" s="205"/>
+      <c r="J22" s="205"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="220"/>
-      <c r="F23" s="220"/>
-      <c r="G23" s="220"/>
-      <c r="H23" s="220"/>
-      <c r="I23" s="220"/>
-      <c r="J23" s="220"/>
+      <c r="E23" s="205"/>
+      <c r="F23" s="205"/>
+      <c r="G23" s="205"/>
+      <c r="H23" s="205"/>
+      <c r="I23" s="205"/>
+      <c r="J23" s="205"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="220"/>
-      <c r="F24" s="220"/>
-      <c r="G24" s="220"/>
-      <c r="H24" s="220"/>
-      <c r="I24" s="220"/>
-      <c r="J24" s="220"/>
+      <c r="E24" s="205"/>
+      <c r="F24" s="205"/>
+      <c r="G24" s="205"/>
+      <c r="H24" s="205"/>
+      <c r="I24" s="205"/>
+      <c r="J24" s="205"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="220"/>
-      <c r="F25" s="220"/>
-      <c r="G25" s="220"/>
-      <c r="H25" s="220"/>
-      <c r="I25" s="220"/>
-      <c r="J25" s="220"/>
+      <c r="E25" s="205"/>
+      <c r="F25" s="205"/>
+      <c r="G25" s="205"/>
+      <c r="H25" s="205"/>
+      <c r="I25" s="205"/>
+      <c r="J25" s="205"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="220"/>
-      <c r="F26" s="220"/>
-      <c r="G26" s="220"/>
-      <c r="H26" s="220"/>
-      <c r="I26" s="220"/>
-      <c r="J26" s="220"/>
+      <c r="E26" s="205"/>
+      <c r="F26" s="205"/>
+      <c r="G26" s="205"/>
+      <c r="H26" s="205"/>
+      <c r="I26" s="205"/>
+      <c r="J26" s="205"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="220"/>
-      <c r="F27" s="220"/>
-      <c r="G27" s="220"/>
-      <c r="H27" s="220"/>
-      <c r="I27" s="220"/>
-      <c r="J27" s="220"/>
+      <c r="E27" s="205"/>
+      <c r="F27" s="205"/>
+      <c r="G27" s="205"/>
+      <c r="H27" s="205"/>
+      <c r="I27" s="205"/>
+      <c r="J27" s="205"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="220"/>
-      <c r="F28" s="220"/>
-      <c r="G28" s="220"/>
-      <c r="H28" s="220"/>
-      <c r="I28" s="220"/>
-      <c r="J28" s="220"/>
+      <c r="E28" s="205"/>
+      <c r="F28" s="205"/>
+      <c r="G28" s="205"/>
+      <c r="H28" s="205"/>
+      <c r="I28" s="205"/>
+      <c r="J28" s="205"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="220"/>
-      <c r="F29" s="220"/>
-      <c r="G29" s="220"/>
-      <c r="H29" s="220"/>
-      <c r="I29" s="220"/>
-      <c r="J29" s="220"/>
+      <c r="E29" s="205"/>
+      <c r="F29" s="205"/>
+      <c r="G29" s="205"/>
+      <c r="H29" s="205"/>
+      <c r="I29" s="205"/>
+      <c r="J29" s="205"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="220"/>
-      <c r="F30" s="220"/>
-      <c r="G30" s="220"/>
-      <c r="H30" s="220"/>
-      <c r="I30" s="220"/>
-      <c r="J30" s="220"/>
+      <c r="E30" s="205"/>
+      <c r="F30" s="205"/>
+      <c r="G30" s="205"/>
+      <c r="H30" s="205"/>
+      <c r="I30" s="205"/>
+      <c r="J30" s="205"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="220"/>
-      <c r="F31" s="220"/>
-      <c r="G31" s="220"/>
-      <c r="H31" s="220"/>
-      <c r="I31" s="220"/>
-      <c r="J31" s="220"/>
+      <c r="E31" s="205"/>
+      <c r="F31" s="205"/>
+      <c r="G31" s="205"/>
+      <c r="H31" s="205"/>
+      <c r="I31" s="205"/>
+      <c r="J31" s="205"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="34"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="220"/>
-      <c r="F32" s="220"/>
-      <c r="G32" s="220"/>
-      <c r="H32" s="220"/>
-      <c r="I32" s="220"/>
-      <c r="J32" s="220"/>
+      <c r="E32" s="205"/>
+      <c r="F32" s="205"/>
+      <c r="G32" s="205"/>
+      <c r="H32" s="205"/>
+      <c r="I32" s="205"/>
+      <c r="J32" s="205"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="220"/>
-      <c r="F33" s="220"/>
-      <c r="G33" s="220"/>
-      <c r="H33" s="220"/>
-      <c r="I33" s="220"/>
-      <c r="J33" s="220"/>
+      <c r="E33" s="205"/>
+      <c r="F33" s="205"/>
+      <c r="G33" s="205"/>
+      <c r="H33" s="205"/>
+      <c r="I33" s="205"/>
+      <c r="J33" s="205"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="220"/>
-      <c r="F34" s="220"/>
-      <c r="G34" s="220"/>
-      <c r="H34" s="220"/>
-      <c r="I34" s="220"/>
-      <c r="J34" s="220"/>
+      <c r="E34" s="205"/>
+      <c r="F34" s="205"/>
+      <c r="G34" s="205"/>
+      <c r="H34" s="205"/>
+      <c r="I34" s="205"/>
+      <c r="J34" s="205"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="220"/>
-      <c r="F35" s="220"/>
-      <c r="G35" s="220"/>
-      <c r="H35" s="220"/>
-      <c r="I35" s="220"/>
-      <c r="J35" s="220"/>
+      <c r="E35" s="205"/>
+      <c r="F35" s="205"/>
+      <c r="G35" s="205"/>
+      <c r="H35" s="205"/>
+      <c r="I35" s="205"/>
+      <c r="J35" s="205"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="220"/>
-      <c r="F36" s="220"/>
-      <c r="G36" s="220"/>
-      <c r="H36" s="220"/>
-      <c r="I36" s="220"/>
-      <c r="J36" s="220"/>
+      <c r="E36" s="205"/>
+      <c r="F36" s="205"/>
+      <c r="G36" s="205"/>
+      <c r="H36" s="205"/>
+      <c r="I36" s="205"/>
+      <c r="J36" s="205"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="220"/>
-      <c r="F37" s="220"/>
-      <c r="G37" s="220"/>
-      <c r="H37" s="220"/>
-      <c r="I37" s="220"/>
-      <c r="J37" s="220"/>
+      <c r="E37" s="205"/>
+      <c r="F37" s="205"/>
+      <c r="G37" s="205"/>
+      <c r="H37" s="205"/>
+      <c r="I37" s="205"/>
+      <c r="J37" s="205"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="220"/>
-      <c r="F38" s="220"/>
-      <c r="G38" s="220"/>
-      <c r="H38" s="220"/>
-      <c r="I38" s="220"/>
-      <c r="J38" s="220"/>
+      <c r="E38" s="205"/>
+      <c r="F38" s="205"/>
+      <c r="G38" s="205"/>
+      <c r="H38" s="205"/>
+      <c r="I38" s="205"/>
+      <c r="J38" s="205"/>
     </row>
     <row r="39" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="220"/>
-      <c r="F39" s="220"/>
-      <c r="G39" s="220"/>
-      <c r="H39" s="220"/>
-      <c r="I39" s="220"/>
-      <c r="J39" s="220"/>
+      <c r="E39" s="205"/>
+      <c r="F39" s="205"/>
+      <c r="G39" s="205"/>
+      <c r="H39" s="205"/>
+      <c r="I39" s="205"/>
+      <c r="J39" s="205"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E14:J14"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="E12:J12"/>
-    <mergeCell ref="E13:J13"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
-    <mergeCell ref="I5:L5"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E20:J20"/>
-    <mergeCell ref="E21:J21"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
     <mergeCell ref="E39:J39"/>
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="I6:L6"/>
@@ -9842,6 +9836,28 @@
     <mergeCell ref="E31:J31"/>
     <mergeCell ref="E25:J25"/>
     <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E14:J14"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="I5:L5"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2">
@@ -9864,14 +9880,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A18" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0">
       <selection activeCell="C24" sqref="C24:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="16" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="16" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" style="16" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" style="16" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" style="16" customWidth="1"/>
@@ -9884,11 +9900,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="210" t="s">
+      <c r="A1" s="227" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
+      <c r="B1" s="227"/>
+      <c r="C1" s="227"/>
       <c r="D1" s="46" t="s">
         <v>1</v>
       </c>
@@ -9919,9 +9935,9 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="210"/>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
+      <c r="A2" s="227"/>
+      <c r="B2" s="227"/>
+      <c r="C2" s="227"/>
       <c r="D2" s="46" t="s">
         <v>7</v>
       </c>
@@ -10261,20 +10277,22 @@
       <c r="J23" s="181"/>
       <c r="K23" s="182"/>
     </row>
-    <row r="24" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="205"/>
-      <c r="B24" s="206"/>
-      <c r="C24" s="282" t="s">
-        <v>255</v>
-      </c>
-      <c r="D24" s="283"/>
-      <c r="E24" s="283"/>
-      <c r="F24" s="283"/>
-      <c r="G24" s="283"/>
-      <c r="H24" s="283"/>
-      <c r="I24" s="283"/>
-      <c r="J24" s="283"/>
-      <c r="K24" s="284"/>
+    <row r="24" spans="1:12" ht="158.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="287" t="s">
+        <v>258</v>
+      </c>
+      <c r="B24" s="288"/>
+      <c r="C24" s="280" t="s">
+        <v>257</v>
+      </c>
+      <c r="D24" s="281"/>
+      <c r="E24" s="281"/>
+      <c r="F24" s="281"/>
+      <c r="G24" s="281"/>
+      <c r="H24" s="281"/>
+      <c r="I24" s="281"/>
+      <c r="J24" s="281"/>
+      <c r="K24" s="282"/>
       <c r="L24" s="17"/>
     </row>
     <row r="25" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -10359,12 +10377,12 @@
       <c r="C30" s="39"/>
       <c r="D30" s="42"/>
       <c r="E30" s="38"/>
-      <c r="F30" s="281"/>
-      <c r="G30" s="281"/>
-      <c r="H30" s="281"/>
-      <c r="I30" s="281"/>
-      <c r="J30" s="281"/>
-      <c r="K30" s="281"/>
+      <c r="F30" s="279"/>
+      <c r="G30" s="279"/>
+      <c r="H30" s="279"/>
+      <c r="I30" s="279"/>
+      <c r="J30" s="279"/>
+      <c r="K30" s="279"/>
       <c r="L30" s="17"/>
     </row>
     <row r="31" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -10373,12 +10391,12 @@
       <c r="C31" s="39"/>
       <c r="D31" s="42"/>
       <c r="E31" s="38"/>
-      <c r="F31" s="281"/>
-      <c r="G31" s="281"/>
-      <c r="H31" s="281"/>
-      <c r="I31" s="281"/>
-      <c r="J31" s="281"/>
-      <c r="K31" s="281"/>
+      <c r="F31" s="279"/>
+      <c r="G31" s="279"/>
+      <c r="H31" s="279"/>
+      <c r="I31" s="279"/>
+      <c r="J31" s="279"/>
+      <c r="K31" s="279"/>
       <c r="L31" s="17"/>
     </row>
     <row r="32" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -10387,12 +10405,12 @@
       <c r="C32" s="39"/>
       <c r="D32" s="42"/>
       <c r="E32" s="38"/>
-      <c r="F32" s="281"/>
-      <c r="G32" s="281"/>
-      <c r="H32" s="281"/>
-      <c r="I32" s="281"/>
-      <c r="J32" s="281"/>
-      <c r="K32" s="281"/>
+      <c r="F32" s="279"/>
+      <c r="G32" s="279"/>
+      <c r="H32" s="279"/>
+      <c r="I32" s="279"/>
+      <c r="J32" s="279"/>
+      <c r="K32" s="279"/>
       <c r="L32" s="17"/>
     </row>
     <row r="33" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10401,12 +10419,12 @@
       <c r="C33" s="39"/>
       <c r="D33" s="42"/>
       <c r="E33" s="38"/>
-      <c r="F33" s="281"/>
-      <c r="G33" s="281"/>
-      <c r="H33" s="281"/>
-      <c r="I33" s="281"/>
-      <c r="J33" s="281"/>
-      <c r="K33" s="281"/>
+      <c r="F33" s="279"/>
+      <c r="G33" s="279"/>
+      <c r="H33" s="279"/>
+      <c r="I33" s="279"/>
+      <c r="J33" s="279"/>
+      <c r="K33" s="279"/>
       <c r="L33" s="17"/>
     </row>
     <row r="34" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -10592,13 +10610,14 @@
       <c r="L46" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="F30:K30"/>
     <mergeCell ref="F31:K31"/>
     <mergeCell ref="F32:K32"/>
     <mergeCell ref="F33:K33"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="C24:K24"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
@@ -10635,11 +10654,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="210" t="s">
+      <c r="A1" s="227" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
+      <c r="B1" s="227"/>
+      <c r="C1" s="227"/>
       <c r="D1" s="46" t="s">
         <v>1</v>
       </c>
@@ -10662,9 +10681,9 @@
       <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="210"/>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
+      <c r="A2" s="227"/>
+      <c r="B2" s="227"/>
+      <c r="C2" s="227"/>
       <c r="D2" s="46" t="s">
         <v>7</v>
       </c>
@@ -11034,12 +11053,12 @@
       <c r="C28" s="39"/>
       <c r="D28" s="42"/>
       <c r="E28" s="38"/>
-      <c r="F28" s="281"/>
-      <c r="G28" s="281"/>
-      <c r="H28" s="281"/>
-      <c r="I28" s="281"/>
-      <c r="J28" s="281"/>
-      <c r="K28" s="281"/>
+      <c r="F28" s="279"/>
+      <c r="G28" s="279"/>
+      <c r="H28" s="279"/>
+      <c r="I28" s="279"/>
+      <c r="J28" s="279"/>
+      <c r="K28" s="279"/>
       <c r="L28" s="17"/>
     </row>
     <row r="29" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -11048,12 +11067,12 @@
       <c r="C29" s="39"/>
       <c r="D29" s="42"/>
       <c r="E29" s="38"/>
-      <c r="F29" s="281"/>
-      <c r="G29" s="281"/>
-      <c r="H29" s="281"/>
-      <c r="I29" s="281"/>
-      <c r="J29" s="281"/>
-      <c r="K29" s="281"/>
+      <c r="F29" s="279"/>
+      <c r="G29" s="279"/>
+      <c r="H29" s="279"/>
+      <c r="I29" s="279"/>
+      <c r="J29" s="279"/>
+      <c r="K29" s="279"/>
       <c r="L29" s="17"/>
     </row>
     <row r="30" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -11062,12 +11081,12 @@
       <c r="C30" s="39"/>
       <c r="D30" s="42"/>
       <c r="E30" s="38"/>
-      <c r="F30" s="281"/>
-      <c r="G30" s="281"/>
-      <c r="H30" s="281"/>
-      <c r="I30" s="281"/>
-      <c r="J30" s="281"/>
-      <c r="K30" s="281"/>
+      <c r="F30" s="279"/>
+      <c r="G30" s="279"/>
+      <c r="H30" s="279"/>
+      <c r="I30" s="279"/>
+      <c r="J30" s="279"/>
+      <c r="K30" s="279"/>
       <c r="L30" s="17"/>
     </row>
     <row r="31" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11076,12 +11095,12 @@
       <c r="C31" s="39"/>
       <c r="D31" s="42"/>
       <c r="E31" s="38"/>
-      <c r="F31" s="281"/>
-      <c r="G31" s="281"/>
-      <c r="H31" s="281"/>
-      <c r="I31" s="281"/>
-      <c r="J31" s="281"/>
-      <c r="K31" s="281"/>
+      <c r="F31" s="279"/>
+      <c r="G31" s="279"/>
+      <c r="H31" s="279"/>
+      <c r="I31" s="279"/>
+      <c r="J31" s="279"/>
+      <c r="K31" s="279"/>
       <c r="L31" s="17"/>
     </row>
     <row r="32" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -11301,14 +11320,14 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="78"/>
-      <c r="E2" s="285" t="s">
+      <c r="E2" s="283" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="285"/>
-      <c r="G2" s="285"/>
-      <c r="H2" s="285"/>
-      <c r="I2" s="285"/>
-      <c r="J2" s="285"/>
+      <c r="F2" s="283"/>
+      <c r="G2" s="283"/>
+      <c r="H2" s="283"/>
+      <c r="I2" s="283"/>
+      <c r="J2" s="283"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="79"/>
@@ -11729,11 +11748,11 @@
       <c r="B28" s="78"/>
       <c r="C28" s="78"/>
       <c r="D28" s="78"/>
-      <c r="E28" s="286" t="s">
+      <c r="E28" s="284" t="s">
         <v>107</v>
       </c>
-      <c r="F28" s="287"/>
-      <c r="G28" s="288"/>
+      <c r="F28" s="285"/>
+      <c r="G28" s="286"/>
       <c r="H28" s="78"/>
       <c r="I28" s="78"/>
       <c r="J28" s="78"/>

</xml_diff>